<commit_message>
Update README.md and clean-ups
</commit_message>
<xml_diff>
--- a/Input/Settings.xlsx
+++ b/Input/Settings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Julia\TradLifeModel\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C4CF099-3F51-4A71-AB97-386EC8FDC50A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE9B40F1-AD9E-4473-80A0-AA598725AFC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="889" activeTab="1" xr2:uid="{ADF8BBD9-0F7A-45CB-8EA8-A3D46B124E82}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="889" xr2:uid="{ADF8BBD9-0F7A-45CB-8EA8-A3D46B124E82}"/>
   </bookViews>
   <sheets>
     <sheet name="general_settings" sheetId="13" r:id="rId1"/>
@@ -22,6 +22,9 @@
   <externalReferences>
     <externalReference r:id="rId6"/>
   </externalReferences>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">product_setup!$A$1:$C$57</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -41,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="172">
   <si>
     <t>acq_exp_per_pol</t>
   </si>
@@ -554,6 +557,9 @@
   </si>
   <si>
     <t>Capital Requirement Gross Up Factor</t>
+  </si>
+  <si>
+    <t>Number of Workers for Multiprocessing</t>
   </si>
 </sst>
 </file>
@@ -712,7 +718,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -737,12 +743,6 @@
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -783,6 +783,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="15" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -841,7 +844,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
       <sheetData sheetId="2">
         <row r="2">
           <cell r="A2" t="str">
@@ -855,7 +858,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="3"/>
+      <sheetData sheetId="3" refreshError="1"/>
       <sheetData sheetId="4">
         <row r="2">
           <cell r="A2" t="str">
@@ -869,7 +872,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="5"/>
+      <sheetData sheetId="5" refreshError="1"/>
       <sheetData sheetId="6">
         <row r="2">
           <cell r="A2" t="str">
@@ -883,7 +886,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="7"/>
+      <sheetData sheetId="7" refreshError="1"/>
       <sheetData sheetId="8">
         <row r="2">
           <cell r="A2" t="str">
@@ -897,7 +900,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="9"/>
+      <sheetData sheetId="9" refreshError="1"/>
       <sheetData sheetId="10">
         <row r="2">
           <cell r="A2" t="str">
@@ -911,7 +914,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="11"/>
+      <sheetData sheetId="11" refreshError="1"/>
       <sheetData sheetId="12">
         <row r="2">
           <cell r="A2" t="str">
@@ -925,7 +928,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="13"/>
+      <sheetData sheetId="13" refreshError="1"/>
       <sheetData sheetId="14">
         <row r="2">
           <cell r="A2" t="str">
@@ -939,7 +942,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="15"/>
+      <sheetData sheetId="15" refreshError="1"/>
       <sheetData sheetId="16">
         <row r="2">
           <cell r="A2" t="str">
@@ -953,7 +956,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="17"/>
+      <sheetData sheetId="17" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1256,15 +1259,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F309708F-75E9-4A4E-B1AF-0EC8FC0F4256}">
-  <dimension ref="A1:B24"/>
+  <dimension ref="A1:B25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="31.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1272,7 +1275,7 @@
       <c r="A1" t="s">
         <v>146</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="10" t="s">
         <v>115</v>
       </c>
     </row>
@@ -1280,7 +1283,7 @@
       <c r="A2" t="s">
         <v>169</v>
       </c>
-      <c r="B2" s="12">
+      <c r="B2" s="36">
         <v>45291</v>
       </c>
     </row>
@@ -1288,7 +1291,7 @@
       <c r="A3" t="s">
         <v>168</v>
       </c>
-      <c r="B3" s="11">
+      <c r="B3" s="15">
         <v>120</v>
       </c>
     </row>
@@ -1296,133 +1299,141 @@
       <c r="A4" t="s">
         <v>170</v>
       </c>
-      <c r="B4" s="11">
+      <c r="B4" s="15">
         <v>0.3</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>148</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>116</v>
+        <v>171</v>
+      </c>
+      <c r="B5" s="15">
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>149</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>117</v>
+        <v>148</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>150</v>
-      </c>
-      <c r="B7" s="2"/>
+        <v>149</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>151</v>
-      </c>
-      <c r="B8" s="2"/>
+        <v>150</v>
+      </c>
+      <c r="B8" s="15"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>152</v>
-      </c>
-      <c r="B9" s="2"/>
+        <v>151</v>
+      </c>
+      <c r="B9" s="15"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>153</v>
-      </c>
-      <c r="B10" s="2"/>
+        <v>152</v>
+      </c>
+      <c r="B10" s="15"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>154</v>
-      </c>
-      <c r="B11" s="2"/>
+        <v>153</v>
+      </c>
+      <c r="B11" s="15"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>155</v>
-      </c>
-      <c r="B12" s="2"/>
+        <v>154</v>
+      </c>
+      <c r="B12" s="15"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>156</v>
-      </c>
-      <c r="B13" s="2"/>
+        <v>155</v>
+      </c>
+      <c r="B13" s="15"/>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>157</v>
-      </c>
-      <c r="B14" s="2"/>
+        <v>156</v>
+      </c>
+      <c r="B14" s="15"/>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>158</v>
-      </c>
-      <c r="B15" s="2"/>
+        <v>157</v>
+      </c>
+      <c r="B15" s="15"/>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>159</v>
-      </c>
-      <c r="B16" s="2"/>
+        <v>158</v>
+      </c>
+      <c r="B16" s="15"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>160</v>
-      </c>
-      <c r="B17" s="2"/>
+        <v>159</v>
+      </c>
+      <c r="B17" s="15"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>161</v>
-      </c>
-      <c r="B18" s="2"/>
+        <v>160</v>
+      </c>
+      <c r="B18" s="15"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>162</v>
-      </c>
-      <c r="B19" s="2"/>
+        <v>161</v>
+      </c>
+      <c r="B19" s="15"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>163</v>
-      </c>
-      <c r="B20" s="2"/>
+        <v>162</v>
+      </c>
+      <c r="B20" s="15"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>164</v>
-      </c>
-      <c r="B21" s="2"/>
+        <v>163</v>
+      </c>
+      <c r="B21" s="15"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>165</v>
-      </c>
-      <c r="B22" s="2"/>
+        <v>164</v>
+      </c>
+      <c r="B22" s="15"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>166</v>
-      </c>
-      <c r="B23" s="2"/>
+        <v>165</v>
+      </c>
+      <c r="B23" s="15"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
+        <v>166</v>
+      </c>
+      <c r="B24" s="15"/>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
         <v>167</v>
       </c>
-      <c r="B24" s="2"/>
+      <c r="B25" s="15"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
@@ -1434,11 +1445,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61890AB8-02EC-40E1-960C-9B07CCD09B96}">
   <dimension ref="A1:U19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2108,7 +2119,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D57" sqref="D57"/>
+      <selection pane="bottomRight" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2139,75 +2150,75 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="20" t="s">
         <v>142</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="21" t="s">
         <v>143</v>
       </c>
-      <c r="C2" s="25" t="s">
+      <c r="C2" s="23" t="s">
         <v>138</v>
       </c>
-      <c r="D2" s="18">
+      <c r="D2" s="16">
         <v>1</v>
       </c>
-      <c r="E2" s="18">
+      <c r="E2" s="16">
         <v>1</v>
       </c>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
-      <c r="I2" s="18"/>
-      <c r="J2" s="18"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="20" t="str">
+      <c r="A3" s="18" t="str">
         <f>A2</f>
         <v>Product Feature</v>
       </c>
-      <c r="B3" s="21" t="str">
+      <c r="B3" s="19" t="str">
         <f t="shared" ref="B3" si="0">B2</f>
         <v>death_ben</v>
       </c>
-      <c r="C3" s="24" t="s">
+      <c r="C3" s="22" t="s">
         <v>137</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="D3" s="15" t="s">
         <v>130</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="E3" s="15" t="s">
         <v>130</v>
       </c>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="17"/>
-      <c r="J3" s="17"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="15"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="29" t="s">
+      <c r="A4" s="27" t="s">
         <v>142</v>
       </c>
       <c r="B4" t="s">
         <v>144</v>
       </c>
-      <c r="C4" s="30" t="s">
+      <c r="C4" s="28" t="s">
         <v>138</v>
       </c>
-      <c r="D4" s="18">
+      <c r="D4" s="16">
         <v>1</v>
       </c>
-      <c r="E4" s="18">
+      <c r="E4" s="16">
         <v>1</v>
       </c>
-      <c r="F4" s="18"/>
-      <c r="G4" s="18"/>
-      <c r="H4" s="18"/>
-      <c r="I4" s="18"/>
-      <c r="J4" s="18"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="16"/>
+      <c r="I4" s="16"/>
+      <c r="J4" s="16"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="29" t="str">
+      <c r="A5" s="27" t="str">
         <f>A4</f>
         <v>Product Feature</v>
       </c>
@@ -2215,91 +2226,91 @@
         <f>B4</f>
         <v>surr_ben</v>
       </c>
-      <c r="C5" s="30" t="s">
+      <c r="C5" s="28" t="s">
         <v>137</v>
       </c>
-      <c r="D5" s="17" t="s">
+      <c r="D5" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="F5" s="17"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="17"/>
-      <c r="I5" s="17"/>
-      <c r="J5" s="17"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="15"/>
+      <c r="J5" s="15"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="20" t="s">
+      <c r="A6" s="18" t="s">
         <v>142</v>
       </c>
-      <c r="B6" s="21" t="s">
+      <c r="B6" s="19" t="s">
         <v>145</v>
       </c>
-      <c r="C6" s="24" t="s">
+      <c r="C6" s="22" t="s">
         <v>138</v>
       </c>
-      <c r="D6" s="18">
+      <c r="D6" s="16">
         <v>1</v>
       </c>
-      <c r="E6" s="18">
+      <c r="E6" s="16">
         <v>1</v>
       </c>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="18"/>
-      <c r="I6" s="18"/>
-      <c r="J6" s="18"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="16"/>
+      <c r="J6" s="16"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" s="20" t="str">
+      <c r="A7" s="18" t="str">
         <f>A6</f>
         <v>Product Feature</v>
       </c>
-      <c r="B7" s="21" t="str">
+      <c r="B7" s="19" t="str">
         <f t="shared" ref="B7" si="1">B6</f>
         <v>commission</v>
       </c>
-      <c r="C7" s="24" t="s">
+      <c r="C7" s="22" t="s">
         <v>137</v>
       </c>
-      <c r="D7" s="17" t="s">
+      <c r="D7" s="15" t="s">
         <v>125</v>
       </c>
-      <c r="E7" s="17" t="s">
+      <c r="E7" s="15" t="s">
         <v>125</v>
       </c>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
-      <c r="H7" s="17"/>
-      <c r="I7" s="17"/>
-      <c r="J7" s="17"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="15"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" s="26" t="s">
+      <c r="A8" s="24" t="s">
         <v>134</v>
       </c>
-      <c r="B8" s="27" t="s">
+      <c r="B8" s="25" t="s">
         <v>118</v>
       </c>
-      <c r="C8" s="28" t="s">
+      <c r="C8" s="26" t="s">
         <v>138</v>
       </c>
-      <c r="D8" s="18">
+      <c r="D8" s="16">
         <v>0.8</v>
       </c>
-      <c r="E8" s="18">
+      <c r="E8" s="16">
         <v>0.8</v>
       </c>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="18"/>
-      <c r="I8" s="18"/>
-      <c r="J8" s="18"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="16"/>
+      <c r="J8" s="16"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" s="29" t="str">
+      <c r="A9" s="27" t="str">
         <f>A8</f>
         <v>Base Projection</v>
       </c>
@@ -2307,91 +2318,91 @@
         <f>B8</f>
         <v>mortality</v>
       </c>
-      <c r="C9" s="30" t="s">
+      <c r="C9" s="28" t="s">
         <v>137</v>
       </c>
-      <c r="D9" s="17" t="s">
+      <c r="D9" s="15" t="s">
         <v>110</v>
       </c>
-      <c r="E9" s="17" t="s">
+      <c r="E9" s="15" t="s">
         <v>110</v>
       </c>
-      <c r="F9" s="17"/>
-      <c r="G9" s="17"/>
-      <c r="H9" s="17"/>
-      <c r="I9" s="17"/>
-      <c r="J9" s="17"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="15"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" s="20" t="s">
+      <c r="A10" s="18" t="s">
         <v>134</v>
       </c>
-      <c r="B10" s="21" t="s">
+      <c r="B10" s="19" t="s">
         <v>119</v>
       </c>
-      <c r="C10" s="24" t="s">
+      <c r="C10" s="22" t="s">
         <v>138</v>
       </c>
-      <c r="D10" s="18">
+      <c r="D10" s="16">
         <v>1</v>
       </c>
-      <c r="E10" s="18">
+      <c r="E10" s="16">
         <v>1</v>
       </c>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="18"/>
-      <c r="I10" s="18"/>
-      <c r="J10" s="18"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="16"/>
+      <c r="I10" s="16"/>
+      <c r="J10" s="16"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" s="20" t="str">
+      <c r="A11" s="18" t="str">
         <f>A10</f>
         <v>Base Projection</v>
       </c>
-      <c r="B11" s="21" t="str">
+      <c r="B11" s="19" t="str">
         <f>B10</f>
         <v>lapse</v>
       </c>
-      <c r="C11" s="24" t="s">
+      <c r="C11" s="22" t="s">
         <v>137</v>
       </c>
-      <c r="D11" s="17" t="s">
+      <c r="D11" s="15" t="s">
         <v>124</v>
       </c>
-      <c r="E11" s="17" t="s">
+      <c r="E11" s="15" t="s">
         <v>124</v>
       </c>
-      <c r="F11" s="17"/>
-      <c r="G11" s="17"/>
-      <c r="H11" s="17"/>
-      <c r="I11" s="17"/>
-      <c r="J11" s="17"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="15"/>
+      <c r="J11" s="15"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A12" s="29" t="s">
+      <c r="A12" s="27" t="s">
         <v>134</v>
       </c>
       <c r="B12" t="s">
         <v>120</v>
       </c>
-      <c r="C12" s="30" t="s">
+      <c r="C12" s="28" t="s">
         <v>138</v>
       </c>
-      <c r="D12" s="18">
+      <c r="D12" s="16">
         <v>1</v>
       </c>
-      <c r="E12" s="18">
+      <c r="E12" s="16">
         <v>1</v>
       </c>
-      <c r="F12" s="18"/>
-      <c r="G12" s="18"/>
-      <c r="H12" s="18"/>
-      <c r="I12" s="18"/>
-      <c r="J12" s="18"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="16"/>
+      <c r="I12" s="16"/>
+      <c r="J12" s="16"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A13" s="29" t="str">
+      <c r="A13" s="27" t="str">
         <f>A12</f>
         <v>Base Projection</v>
       </c>
@@ -2399,115 +2410,115 @@
         <f>B12</f>
         <v>expense</v>
       </c>
-      <c r="C13" s="30" t="s">
+      <c r="C13" s="28" t="s">
         <v>137</v>
       </c>
-      <c r="D13" s="17" t="s">
+      <c r="D13" s="15" t="s">
         <v>126</v>
       </c>
-      <c r="E13" s="17" t="s">
+      <c r="E13" s="15" t="s">
         <v>126</v>
       </c>
-      <c r="F13" s="17"/>
-      <c r="G13" s="17"/>
-      <c r="H13" s="17"/>
-      <c r="I13" s="17"/>
-      <c r="J13" s="17"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
+      <c r="I13" s="15"/>
+      <c r="J13" s="15"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14" s="20" t="s">
+      <c r="A14" s="18" t="s">
         <v>134</v>
       </c>
-      <c r="B14" s="21" t="s">
+      <c r="B14" s="19" t="s">
         <v>113</v>
       </c>
-      <c r="C14" s="24" t="s">
+      <c r="C14" s="22" t="s">
         <v>138</v>
       </c>
-      <c r="D14" s="18">
+      <c r="D14" s="16">
         <v>1</v>
       </c>
-      <c r="E14" s="18">
+      <c r="E14" s="16">
         <v>1</v>
       </c>
-      <c r="F14" s="18"/>
-      <c r="G14" s="18"/>
-      <c r="H14" s="18"/>
-      <c r="I14" s="18"/>
-      <c r="J14" s="18"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="16"/>
+      <c r="I14" s="16"/>
+      <c r="J14" s="16"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A15" s="20" t="str">
+      <c r="A15" s="18" t="str">
         <f t="shared" ref="A15:A16" si="2">A14</f>
         <v>Base Projection</v>
       </c>
-      <c r="B15" s="21" t="str">
+      <c r="B15" s="19" t="str">
         <f t="shared" ref="B15:B16" si="3">B14</f>
         <v>disc_rate</v>
       </c>
-      <c r="C15" s="24" t="s">
+      <c r="C15" s="22" t="s">
         <v>137</v>
       </c>
-      <c r="D15" s="17" t="s">
+      <c r="D15" s="15" t="s">
         <v>127</v>
       </c>
-      <c r="E15" s="17" t="s">
+      <c r="E15" s="15" t="s">
         <v>127</v>
       </c>
-      <c r="F15" s="17"/>
-      <c r="G15" s="17"/>
-      <c r="H15" s="17"/>
-      <c r="I15" s="17"/>
-      <c r="J15" s="17"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="15"/>
+      <c r="H15" s="15"/>
+      <c r="I15" s="15"/>
+      <c r="J15" s="15"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A16" s="20" t="str">
+      <c r="A16" s="18" t="str">
         <f t="shared" si="2"/>
         <v>Base Projection</v>
       </c>
-      <c r="B16" s="21" t="str">
+      <c r="B16" s="19" t="str">
         <f t="shared" si="3"/>
         <v>disc_rate</v>
       </c>
-      <c r="C16" s="24" t="s">
+      <c r="C16" s="22" t="s">
         <v>136</v>
       </c>
-      <c r="D16" s="17" t="s">
+      <c r="D16" s="15" t="s">
         <v>113</v>
       </c>
-      <c r="E16" s="17" t="s">
+      <c r="E16" s="15" t="s">
         <v>113</v>
       </c>
-      <c r="F16" s="17"/>
-      <c r="G16" s="17"/>
-      <c r="H16" s="17"/>
-      <c r="I16" s="17"/>
-      <c r="J16" s="17"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="15"/>
+      <c r="H16" s="15"/>
+      <c r="I16" s="15"/>
+      <c r="J16" s="15"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A17" s="29" t="s">
+      <c r="A17" s="27" t="s">
         <v>134</v>
       </c>
       <c r="B17" t="s">
         <v>121</v>
       </c>
-      <c r="C17" s="30" t="s">
+      <c r="C17" s="28" t="s">
         <v>138</v>
       </c>
-      <c r="D17" s="18">
+      <c r="D17" s="16">
         <v>1</v>
       </c>
-      <c r="E17" s="18">
+      <c r="E17" s="16">
         <v>1</v>
       </c>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
-      <c r="H17" s="18"/>
-      <c r="I17" s="18"/>
-      <c r="J17" s="18"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="16"/>
+      <c r="H17" s="16"/>
+      <c r="I17" s="16"/>
+      <c r="J17" s="16"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A18" s="29" t="str">
+      <c r="A18" s="27" t="str">
         <f t="shared" ref="A18:A19" si="4">A17</f>
         <v>Base Projection</v>
       </c>
@@ -2515,23 +2526,23 @@
         <f t="shared" ref="B18:B19" si="5">B17</f>
         <v>invt_return</v>
       </c>
-      <c r="C18" s="30" t="s">
+      <c r="C18" s="28" t="s">
         <v>137</v>
       </c>
-      <c r="D18" s="17" t="s">
+      <c r="D18" s="15" t="s">
         <v>127</v>
       </c>
-      <c r="E18" s="17" t="s">
+      <c r="E18" s="15" t="s">
         <v>127</v>
       </c>
-      <c r="F18" s="17"/>
-      <c r="G18" s="17"/>
-      <c r="H18" s="17"/>
-      <c r="I18" s="17"/>
-      <c r="J18" s="17"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="15"/>
+      <c r="H18" s="15"/>
+      <c r="I18" s="15"/>
+      <c r="J18" s="15"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A19" s="29" t="str">
+      <c r="A19" s="27" t="str">
         <f t="shared" si="4"/>
         <v>Base Projection</v>
       </c>
@@ -2539,252 +2550,252 @@
         <f t="shared" si="5"/>
         <v>invt_return</v>
       </c>
-      <c r="C19" s="30" t="s">
+      <c r="C19" s="28" t="s">
         <v>136</v>
       </c>
-      <c r="D19" s="17" t="s">
+      <c r="D19" s="15" t="s">
         <v>112</v>
       </c>
-      <c r="E19" s="17" t="s">
+      <c r="E19" s="15" t="s">
         <v>112</v>
       </c>
-      <c r="F19" s="17"/>
-      <c r="G19" s="17"/>
-      <c r="H19" s="17"/>
-      <c r="I19" s="17"/>
-      <c r="J19" s="17"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="15"/>
+      <c r="H19" s="15"/>
+      <c r="I19" s="15"/>
+      <c r="J19" s="15"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A20" s="20" t="s">
+      <c r="A20" s="18" t="s">
         <v>134</v>
       </c>
-      <c r="B20" s="21" t="s">
+      <c r="B20" s="19" t="s">
         <v>122</v>
       </c>
-      <c r="C20" s="24" t="s">
+      <c r="C20" s="22" t="s">
         <v>138</v>
       </c>
-      <c r="D20" s="18">
+      <c r="D20" s="16">
         <v>1</v>
       </c>
-      <c r="E20" s="18">
+      <c r="E20" s="16">
         <v>1</v>
       </c>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
-      <c r="H20" s="18"/>
-      <c r="I20" s="18"/>
-      <c r="J20" s="18"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="16"/>
+      <c r="H20" s="16"/>
+      <c r="I20" s="16"/>
+      <c r="J20" s="16"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A21" s="20" t="str">
+      <c r="A21" s="18" t="str">
         <f t="shared" ref="A21:A22" si="6">A20</f>
         <v>Base Projection</v>
       </c>
-      <c r="B21" s="21" t="str">
+      <c r="B21" s="19" t="str">
         <f t="shared" ref="B21:B22" si="7">B20</f>
         <v>prem_tax</v>
       </c>
-      <c r="C21" s="24" t="s">
+      <c r="C21" s="22" t="s">
         <v>137</v>
       </c>
-      <c r="D21" s="17" t="s">
+      <c r="D21" s="15" t="s">
         <v>128</v>
       </c>
-      <c r="E21" s="17" t="s">
+      <c r="E21" s="15" t="s">
         <v>128</v>
       </c>
-      <c r="F21" s="17"/>
-      <c r="G21" s="17"/>
-      <c r="H21" s="17"/>
-      <c r="I21" s="17"/>
-      <c r="J21" s="17"/>
+      <c r="F21" s="15"/>
+      <c r="G21" s="15"/>
+      <c r="H21" s="15"/>
+      <c r="I21" s="15"/>
+      <c r="J21" s="15"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A22" s="20" t="str">
+      <c r="A22" s="18" t="str">
         <f t="shared" si="6"/>
         <v>Base Projection</v>
       </c>
-      <c r="B22" s="21" t="str">
+      <c r="B22" s="19" t="str">
         <f t="shared" si="7"/>
         <v>prem_tax</v>
       </c>
-      <c r="C22" s="24" t="s">
+      <c r="C22" s="22" t="s">
         <v>136</v>
       </c>
-      <c r="D22" s="17" t="s">
+      <c r="D22" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="E22" s="17" t="s">
+      <c r="E22" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="F22" s="17"/>
-      <c r="G22" s="17"/>
-      <c r="H22" s="17"/>
-      <c r="I22" s="17"/>
-      <c r="J22" s="17"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="15"/>
+      <c r="H22" s="15"/>
+      <c r="I22" s="15"/>
+      <c r="J22" s="15"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A23" s="29" t="s">
+      <c r="A23" s="27" t="s">
         <v>134</v>
       </c>
       <c r="B23" t="s">
         <v>123</v>
       </c>
-      <c r="C23" s="30" t="s">
+      <c r="C23" s="28" t="s">
         <v>138</v>
       </c>
-      <c r="D23" s="18">
+      <c r="D23" s="16">
         <v>1</v>
       </c>
-      <c r="E23" s="18">
+      <c r="E23" s="16">
         <v>1</v>
       </c>
-      <c r="F23" s="18"/>
-      <c r="G23" s="18"/>
-      <c r="H23" s="18"/>
-      <c r="I23" s="18"/>
-      <c r="J23" s="18"/>
+      <c r="F23" s="16"/>
+      <c r="G23" s="16"/>
+      <c r="H23" s="16"/>
+      <c r="I23" s="16"/>
+      <c r="J23" s="16"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A24" s="29" t="s">
+      <c r="A24" s="27" t="s">
         <v>134</v>
       </c>
       <c r="B24" t="s">
         <v>123</v>
       </c>
-      <c r="C24" s="30" t="s">
+      <c r="C24" s="28" t="s">
         <v>137</v>
       </c>
-      <c r="D24" s="18" t="s">
+      <c r="D24" s="15" t="s">
         <v>129</v>
       </c>
-      <c r="E24" s="18" t="s">
+      <c r="E24" s="15" t="s">
         <v>129</v>
       </c>
-      <c r="F24" s="18"/>
-      <c r="G24" s="18"/>
-      <c r="H24" s="18"/>
-      <c r="I24" s="18"/>
-      <c r="J24" s="18"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="16"/>
+      <c r="H24" s="16"/>
+      <c r="I24" s="16"/>
+      <c r="J24" s="16"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A25" s="29" t="s">
+      <c r="A25" s="27" t="s">
         <v>134</v>
       </c>
       <c r="B25" t="str">
         <f t="shared" ref="B25" si="8">B23</f>
         <v>tax</v>
       </c>
-      <c r="C25" s="30" t="s">
+      <c r="C25" s="28" t="s">
         <v>136</v>
       </c>
-      <c r="D25" s="31" t="s">
+      <c r="D25" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="E25" s="31" t="s">
+      <c r="E25" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="F25" s="17"/>
-      <c r="G25" s="17"/>
-      <c r="H25" s="17"/>
-      <c r="I25" s="17"/>
-      <c r="J25" s="17"/>
+      <c r="F25" s="15"/>
+      <c r="G25" s="15"/>
+      <c r="H25" s="15"/>
+      <c r="I25" s="15"/>
+      <c r="J25" s="15"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A26" s="22" t="s">
+      <c r="A26" s="20" t="s">
         <v>133</v>
       </c>
-      <c r="B26" s="23" t="s">
+      <c r="B26" s="21" t="s">
         <v>118</v>
       </c>
-      <c r="C26" s="25" t="s">
+      <c r="C26" s="23" t="s">
         <v>138</v>
       </c>
-      <c r="D26" s="18">
+      <c r="D26" s="16">
         <v>0.8</v>
       </c>
-      <c r="E26" s="18">
+      <c r="E26" s="16">
         <v>0.8</v>
       </c>
-      <c r="F26" s="18"/>
-      <c r="G26" s="18"/>
-      <c r="H26" s="18"/>
-      <c r="I26" s="18"/>
-      <c r="J26" s="18"/>
+      <c r="F26" s="16"/>
+      <c r="G26" s="16"/>
+      <c r="H26" s="16"/>
+      <c r="I26" s="16"/>
+      <c r="J26" s="16"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A27" s="20" t="str">
+      <c r="A27" s="18" t="str">
         <f t="shared" ref="A27:A28" si="9">A26</f>
         <v>Valuation</v>
       </c>
-      <c r="B27" s="21" t="str">
+      <c r="B27" s="19" t="str">
         <f t="shared" ref="B27:B28" si="10">B26</f>
         <v>mortality</v>
       </c>
-      <c r="C27" s="24" t="s">
+      <c r="C27" s="22" t="s">
         <v>137</v>
       </c>
-      <c r="D27" s="17" t="s">
+      <c r="D27" s="15" t="s">
         <v>110</v>
       </c>
-      <c r="E27" s="17" t="s">
+      <c r="E27" s="15" t="s">
         <v>110</v>
       </c>
-      <c r="F27" s="17"/>
-      <c r="G27" s="17"/>
-      <c r="H27" s="17"/>
-      <c r="I27" s="17"/>
-      <c r="J27" s="17"/>
+      <c r="F27" s="15"/>
+      <c r="G27" s="15"/>
+      <c r="H27" s="15"/>
+      <c r="I27" s="15"/>
+      <c r="J27" s="15"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A28" s="20" t="str">
+      <c r="A28" s="18" t="str">
         <f t="shared" si="9"/>
         <v>Valuation</v>
       </c>
-      <c r="B28" s="21" t="str">
+      <c r="B28" s="19" t="str">
         <f t="shared" si="10"/>
         <v>mortality</v>
       </c>
-      <c r="C28" s="24" t="s">
+      <c r="C28" s="22" t="s">
         <v>135</v>
       </c>
-      <c r="D28" s="17">
+      <c r="D28" s="15">
         <v>0.1</v>
       </c>
-      <c r="E28" s="17">
+      <c r="E28" s="15">
         <v>0.1</v>
       </c>
-      <c r="F28" s="17"/>
-      <c r="G28" s="17"/>
-      <c r="H28" s="17"/>
-      <c r="I28" s="17"/>
-      <c r="J28" s="17"/>
+      <c r="F28" s="15"/>
+      <c r="G28" s="15"/>
+      <c r="H28" s="15"/>
+      <c r="I28" s="15"/>
+      <c r="J28" s="15"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A29" s="29" t="s">
+      <c r="A29" s="27" t="s">
         <v>133</v>
       </c>
       <c r="B29" t="s">
         <v>119</v>
       </c>
-      <c r="C29" s="30" t="s">
+      <c r="C29" s="28" t="s">
         <v>138</v>
       </c>
-      <c r="D29" s="18">
+      <c r="D29" s="16">
         <v>1</v>
       </c>
-      <c r="E29" s="18">
+      <c r="E29" s="16">
         <v>1</v>
       </c>
-      <c r="F29" s="18"/>
-      <c r="G29" s="18"/>
-      <c r="H29" s="18"/>
-      <c r="I29" s="18"/>
-      <c r="J29" s="18"/>
+      <c r="F29" s="16"/>
+      <c r="G29" s="16"/>
+      <c r="H29" s="16"/>
+      <c r="I29" s="16"/>
+      <c r="J29" s="16"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A30" s="29" t="str">
+      <c r="A30" s="27" t="str">
         <f t="shared" ref="A30:A31" si="11">A29</f>
         <v>Valuation</v>
       </c>
@@ -2792,23 +2803,23 @@
         <f t="shared" ref="B30:B31" si="12">B29</f>
         <v>lapse</v>
       </c>
-      <c r="C30" s="30" t="s">
+      <c r="C30" s="28" t="s">
         <v>137</v>
       </c>
-      <c r="D30" s="17" t="s">
+      <c r="D30" s="15" t="s">
         <v>124</v>
       </c>
-      <c r="E30" s="17" t="s">
+      <c r="E30" s="15" t="s">
         <v>124</v>
       </c>
-      <c r="F30" s="17"/>
-      <c r="G30" s="17"/>
-      <c r="H30" s="17"/>
-      <c r="I30" s="17"/>
-      <c r="J30" s="17"/>
+      <c r="F30" s="15"/>
+      <c r="G30" s="15"/>
+      <c r="H30" s="15"/>
+      <c r="I30" s="15"/>
+      <c r="J30" s="15"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A31" s="29" t="str">
+      <c r="A31" s="27" t="str">
         <f t="shared" si="11"/>
         <v>Valuation</v>
       </c>
@@ -2816,115 +2827,115 @@
         <f t="shared" si="12"/>
         <v>lapse</v>
       </c>
-      <c r="C31" s="30" t="s">
+      <c r="C31" s="28" t="s">
         <v>135</v>
       </c>
-      <c r="D31" s="17">
+      <c r="D31" s="15">
         <v>0.2</v>
       </c>
-      <c r="E31" s="17">
+      <c r="E31" s="15">
         <v>0.2</v>
       </c>
-      <c r="F31" s="17"/>
-      <c r="G31" s="17"/>
-      <c r="H31" s="17"/>
-      <c r="I31" s="17"/>
-      <c r="J31" s="17"/>
+      <c r="F31" s="15"/>
+      <c r="G31" s="15"/>
+      <c r="H31" s="15"/>
+      <c r="I31" s="15"/>
+      <c r="J31" s="15"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A32" s="20" t="s">
+      <c r="A32" s="18" t="s">
         <v>133</v>
       </c>
-      <c r="B32" s="21" t="s">
+      <c r="B32" s="19" t="s">
         <v>120</v>
       </c>
-      <c r="C32" s="24" t="s">
+      <c r="C32" s="22" t="s">
         <v>138</v>
       </c>
-      <c r="D32" s="18">
+      <c r="D32" s="16">
         <v>1</v>
       </c>
-      <c r="E32" s="18">
+      <c r="E32" s="16">
         <v>1</v>
       </c>
-      <c r="F32" s="18"/>
-      <c r="G32" s="18"/>
-      <c r="H32" s="18"/>
-      <c r="I32" s="18"/>
-      <c r="J32" s="18"/>
+      <c r="F32" s="16"/>
+      <c r="G32" s="16"/>
+      <c r="H32" s="16"/>
+      <c r="I32" s="16"/>
+      <c r="J32" s="16"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A33" s="20" t="str">
+      <c r="A33" s="18" t="str">
         <f t="shared" ref="A33:A34" si="13">A32</f>
         <v>Valuation</v>
       </c>
-      <c r="B33" s="21" t="str">
+      <c r="B33" s="19" t="str">
         <f t="shared" ref="B33:B34" si="14">B32</f>
         <v>expense</v>
       </c>
-      <c r="C33" s="24" t="s">
+      <c r="C33" s="22" t="s">
         <v>137</v>
       </c>
-      <c r="D33" s="17" t="s">
+      <c r="D33" s="15" t="s">
         <v>126</v>
       </c>
-      <c r="E33" s="17" t="s">
+      <c r="E33" s="15" t="s">
         <v>126</v>
       </c>
-      <c r="F33" s="17"/>
-      <c r="G33" s="17"/>
-      <c r="H33" s="17"/>
-      <c r="I33" s="17"/>
-      <c r="J33" s="17"/>
+      <c r="F33" s="15"/>
+      <c r="G33" s="15"/>
+      <c r="H33" s="15"/>
+      <c r="I33" s="15"/>
+      <c r="J33" s="15"/>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A34" s="20" t="str">
+      <c r="A34" s="18" t="str">
         <f t="shared" si="13"/>
         <v>Valuation</v>
       </c>
-      <c r="B34" s="21" t="str">
+      <c r="B34" s="19" t="str">
         <f t="shared" si="14"/>
         <v>expense</v>
       </c>
-      <c r="C34" s="24" t="s">
+      <c r="C34" s="22" t="s">
         <v>135</v>
       </c>
-      <c r="D34" s="17">
+      <c r="D34" s="15">
         <v>0.1</v>
       </c>
-      <c r="E34" s="17">
+      <c r="E34" s="15">
         <v>0.1</v>
       </c>
-      <c r="F34" s="17"/>
-      <c r="G34" s="17"/>
-      <c r="H34" s="17"/>
-      <c r="I34" s="17"/>
-      <c r="J34" s="17"/>
+      <c r="F34" s="15"/>
+      <c r="G34" s="15"/>
+      <c r="H34" s="15"/>
+      <c r="I34" s="15"/>
+      <c r="J34" s="15"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A35" s="29" t="s">
+      <c r="A35" s="27" t="s">
         <v>133</v>
       </c>
       <c r="B35" t="s">
         <v>113</v>
       </c>
-      <c r="C35" s="30" t="s">
+      <c r="C35" s="28" t="s">
         <v>138</v>
       </c>
-      <c r="D35" s="18">
+      <c r="D35" s="16">
         <v>1</v>
       </c>
-      <c r="E35" s="18">
+      <c r="E35" s="16">
         <v>1</v>
       </c>
-      <c r="F35" s="18"/>
-      <c r="G35" s="18"/>
-      <c r="H35" s="18"/>
-      <c r="I35" s="18"/>
-      <c r="J35" s="18"/>
+      <c r="F35" s="16"/>
+      <c r="G35" s="16"/>
+      <c r="H35" s="16"/>
+      <c r="I35" s="16"/>
+      <c r="J35" s="16"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A36" s="29" t="str">
+      <c r="A36" s="27" t="str">
         <f t="shared" ref="A36:A38" si="15">A35</f>
         <v>Valuation</v>
       </c>
@@ -2932,23 +2943,23 @@
         <f t="shared" ref="B36:B38" si="16">B35</f>
         <v>disc_rate</v>
       </c>
-      <c r="C36" s="30" t="s">
+      <c r="C36" s="28" t="s">
         <v>137</v>
       </c>
-      <c r="D36" s="17" t="s">
+      <c r="D36" s="15" t="s">
         <v>127</v>
       </c>
-      <c r="E36" s="17" t="s">
+      <c r="E36" s="15" t="s">
         <v>127</v>
       </c>
-      <c r="F36" s="17"/>
-      <c r="G36" s="17"/>
-      <c r="H36" s="17"/>
-      <c r="I36" s="17"/>
-      <c r="J36" s="17"/>
+      <c r="F36" s="15"/>
+      <c r="G36" s="15"/>
+      <c r="H36" s="15"/>
+      <c r="I36" s="15"/>
+      <c r="J36" s="15"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A37" s="29" t="str">
+      <c r="A37" s="27" t="str">
         <f t="shared" si="15"/>
         <v>Valuation</v>
       </c>
@@ -2956,23 +2967,23 @@
         <f t="shared" si="16"/>
         <v>disc_rate</v>
       </c>
-      <c r="C37" s="30" t="s">
+      <c r="C37" s="28" t="s">
         <v>136</v>
       </c>
-      <c r="D37" s="18" t="s">
+      <c r="D37" s="16" t="s">
         <v>114</v>
       </c>
-      <c r="E37" s="18" t="s">
+      <c r="E37" s="16" t="s">
         <v>114</v>
       </c>
-      <c r="F37" s="18"/>
-      <c r="G37" s="18"/>
-      <c r="H37" s="18"/>
-      <c r="I37" s="18"/>
-      <c r="J37" s="18"/>
+      <c r="F37" s="16"/>
+      <c r="G37" s="16"/>
+      <c r="H37" s="16"/>
+      <c r="I37" s="16"/>
+      <c r="J37" s="16"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A38" s="29" t="str">
+      <c r="A38" s="27" t="str">
         <f t="shared" si="15"/>
         <v>Valuation</v>
       </c>
@@ -2980,113 +2991,113 @@
         <f t="shared" si="16"/>
         <v>disc_rate</v>
       </c>
-      <c r="C38" s="30" t="s">
+      <c r="C38" s="28" t="s">
         <v>135</v>
       </c>
-      <c r="D38" s="19">
-        <v>0</v>
-      </c>
-      <c r="E38" s="19">
-        <v>0</v>
-      </c>
-      <c r="F38" s="19"/>
-      <c r="G38" s="19"/>
-      <c r="H38" s="19"/>
-      <c r="I38" s="19"/>
-      <c r="J38" s="19"/>
+      <c r="D38" s="17">
+        <v>0</v>
+      </c>
+      <c r="E38" s="17">
+        <v>0</v>
+      </c>
+      <c r="F38" s="17"/>
+      <c r="G38" s="17"/>
+      <c r="H38" s="17"/>
+      <c r="I38" s="17"/>
+      <c r="J38" s="17"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A39" s="20" t="s">
+      <c r="A39" s="18" t="s">
         <v>133</v>
       </c>
-      <c r="B39" s="21" t="s">
+      <c r="B39" s="19" t="s">
         <v>122</v>
       </c>
-      <c r="C39" s="24" t="s">
+      <c r="C39" s="22" t="s">
         <v>138</v>
       </c>
-      <c r="D39" s="18">
+      <c r="D39" s="16">
         <v>1</v>
       </c>
-      <c r="E39" s="18">
+      <c r="E39" s="16">
         <v>1</v>
       </c>
-      <c r="F39" s="18"/>
-      <c r="G39" s="18"/>
-      <c r="H39" s="18"/>
-      <c r="I39" s="18"/>
-      <c r="J39" s="18"/>
+      <c r="F39" s="16"/>
+      <c r="G39" s="16"/>
+      <c r="H39" s="16"/>
+      <c r="I39" s="16"/>
+      <c r="J39" s="16"/>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A40" s="20" t="s">
+      <c r="A40" s="18" t="s">
         <v>133</v>
       </c>
-      <c r="B40" s="21" t="str">
+      <c r="B40" s="19" t="str">
         <f t="shared" ref="B40:B41" si="17">B39</f>
         <v>prem_tax</v>
       </c>
-      <c r="C40" s="24" t="s">
+      <c r="C40" s="22" t="s">
         <v>137</v>
       </c>
-      <c r="D40" s="17" t="s">
+      <c r="D40" s="15" t="s">
         <v>128</v>
       </c>
-      <c r="E40" s="17" t="s">
+      <c r="E40" s="15" t="s">
         <v>128</v>
       </c>
-      <c r="F40" s="17"/>
-      <c r="G40" s="17"/>
-      <c r="H40" s="17"/>
-      <c r="I40" s="17"/>
-      <c r="J40" s="17"/>
+      <c r="F40" s="15"/>
+      <c r="G40" s="15"/>
+      <c r="H40" s="15"/>
+      <c r="I40" s="15"/>
+      <c r="J40" s="15"/>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A41" s="32" t="s">
+      <c r="A41" s="30" t="s">
         <v>133</v>
       </c>
-      <c r="B41" s="33" t="str">
+      <c r="B41" s="31" t="str">
         <f t="shared" si="17"/>
         <v>prem_tax</v>
       </c>
-      <c r="C41" s="34" t="s">
+      <c r="C41" s="32" t="s">
         <v>136</v>
       </c>
-      <c r="D41" s="17" t="s">
+      <c r="D41" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="E41" s="17" t="s">
+      <c r="E41" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="F41" s="17"/>
-      <c r="G41" s="17"/>
-      <c r="H41" s="17"/>
-      <c r="I41" s="17"/>
-      <c r="J41" s="17"/>
+      <c r="F41" s="15"/>
+      <c r="G41" s="15"/>
+      <c r="H41" s="15"/>
+      <c r="I41" s="15"/>
+      <c r="J41" s="15"/>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A42" s="29" t="s">
+      <c r="A42" s="27" t="s">
         <v>132</v>
       </c>
       <c r="B42" t="s">
         <v>118</v>
       </c>
-      <c r="C42" s="30" t="s">
+      <c r="C42" s="28" t="s">
         <v>138</v>
       </c>
-      <c r="D42" s="18">
+      <c r="D42" s="16">
         <v>0.8</v>
       </c>
-      <c r="E42" s="18">
+      <c r="E42" s="16">
         <v>0.8</v>
       </c>
-      <c r="F42" s="18"/>
-      <c r="G42" s="18"/>
-      <c r="H42" s="18"/>
-      <c r="I42" s="18"/>
-      <c r="J42" s="18"/>
+      <c r="F42" s="16"/>
+      <c r="G42" s="16"/>
+      <c r="H42" s="16"/>
+      <c r="I42" s="16"/>
+      <c r="J42" s="16"/>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A43" s="29" t="str">
+      <c r="A43" s="27" t="str">
         <f t="shared" ref="A43:A44" si="18">A42</f>
         <v>Capital Requirement</v>
       </c>
@@ -3094,23 +3105,23 @@
         <f t="shared" ref="B43:B44" si="19">B42</f>
         <v>mortality</v>
       </c>
-      <c r="C43" s="30" t="s">
+      <c r="C43" s="28" t="s">
         <v>137</v>
       </c>
-      <c r="D43" s="17" t="s">
+      <c r="D43" s="15" t="s">
         <v>110</v>
       </c>
-      <c r="E43" s="17" t="s">
+      <c r="E43" s="15" t="s">
         <v>110</v>
       </c>
-      <c r="F43" s="17"/>
-      <c r="G43" s="17"/>
-      <c r="H43" s="17"/>
-      <c r="I43" s="17"/>
-      <c r="J43" s="17"/>
+      <c r="F43" s="15"/>
+      <c r="G43" s="15"/>
+      <c r="H43" s="15"/>
+      <c r="I43" s="15"/>
+      <c r="J43" s="15"/>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A44" s="29" t="str">
+      <c r="A44" s="27" t="str">
         <f t="shared" si="18"/>
         <v>Capital Requirement</v>
       </c>
@@ -3118,115 +3129,115 @@
         <f t="shared" si="19"/>
         <v>mortality</v>
       </c>
-      <c r="C44" s="30" t="s">
+      <c r="C44" s="28" t="s">
         <v>135</v>
       </c>
-      <c r="D44" s="17">
+      <c r="D44" s="15">
         <v>0.15</v>
       </c>
-      <c r="E44" s="17">
+      <c r="E44" s="15">
         <v>0.15</v>
       </c>
-      <c r="F44" s="17"/>
-      <c r="G44" s="17"/>
-      <c r="H44" s="17"/>
-      <c r="I44" s="17"/>
-      <c r="J44" s="17"/>
+      <c r="F44" s="15"/>
+      <c r="G44" s="15"/>
+      <c r="H44" s="15"/>
+      <c r="I44" s="15"/>
+      <c r="J44" s="15"/>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A45" s="20" t="s">
+      <c r="A45" s="18" t="s">
         <v>132</v>
       </c>
-      <c r="B45" s="21" t="s">
+      <c r="B45" s="19" t="s">
         <v>119</v>
       </c>
-      <c r="C45" s="24" t="s">
+      <c r="C45" s="22" t="s">
         <v>138</v>
       </c>
-      <c r="D45" s="18">
+      <c r="D45" s="16">
         <v>1</v>
       </c>
-      <c r="E45" s="18">
+      <c r="E45" s="16">
         <v>1</v>
       </c>
-      <c r="F45" s="18"/>
-      <c r="G45" s="18"/>
-      <c r="H45" s="18"/>
-      <c r="I45" s="18"/>
-      <c r="J45" s="18"/>
+      <c r="F45" s="16"/>
+      <c r="G45" s="16"/>
+      <c r="H45" s="16"/>
+      <c r="I45" s="16"/>
+      <c r="J45" s="16"/>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A46" s="20" t="str">
+      <c r="A46" s="18" t="str">
         <f t="shared" ref="A46:A47" si="20">A45</f>
         <v>Capital Requirement</v>
       </c>
-      <c r="B46" s="21" t="str">
+      <c r="B46" s="19" t="str">
         <f t="shared" ref="B46:B47" si="21">B45</f>
         <v>lapse</v>
       </c>
-      <c r="C46" s="24" t="s">
+      <c r="C46" s="22" t="s">
         <v>137</v>
       </c>
-      <c r="D46" s="18" t="s">
+      <c r="D46" s="15" t="s">
         <v>124</v>
       </c>
-      <c r="E46" s="18" t="s">
+      <c r="E46" s="15" t="s">
         <v>124</v>
       </c>
-      <c r="F46" s="18"/>
-      <c r="G46" s="18"/>
-      <c r="H46" s="18"/>
-      <c r="I46" s="18"/>
-      <c r="J46" s="18"/>
+      <c r="F46" s="15"/>
+      <c r="G46" s="16"/>
+      <c r="H46" s="16"/>
+      <c r="I46" s="16"/>
+      <c r="J46" s="16"/>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A47" s="20" t="str">
+      <c r="A47" s="18" t="str">
         <f t="shared" si="20"/>
         <v>Capital Requirement</v>
       </c>
-      <c r="B47" s="21" t="str">
+      <c r="B47" s="19" t="str">
         <f t="shared" si="21"/>
         <v>lapse</v>
       </c>
-      <c r="C47" s="24" t="s">
+      <c r="C47" s="22" t="s">
         <v>135</v>
       </c>
-      <c r="D47" s="18">
+      <c r="D47" s="16">
         <v>0.5</v>
       </c>
-      <c r="E47" s="18">
+      <c r="E47" s="16">
         <v>0.5</v>
       </c>
-      <c r="F47" s="18"/>
-      <c r="G47" s="18"/>
-      <c r="H47" s="18"/>
-      <c r="I47" s="18"/>
-      <c r="J47" s="18"/>
+      <c r="F47" s="16"/>
+      <c r="G47" s="16"/>
+      <c r="H47" s="16"/>
+      <c r="I47" s="16"/>
+      <c r="J47" s="16"/>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A48" s="29" t="s">
+      <c r="A48" s="27" t="s">
         <v>132</v>
       </c>
       <c r="B48" t="s">
         <v>120</v>
       </c>
-      <c r="C48" s="30" t="s">
+      <c r="C48" s="28" t="s">
         <v>138</v>
       </c>
-      <c r="D48" s="18">
+      <c r="D48" s="16">
         <v>1</v>
       </c>
-      <c r="E48" s="18">
+      <c r="E48" s="16">
         <v>1</v>
       </c>
-      <c r="F48" s="18"/>
-      <c r="G48" s="18"/>
-      <c r="H48" s="18"/>
-      <c r="I48" s="18"/>
-      <c r="J48" s="18"/>
+      <c r="F48" s="16"/>
+      <c r="G48" s="16"/>
+      <c r="H48" s="16"/>
+      <c r="I48" s="16"/>
+      <c r="J48" s="16"/>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A49" s="29" t="str">
+      <c r="A49" s="27" t="str">
         <f t="shared" ref="A49:A50" si="22">A48</f>
         <v>Capital Requirement</v>
       </c>
@@ -3234,23 +3245,23 @@
         <f t="shared" ref="B49:B50" si="23">B48</f>
         <v>expense</v>
       </c>
-      <c r="C49" s="30" t="s">
+      <c r="C49" s="28" t="s">
         <v>137</v>
       </c>
-      <c r="D49" s="17" t="s">
+      <c r="D49" s="15" t="s">
         <v>126</v>
       </c>
-      <c r="E49" s="17" t="s">
+      <c r="E49" s="15" t="s">
         <v>126</v>
       </c>
-      <c r="F49" s="17"/>
-      <c r="G49" s="17"/>
-      <c r="H49" s="17"/>
-      <c r="I49" s="17"/>
-      <c r="J49" s="17"/>
+      <c r="F49" s="15"/>
+      <c r="G49" s="15"/>
+      <c r="H49" s="15"/>
+      <c r="I49" s="15"/>
+      <c r="J49" s="15"/>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A50" s="29" t="str">
+      <c r="A50" s="27" t="str">
         <f t="shared" si="22"/>
         <v>Capital Requirement</v>
       </c>
@@ -3258,183 +3269,244 @@
         <f t="shared" si="23"/>
         <v>expense</v>
       </c>
-      <c r="C50" s="30" t="s">
+      <c r="C50" s="28" t="s">
         <v>135</v>
       </c>
-      <c r="D50" s="17">
+      <c r="D50" s="15">
         <v>0.2</v>
       </c>
-      <c r="E50" s="17">
+      <c r="E50" s="15">
         <v>0.2</v>
       </c>
-      <c r="F50" s="17"/>
-      <c r="G50" s="17"/>
-      <c r="H50" s="17"/>
-      <c r="I50" s="17"/>
-      <c r="J50" s="17"/>
+      <c r="F50" s="15"/>
+      <c r="G50" s="15"/>
+      <c r="H50" s="15"/>
+      <c r="I50" s="15"/>
+      <c r="J50" s="15"/>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A51" s="20" t="s">
+      <c r="A51" s="18" t="s">
         <v>132</v>
       </c>
-      <c r="B51" s="21" t="s">
+      <c r="B51" s="19" t="s">
         <v>113</v>
       </c>
-      <c r="C51" s="24" t="s">
+      <c r="C51" s="22" t="s">
         <v>138</v>
       </c>
-      <c r="D51" s="18">
+      <c r="D51" s="16">
         <v>1</v>
       </c>
-      <c r="E51" s="18">
+      <c r="E51" s="16">
         <v>1</v>
       </c>
-      <c r="F51" s="18"/>
-      <c r="G51" s="18"/>
-      <c r="H51" s="18"/>
-      <c r="I51" s="18"/>
-      <c r="J51" s="18"/>
+      <c r="F51" s="16"/>
+      <c r="G51" s="16"/>
+      <c r="H51" s="16"/>
+      <c r="I51" s="16"/>
+      <c r="J51" s="16"/>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A52" s="20" t="str">
+      <c r="A52" s="18" t="str">
         <f t="shared" ref="A52:A53" si="24">A51</f>
         <v>Capital Requirement</v>
       </c>
-      <c r="B52" s="21" t="str">
+      <c r="B52" s="19" t="str">
         <f t="shared" ref="B52:B54" si="25">B51</f>
         <v>disc_rate</v>
       </c>
-      <c r="C52" s="24" t="s">
+      <c r="C52" s="22" t="s">
         <v>137</v>
       </c>
-      <c r="D52" s="18" t="s">
+      <c r="D52" s="15" t="s">
         <v>127</v>
       </c>
-      <c r="E52" s="18" t="s">
+      <c r="E52" s="15" t="s">
         <v>127</v>
       </c>
-      <c r="F52" s="18"/>
-      <c r="G52" s="18"/>
-      <c r="H52" s="18"/>
-      <c r="I52" s="18"/>
-      <c r="J52" s="18"/>
+      <c r="F52" s="15"/>
+      <c r="G52" s="16"/>
+      <c r="H52" s="16"/>
+      <c r="I52" s="16"/>
+      <c r="J52" s="16"/>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A53" s="20" t="str">
+      <c r="A53" s="18" t="str">
         <f t="shared" si="24"/>
         <v>Capital Requirement</v>
       </c>
-      <c r="B53" s="21" t="str">
+      <c r="B53" s="19" t="str">
         <f t="shared" si="25"/>
         <v>disc_rate</v>
       </c>
-      <c r="C53" s="24" t="s">
+      <c r="C53" s="22" t="s">
         <v>136</v>
       </c>
-      <c r="D53" s="18" t="s">
+      <c r="D53" s="16" t="s">
         <v>114</v>
       </c>
-      <c r="E53" s="18" t="s">
+      <c r="E53" s="16" t="s">
         <v>114</v>
       </c>
-      <c r="F53" s="18"/>
-      <c r="G53" s="18"/>
-      <c r="H53" s="18"/>
-      <c r="I53" s="18"/>
-      <c r="J53" s="18"/>
+      <c r="F53" s="16"/>
+      <c r="G53" s="16"/>
+      <c r="H53" s="16"/>
+      <c r="I53" s="16"/>
+      <c r="J53" s="16"/>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A54" s="20" t="s">
+      <c r="A54" s="18" t="s">
         <v>132</v>
       </c>
-      <c r="B54" s="21" t="str">
+      <c r="B54" s="19" t="str">
         <f t="shared" si="25"/>
         <v>disc_rate</v>
       </c>
-      <c r="C54" s="24" t="s">
+      <c r="C54" s="22" t="s">
         <v>135</v>
       </c>
-      <c r="D54" s="18">
-        <v>0</v>
-      </c>
-      <c r="E54" s="18">
-        <v>0</v>
-      </c>
-      <c r="F54" s="18"/>
-      <c r="G54" s="18"/>
-      <c r="H54" s="18"/>
-      <c r="I54" s="18"/>
-      <c r="J54" s="18"/>
+      <c r="D54" s="16">
+        <v>0</v>
+      </c>
+      <c r="E54" s="16">
+        <v>0</v>
+      </c>
+      <c r="F54" s="16"/>
+      <c r="G54" s="16"/>
+      <c r="H54" s="16"/>
+      <c r="I54" s="16"/>
+      <c r="J54" s="16"/>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A55" s="29" t="s">
+      <c r="A55" s="27" t="s">
         <v>132</v>
       </c>
       <c r="B55" t="s">
         <v>122</v>
       </c>
-      <c r="C55" s="30" t="s">
+      <c r="C55" s="28" t="s">
         <v>138</v>
       </c>
-      <c r="D55" s="18">
+      <c r="D55" s="16">
         <v>1</v>
       </c>
-      <c r="E55" s="18">
+      <c r="E55" s="16">
         <v>1</v>
       </c>
-      <c r="F55" s="18"/>
-      <c r="G55" s="18"/>
-      <c r="H55" s="18"/>
-      <c r="I55" s="18"/>
-      <c r="J55" s="18"/>
+      <c r="F55" s="16"/>
+      <c r="G55" s="16"/>
+      <c r="H55" s="16"/>
+      <c r="I55" s="16"/>
+      <c r="J55" s="16"/>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A56" s="29" t="s">
+      <c r="A56" s="27" t="s">
         <v>132</v>
       </c>
       <c r="B56" t="s">
         <v>122</v>
       </c>
-      <c r="C56" s="30" t="s">
+      <c r="C56" s="28" t="s">
         <v>137</v>
       </c>
-      <c r="D56" s="18" t="s">
+      <c r="D56" s="15" t="s">
         <v>128</v>
       </c>
-      <c r="E56" s="18" t="s">
+      <c r="E56" s="15" t="s">
         <v>128</v>
       </c>
-      <c r="F56" s="18"/>
-      <c r="G56" s="18"/>
-      <c r="H56" s="18"/>
-      <c r="I56" s="18"/>
-      <c r="J56" s="18"/>
+      <c r="F56" s="15"/>
+      <c r="G56" s="16"/>
+      <c r="H56" s="16"/>
+      <c r="I56" s="16"/>
+      <c r="J56" s="16"/>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A57" s="35" t="s">
+      <c r="A57" s="33" t="s">
         <v>132</v>
       </c>
-      <c r="B57" s="36" t="str">
+      <c r="B57" s="34" t="str">
         <f t="shared" ref="B57" si="26">B56</f>
         <v>prem_tax</v>
       </c>
-      <c r="C57" s="37" t="s">
+      <c r="C57" s="35" t="s">
         <v>136</v>
       </c>
-      <c r="D57" s="17" t="s">
+      <c r="D57" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="E57" s="17" t="s">
+      <c r="E57" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="F57" s="17"/>
-      <c r="G57" s="17"/>
-      <c r="H57" s="17"/>
-      <c r="I57" s="17"/>
-      <c r="J57" s="17"/>
+      <c r="F57" s="15"/>
+      <c r="G57" s="15"/>
+      <c r="H57" s="15"/>
+      <c r="I57" s="15"/>
+      <c r="J57" s="15"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:C57" xr:uid="{C1E729B3-29BA-40F1-80D4-2208DEC4BA85}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="9">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{B156BC01-CF78-4DB9-8231-60269D526FDC}">
+          <x14:formula1>
+            <xm:f>table_listings!$I$3:$I$22</xm:f>
+          </x14:formula1>
+          <xm:sqref>D7:E7</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C9FC5672-069A-4FB2-A184-E15D7D72A88D}">
+          <x14:formula1>
+            <xm:f>table_listings!$M$3:$M$22</xm:f>
+          </x14:formula1>
+          <xm:sqref>D9:E9 D27:E27 D43:E43</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{1B6A367A-1DBF-4CBF-BB27-6C0C1230014B}">
+          <x14:formula1>
+            <xm:f>table_listings!$E$3:$E$22</xm:f>
+          </x14:formula1>
+          <xm:sqref>D5:E5</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C85AB188-8BEE-4865-A320-13F26EF74A68}">
+          <x14:formula1>
+            <xm:f>table_listings!$A$3:$A$22</xm:f>
+          </x14:formula1>
+          <xm:sqref>D3:E3</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{9B11AC40-BA78-465E-A8C2-ABDE8DC86665}">
+          <x14:formula1>
+            <xm:f>table_listings!$Q$3:$Q$22</xm:f>
+          </x14:formula1>
+          <xm:sqref>D11:E11 D30:E30 D46:E46</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{3672E154-D911-4052-9461-331AE0607E99}">
+          <x14:formula1>
+            <xm:f>table_listings!$Y$3:$Y$22</xm:f>
+          </x14:formula1>
+          <xm:sqref>D15:E15 D36:E36 D52:E52 D18:E18</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{AE6B13E0-3C67-444A-9E02-E0311D9C7B6B}">
+          <x14:formula1>
+            <xm:f>table_listings!$U$3:$U$22</xm:f>
+          </x14:formula1>
+          <xm:sqref>D13:E13 D33:E33 D49:E49</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{9147491E-BAE9-4A7D-A399-337FB5EBD658}">
+          <x14:formula1>
+            <xm:f>table_listings!$AC$3:$AC$22</xm:f>
+          </x14:formula1>
+          <xm:sqref>D21:E21 D40:E40 D56:E56</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{A8A71A06-9618-4D56-9684-D28AB541F566}">
+          <x14:formula1>
+            <xm:f>table_listings!$AG$3:$AG$22</xm:f>
+          </x14:formula1>
+          <xm:sqref>D24:E24</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -3448,7 +3520,7 @@
   <cols>
     <col min="1" max="1" width="10.77734375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="2.21875" customWidth="1"/>
     <col min="5" max="5" width="10.77734375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="23.5546875" bestFit="1" customWidth="1"/>
@@ -3483,133 +3555,133 @@
     <col min="35" max="35" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:35" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="12" t="s">
         <v>143</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="E1" s="14" t="s">
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="E1" s="12" t="s">
         <v>144</v>
       </c>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="I1" s="14" t="s">
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="I1" s="12" t="s">
         <v>145</v>
       </c>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="M1" s="14" t="s">
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="M1" s="12" t="s">
         <v>118</v>
       </c>
-      <c r="N1" s="14"/>
-      <c r="O1" s="14"/>
-      <c r="Q1" s="14" t="s">
+      <c r="N1" s="12"/>
+      <c r="O1" s="12"/>
+      <c r="Q1" s="12" t="s">
         <v>119</v>
       </c>
-      <c r="R1" s="14"/>
-      <c r="S1" s="14"/>
-      <c r="U1" s="14" t="s">
+      <c r="R1" s="12"/>
+      <c r="S1" s="12"/>
+      <c r="U1" s="12" t="s">
         <v>120</v>
       </c>
-      <c r="V1" s="14"/>
-      <c r="W1" s="14"/>
-      <c r="Y1" s="14" t="s">
+      <c r="V1" s="12"/>
+      <c r="W1" s="12"/>
+      <c r="Y1" s="12" t="s">
         <v>113</v>
       </c>
-      <c r="Z1" s="14"/>
-      <c r="AA1" s="14"/>
-      <c r="AC1" s="14" t="s">
+      <c r="Z1" s="12"/>
+      <c r="AA1" s="12"/>
+      <c r="AC1" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="AD1" s="14"/>
-      <c r="AE1" s="14"/>
-      <c r="AG1" s="14" t="s">
+      <c r="AD1" s="12"/>
+      <c r="AE1" s="12"/>
+      <c r="AG1" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="AH1" s="14"/>
-      <c r="AI1" s="14"/>
-    </row>
-    <row r="2" spans="1:35" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="15" t="s">
+      <c r="AH1" s="12"/>
+      <c r="AI1" s="12"/>
+    </row>
+    <row r="2" spans="1:35" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="13" t="s">
         <v>109</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="13" t="s">
         <v>147</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="E2" s="13" t="s">
         <v>109</v>
       </c>
-      <c r="F2" s="15" t="s">
+      <c r="F2" s="13" t="s">
         <v>147</v>
       </c>
-      <c r="G2" s="15" t="s">
+      <c r="G2" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="I2" s="15" t="s">
+      <c r="I2" s="13" t="s">
         <v>109</v>
       </c>
-      <c r="J2" s="15" t="s">
+      <c r="J2" s="13" t="s">
         <v>147</v>
       </c>
-      <c r="K2" s="15" t="s">
+      <c r="K2" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="M2" s="15" t="s">
+      <c r="M2" s="13" t="s">
         <v>109</v>
       </c>
-      <c r="N2" s="15" t="s">
+      <c r="N2" s="13" t="s">
         <v>147</v>
       </c>
-      <c r="O2" s="15" t="s">
+      <c r="O2" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="Q2" s="15" t="s">
+      <c r="Q2" s="13" t="s">
         <v>109</v>
       </c>
-      <c r="R2" s="15" t="s">
+      <c r="R2" s="13" t="s">
         <v>147</v>
       </c>
-      <c r="S2" s="15" t="s">
+      <c r="S2" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="U2" s="15" t="s">
+      <c r="U2" s="13" t="s">
         <v>109</v>
       </c>
-      <c r="V2" s="15" t="s">
+      <c r="V2" s="13" t="s">
         <v>147</v>
       </c>
-      <c r="W2" s="15" t="s">
+      <c r="W2" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="Y2" s="15" t="s">
+      <c r="Y2" s="13" t="s">
         <v>109</v>
       </c>
-      <c r="Z2" s="15" t="s">
+      <c r="Z2" s="13" t="s">
         <v>147</v>
       </c>
-      <c r="AA2" s="15" t="s">
+      <c r="AA2" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="AC2" s="15" t="s">
+      <c r="AC2" s="13" t="s">
         <v>109</v>
       </c>
-      <c r="AD2" s="15" t="s">
+      <c r="AD2" s="13" t="s">
         <v>147</v>
       </c>
-      <c r="AE2" s="15" t="s">
+      <c r="AE2" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="AG2" s="15" t="s">
+      <c r="AG2" s="13" t="s">
         <v>109</v>
       </c>
-      <c r="AH2" s="15" t="s">
+      <c r="AH2" s="13" t="s">
         <v>147</v>
       </c>
-      <c r="AI2" s="15" t="s">
+      <c r="AI2" s="13" t="s">
         <v>111</v>
       </c>
     </row>
@@ -5814,994 +5886,265 @@
       </c>
     </row>
     <row r="23" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A23" s="9">
-        <f>[1]death_ben!A22</f>
-        <v>0</v>
-      </c>
-      <c r="B23" s="9">
-        <f>[1]death_ben!B22</f>
-        <v>0</v>
-      </c>
-      <c r="C23" s="9">
-        <f>[1]death_ben!C22</f>
-        <v>0</v>
-      </c>
-      <c r="E23" s="9">
-        <f>[1]surr_ben!A22</f>
-        <v>0</v>
-      </c>
-      <c r="F23" s="9">
-        <f>[1]surr_ben!B22</f>
-        <v>0</v>
-      </c>
-      <c r="G23" s="9">
-        <f>[1]surr_ben!C22</f>
-        <v>0</v>
-      </c>
-      <c r="I23" s="9">
-        <f>[1]commission!A22</f>
-        <v>0</v>
-      </c>
-      <c r="J23" s="9">
-        <f>[1]commission!B22</f>
-        <v>0</v>
-      </c>
-      <c r="K23" s="9">
-        <f>[1]commission!C22</f>
-        <v>0</v>
-      </c>
-      <c r="M23" s="9">
-        <f>[1]mortality!A22</f>
-        <v>0</v>
-      </c>
-      <c r="N23" s="9">
-        <f>[1]mortality!B22</f>
-        <v>0</v>
-      </c>
-      <c r="O23" s="9">
-        <f>[1]mortality!C22</f>
-        <v>0</v>
-      </c>
-      <c r="Q23" s="9">
-        <f>[1]lapse!A22</f>
-        <v>0</v>
-      </c>
-      <c r="R23" s="9">
-        <f>[1]lapse!B22</f>
-        <v>0</v>
-      </c>
-      <c r="S23" s="9">
-        <f>[1]lapse!C22</f>
-        <v>0</v>
-      </c>
-      <c r="U23" s="9">
-        <f>[1]expense!A22</f>
-        <v>0</v>
-      </c>
-      <c r="V23" s="9">
-        <f>[1]expense!B22</f>
-        <v>0</v>
-      </c>
-      <c r="W23" s="9">
-        <f>[1]expense!C22</f>
-        <v>0</v>
-      </c>
-      <c r="Y23" s="9">
-        <f>[1]disc_rate!A22</f>
-        <v>0</v>
-      </c>
-      <c r="Z23" s="9">
-        <f>[1]disc_rate!B22</f>
-        <v>0</v>
-      </c>
-      <c r="AA23" s="9">
-        <f>[1]disc_rate!C22</f>
-        <v>0</v>
-      </c>
-      <c r="AC23" s="9">
-        <f>[1]prem_tax!A22</f>
-        <v>0</v>
-      </c>
-      <c r="AD23" s="9">
-        <f>[1]prem_tax!B22</f>
-        <v>0</v>
-      </c>
-      <c r="AE23" s="9">
-        <f>[1]prem_tax!C22</f>
-        <v>0</v>
-      </c>
-      <c r="AG23" s="9">
-        <f>[1]tax!A22</f>
-        <v>0</v>
-      </c>
-      <c r="AH23" s="9">
-        <f>[1]tax!B22</f>
-        <v>0</v>
-      </c>
-      <c r="AI23" s="9">
-        <f>[1]tax!C22</f>
-        <v>0</v>
-      </c>
+      <c r="A23" s="9"/>
+      <c r="B23" s="9"/>
+      <c r="C23" s="9"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="9"/>
+      <c r="I23" s="9"/>
+      <c r="J23" s="9"/>
+      <c r="K23" s="9"/>
+      <c r="M23" s="9"/>
+      <c r="N23" s="9"/>
+      <c r="O23" s="9"/>
+      <c r="Q23" s="9"/>
+      <c r="R23" s="9"/>
+      <c r="S23" s="9"/>
+      <c r="U23" s="9"/>
+      <c r="V23" s="9"/>
+      <c r="W23" s="9"/>
+      <c r="Y23" s="9"/>
+      <c r="Z23" s="9"/>
+      <c r="AA23" s="9"/>
+      <c r="AC23" s="9"/>
+      <c r="AD23" s="9"/>
+      <c r="AE23" s="9"/>
+      <c r="AG23" s="9"/>
+      <c r="AH23" s="9"/>
+      <c r="AI23" s="9"/>
     </row>
     <row r="24" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A24" s="9">
-        <f>[1]death_ben!A23</f>
-        <v>0</v>
-      </c>
-      <c r="B24" s="9">
-        <f>[1]death_ben!B23</f>
-        <v>0</v>
-      </c>
-      <c r="C24" s="9">
-        <f>[1]death_ben!C23</f>
-        <v>0</v>
-      </c>
-      <c r="E24" s="9">
-        <f>[1]surr_ben!A23</f>
-        <v>0</v>
-      </c>
-      <c r="F24" s="9">
-        <f>[1]surr_ben!B23</f>
-        <v>0</v>
-      </c>
-      <c r="G24" s="9">
-        <f>[1]surr_ben!C23</f>
-        <v>0</v>
-      </c>
-      <c r="I24" s="9">
-        <f>[1]commission!A23</f>
-        <v>0</v>
-      </c>
-      <c r="J24" s="9">
-        <f>[1]commission!B23</f>
-        <v>0</v>
-      </c>
-      <c r="K24" s="9">
-        <f>[1]commission!C23</f>
-        <v>0</v>
-      </c>
-      <c r="M24" s="9">
-        <f>[1]mortality!A23</f>
-        <v>0</v>
-      </c>
-      <c r="N24" s="9">
-        <f>[1]mortality!B23</f>
-        <v>0</v>
-      </c>
-      <c r="O24" s="9">
-        <f>[1]mortality!C23</f>
-        <v>0</v>
-      </c>
-      <c r="Q24" s="9">
-        <f>[1]lapse!A23</f>
-        <v>0</v>
-      </c>
-      <c r="R24" s="9">
-        <f>[1]lapse!B23</f>
-        <v>0</v>
-      </c>
-      <c r="S24" s="9">
-        <f>[1]lapse!C23</f>
-        <v>0</v>
-      </c>
-      <c r="U24" s="9">
-        <f>[1]expense!A23</f>
-        <v>0</v>
-      </c>
-      <c r="V24" s="9">
-        <f>[1]expense!B23</f>
-        <v>0</v>
-      </c>
-      <c r="W24" s="9">
-        <f>[1]expense!C23</f>
-        <v>0</v>
-      </c>
-      <c r="Y24" s="9">
-        <f>[1]disc_rate!A23</f>
-        <v>0</v>
-      </c>
-      <c r="Z24" s="9">
-        <f>[1]disc_rate!B23</f>
-        <v>0</v>
-      </c>
-      <c r="AA24" s="9">
-        <f>[1]disc_rate!C23</f>
-        <v>0</v>
-      </c>
-      <c r="AC24" s="9">
-        <f>[1]prem_tax!A23</f>
-        <v>0</v>
-      </c>
-      <c r="AD24" s="9">
-        <f>[1]prem_tax!B23</f>
-        <v>0</v>
-      </c>
-      <c r="AE24" s="9">
-        <f>[1]prem_tax!C23</f>
-        <v>0</v>
-      </c>
-      <c r="AG24" s="9">
-        <f>[1]tax!A23</f>
-        <v>0</v>
-      </c>
-      <c r="AH24" s="9">
-        <f>[1]tax!B23</f>
-        <v>0</v>
-      </c>
-      <c r="AI24" s="9">
-        <f>[1]tax!C23</f>
-        <v>0</v>
-      </c>
+      <c r="A24" s="9"/>
+      <c r="B24" s="9"/>
+      <c r="C24" s="9"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="9"/>
+      <c r="I24" s="9"/>
+      <c r="J24" s="9"/>
+      <c r="K24" s="9"/>
+      <c r="M24" s="9"/>
+      <c r="N24" s="9"/>
+      <c r="O24" s="9"/>
+      <c r="Q24" s="9"/>
+      <c r="R24" s="9"/>
+      <c r="S24" s="9"/>
+      <c r="U24" s="9"/>
+      <c r="V24" s="9"/>
+      <c r="W24" s="9"/>
+      <c r="Y24" s="9"/>
+      <c r="Z24" s="9"/>
+      <c r="AA24" s="9"/>
+      <c r="AC24" s="9"/>
+      <c r="AD24" s="9"/>
+      <c r="AE24" s="9"/>
+      <c r="AG24" s="9"/>
+      <c r="AH24" s="9"/>
+      <c r="AI24" s="9"/>
     </row>
     <row r="25" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A25" s="9">
-        <f>[1]death_ben!A24</f>
-        <v>0</v>
-      </c>
-      <c r="B25" s="9">
-        <f>[1]death_ben!B24</f>
-        <v>0</v>
-      </c>
-      <c r="C25" s="9">
-        <f>[1]death_ben!C24</f>
-        <v>0</v>
-      </c>
-      <c r="E25" s="9">
-        <f>[1]surr_ben!A24</f>
-        <v>0</v>
-      </c>
-      <c r="F25" s="9">
-        <f>[1]surr_ben!B24</f>
-        <v>0</v>
-      </c>
-      <c r="G25" s="9">
-        <f>[1]surr_ben!C24</f>
-        <v>0</v>
-      </c>
-      <c r="I25" s="9">
-        <f>[1]commission!A24</f>
-        <v>0</v>
-      </c>
-      <c r="J25" s="9">
-        <f>[1]commission!B24</f>
-        <v>0</v>
-      </c>
-      <c r="K25" s="9">
-        <f>[1]commission!C24</f>
-        <v>0</v>
-      </c>
-      <c r="M25" s="9">
-        <f>[1]mortality!A24</f>
-        <v>0</v>
-      </c>
-      <c r="N25" s="9">
-        <f>[1]mortality!B24</f>
-        <v>0</v>
-      </c>
-      <c r="O25" s="9">
-        <f>[1]mortality!C24</f>
-        <v>0</v>
-      </c>
-      <c r="Q25" s="9">
-        <f>[1]lapse!A24</f>
-        <v>0</v>
-      </c>
-      <c r="R25" s="9">
-        <f>[1]lapse!B24</f>
-        <v>0</v>
-      </c>
-      <c r="S25" s="9">
-        <f>[1]lapse!C24</f>
-        <v>0</v>
-      </c>
-      <c r="U25" s="9">
-        <f>[1]expense!A24</f>
-        <v>0</v>
-      </c>
-      <c r="V25" s="9">
-        <f>[1]expense!B24</f>
-        <v>0</v>
-      </c>
-      <c r="W25" s="9">
-        <f>[1]expense!C24</f>
-        <v>0</v>
-      </c>
-      <c r="Y25" s="9">
-        <f>[1]disc_rate!A24</f>
-        <v>0</v>
-      </c>
-      <c r="Z25" s="9">
-        <f>[1]disc_rate!B24</f>
-        <v>0</v>
-      </c>
-      <c r="AA25" s="9">
-        <f>[1]disc_rate!C24</f>
-        <v>0</v>
-      </c>
-      <c r="AC25" s="9">
-        <f>[1]prem_tax!A24</f>
-        <v>0</v>
-      </c>
-      <c r="AD25" s="9">
-        <f>[1]prem_tax!B24</f>
-        <v>0</v>
-      </c>
-      <c r="AE25" s="9">
-        <f>[1]prem_tax!C24</f>
-        <v>0</v>
-      </c>
-      <c r="AG25" s="9">
-        <f>[1]tax!A24</f>
-        <v>0</v>
-      </c>
-      <c r="AH25" s="9">
-        <f>[1]tax!B24</f>
-        <v>0</v>
-      </c>
-      <c r="AI25" s="9">
-        <f>[1]tax!C24</f>
-        <v>0</v>
-      </c>
+      <c r="A25" s="9"/>
+      <c r="B25" s="9"/>
+      <c r="C25" s="9"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="9"/>
+      <c r="G25" s="9"/>
+      <c r="I25" s="9"/>
+      <c r="J25" s="9"/>
+      <c r="K25" s="9"/>
+      <c r="M25" s="9"/>
+      <c r="N25" s="9"/>
+      <c r="O25" s="9"/>
+      <c r="Q25" s="9"/>
+      <c r="R25" s="9"/>
+      <c r="S25" s="9"/>
+      <c r="U25" s="9"/>
+      <c r="V25" s="9"/>
+      <c r="W25" s="9"/>
+      <c r="Y25" s="9"/>
+      <c r="Z25" s="9"/>
+      <c r="AA25" s="9"/>
+      <c r="AC25" s="9"/>
+      <c r="AD25" s="9"/>
+      <c r="AE25" s="9"/>
+      <c r="AG25" s="9"/>
+      <c r="AH25" s="9"/>
+      <c r="AI25" s="9"/>
     </row>
     <row r="26" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A26" s="9">
-        <f>[1]death_ben!A25</f>
-        <v>0</v>
-      </c>
-      <c r="B26" s="9">
-        <f>[1]death_ben!B25</f>
-        <v>0</v>
-      </c>
-      <c r="C26" s="9">
-        <f>[1]death_ben!C25</f>
-        <v>0</v>
-      </c>
-      <c r="E26" s="9">
-        <f>[1]surr_ben!A25</f>
-        <v>0</v>
-      </c>
-      <c r="F26" s="9">
-        <f>[1]surr_ben!B25</f>
-        <v>0</v>
-      </c>
-      <c r="G26" s="9">
-        <f>[1]surr_ben!C25</f>
-        <v>0</v>
-      </c>
-      <c r="I26" s="9">
-        <f>[1]commission!A25</f>
-        <v>0</v>
-      </c>
-      <c r="J26" s="9">
-        <f>[1]commission!B25</f>
-        <v>0</v>
-      </c>
-      <c r="K26" s="9">
-        <f>[1]commission!C25</f>
-        <v>0</v>
-      </c>
-      <c r="M26" s="9">
-        <f>[1]mortality!A25</f>
-        <v>0</v>
-      </c>
-      <c r="N26" s="9">
-        <f>[1]mortality!B25</f>
-        <v>0</v>
-      </c>
-      <c r="O26" s="9">
-        <f>[1]mortality!C25</f>
-        <v>0</v>
-      </c>
-      <c r="Q26" s="9">
-        <f>[1]lapse!A25</f>
-        <v>0</v>
-      </c>
-      <c r="R26" s="9">
-        <f>[1]lapse!B25</f>
-        <v>0</v>
-      </c>
-      <c r="S26" s="9">
-        <f>[1]lapse!C25</f>
-        <v>0</v>
-      </c>
-      <c r="U26" s="9">
-        <f>[1]expense!A25</f>
-        <v>0</v>
-      </c>
-      <c r="V26" s="9">
-        <f>[1]expense!B25</f>
-        <v>0</v>
-      </c>
-      <c r="W26" s="9">
-        <f>[1]expense!C25</f>
-        <v>0</v>
-      </c>
-      <c r="Y26" s="9">
-        <f>[1]disc_rate!A25</f>
-        <v>0</v>
-      </c>
-      <c r="Z26" s="9">
-        <f>[1]disc_rate!B25</f>
-        <v>0</v>
-      </c>
-      <c r="AA26" s="9">
-        <f>[1]disc_rate!C25</f>
-        <v>0</v>
-      </c>
-      <c r="AC26" s="9">
-        <f>[1]prem_tax!A25</f>
-        <v>0</v>
-      </c>
-      <c r="AD26" s="9">
-        <f>[1]prem_tax!B25</f>
-        <v>0</v>
-      </c>
-      <c r="AE26" s="9">
-        <f>[1]prem_tax!C25</f>
-        <v>0</v>
-      </c>
-      <c r="AG26" s="9">
-        <f>[1]tax!A25</f>
-        <v>0</v>
-      </c>
-      <c r="AH26" s="9">
-        <f>[1]tax!B25</f>
-        <v>0</v>
-      </c>
-      <c r="AI26" s="9">
-        <f>[1]tax!C25</f>
-        <v>0</v>
-      </c>
+      <c r="A26" s="9"/>
+      <c r="B26" s="9"/>
+      <c r="C26" s="9"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="9"/>
+      <c r="G26" s="9"/>
+      <c r="I26" s="9"/>
+      <c r="J26" s="9"/>
+      <c r="K26" s="9"/>
+      <c r="M26" s="9"/>
+      <c r="N26" s="9"/>
+      <c r="O26" s="9"/>
+      <c r="Q26" s="9"/>
+      <c r="R26" s="9"/>
+      <c r="S26" s="9"/>
+      <c r="U26" s="9"/>
+      <c r="V26" s="9"/>
+      <c r="W26" s="9"/>
+      <c r="Y26" s="9"/>
+      <c r="Z26" s="9"/>
+      <c r="AA26" s="9"/>
+      <c r="AC26" s="9"/>
+      <c r="AD26" s="9"/>
+      <c r="AE26" s="9"/>
+      <c r="AG26" s="9"/>
+      <c r="AH26" s="9"/>
+      <c r="AI26" s="9"/>
     </row>
     <row r="27" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A27" s="9">
-        <f>[1]death_ben!A26</f>
-        <v>0</v>
-      </c>
-      <c r="B27" s="9">
-        <f>[1]death_ben!B26</f>
-        <v>0</v>
-      </c>
-      <c r="C27" s="9">
-        <f>[1]death_ben!C26</f>
-        <v>0</v>
-      </c>
-      <c r="E27" s="9">
-        <f>[1]surr_ben!A26</f>
-        <v>0</v>
-      </c>
-      <c r="F27" s="9">
-        <f>[1]surr_ben!B26</f>
-        <v>0</v>
-      </c>
-      <c r="G27" s="9">
-        <f>[1]surr_ben!C26</f>
-        <v>0</v>
-      </c>
-      <c r="I27" s="9">
-        <f>[1]commission!A26</f>
-        <v>0</v>
-      </c>
-      <c r="J27" s="9">
-        <f>[1]commission!B26</f>
-        <v>0</v>
-      </c>
-      <c r="K27" s="9">
-        <f>[1]commission!C26</f>
-        <v>0</v>
-      </c>
-      <c r="M27" s="9">
-        <f>[1]mortality!A26</f>
-        <v>0</v>
-      </c>
-      <c r="N27" s="9">
-        <f>[1]mortality!B26</f>
-        <v>0</v>
-      </c>
-      <c r="O27" s="9">
-        <f>[1]mortality!C26</f>
-        <v>0</v>
-      </c>
-      <c r="Q27" s="9">
-        <f>[1]lapse!A26</f>
-        <v>0</v>
-      </c>
-      <c r="R27" s="9">
-        <f>[1]lapse!B26</f>
-        <v>0</v>
-      </c>
-      <c r="S27" s="9">
-        <f>[1]lapse!C26</f>
-        <v>0</v>
-      </c>
-      <c r="U27" s="9">
-        <f>[1]expense!A26</f>
-        <v>0</v>
-      </c>
-      <c r="V27" s="9">
-        <f>[1]expense!B26</f>
-        <v>0</v>
-      </c>
-      <c r="W27" s="9">
-        <f>[1]expense!C26</f>
-        <v>0</v>
-      </c>
-      <c r="Y27" s="9">
-        <f>[1]disc_rate!A26</f>
-        <v>0</v>
-      </c>
-      <c r="Z27" s="9">
-        <f>[1]disc_rate!B26</f>
-        <v>0</v>
-      </c>
-      <c r="AA27" s="9">
-        <f>[1]disc_rate!C26</f>
-        <v>0</v>
-      </c>
-      <c r="AC27" s="9">
-        <f>[1]prem_tax!A26</f>
-        <v>0</v>
-      </c>
-      <c r="AD27" s="9">
-        <f>[1]prem_tax!B26</f>
-        <v>0</v>
-      </c>
-      <c r="AE27" s="9">
-        <f>[1]prem_tax!C26</f>
-        <v>0</v>
-      </c>
-      <c r="AG27" s="9">
-        <f>[1]tax!A26</f>
-        <v>0</v>
-      </c>
-      <c r="AH27" s="9">
-        <f>[1]tax!B26</f>
-        <v>0</v>
-      </c>
-      <c r="AI27" s="9">
-        <f>[1]tax!C26</f>
-        <v>0</v>
-      </c>
+      <c r="A27" s="9"/>
+      <c r="B27" s="9"/>
+      <c r="C27" s="9"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9"/>
+      <c r="G27" s="9"/>
+      <c r="I27" s="9"/>
+      <c r="J27" s="9"/>
+      <c r="K27" s="9"/>
+      <c r="M27" s="9"/>
+      <c r="N27" s="9"/>
+      <c r="O27" s="9"/>
+      <c r="Q27" s="9"/>
+      <c r="R27" s="9"/>
+      <c r="S27" s="9"/>
+      <c r="U27" s="9"/>
+      <c r="V27" s="9"/>
+      <c r="W27" s="9"/>
+      <c r="Y27" s="9"/>
+      <c r="Z27" s="9"/>
+      <c r="AA27" s="9"/>
+      <c r="AC27" s="9"/>
+      <c r="AD27" s="9"/>
+      <c r="AE27" s="9"/>
+      <c r="AG27" s="9"/>
+      <c r="AH27" s="9"/>
+      <c r="AI27" s="9"/>
     </row>
     <row r="28" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A28" s="9">
-        <f>[1]death_ben!A27</f>
-        <v>0</v>
-      </c>
-      <c r="B28" s="9">
-        <f>[1]death_ben!B27</f>
-        <v>0</v>
-      </c>
-      <c r="C28" s="9">
-        <f>[1]death_ben!C27</f>
-        <v>0</v>
-      </c>
-      <c r="E28" s="9">
-        <f>[1]surr_ben!A27</f>
-        <v>0</v>
-      </c>
-      <c r="F28" s="9">
-        <f>[1]surr_ben!B27</f>
-        <v>0</v>
-      </c>
-      <c r="G28" s="9">
-        <f>[1]surr_ben!C27</f>
-        <v>0</v>
-      </c>
-      <c r="I28" s="9">
-        <f>[1]commission!A27</f>
-        <v>0</v>
-      </c>
-      <c r="J28" s="9">
-        <f>[1]commission!B27</f>
-        <v>0</v>
-      </c>
-      <c r="K28" s="9">
-        <f>[1]commission!C27</f>
-        <v>0</v>
-      </c>
-      <c r="M28" s="9">
-        <f>[1]mortality!A27</f>
-        <v>0</v>
-      </c>
-      <c r="N28" s="9">
-        <f>[1]mortality!B27</f>
-        <v>0</v>
-      </c>
-      <c r="O28" s="9">
-        <f>[1]mortality!C27</f>
-        <v>0</v>
-      </c>
-      <c r="Q28" s="9">
-        <f>[1]lapse!A27</f>
-        <v>0</v>
-      </c>
-      <c r="R28" s="9">
-        <f>[1]lapse!B27</f>
-        <v>0</v>
-      </c>
-      <c r="S28" s="9">
-        <f>[1]lapse!C27</f>
-        <v>0</v>
-      </c>
-      <c r="U28" s="9">
-        <f>[1]expense!A27</f>
-        <v>0</v>
-      </c>
-      <c r="V28" s="9">
-        <f>[1]expense!B27</f>
-        <v>0</v>
-      </c>
-      <c r="W28" s="9">
-        <f>[1]expense!C27</f>
-        <v>0</v>
-      </c>
-      <c r="Y28" s="9">
-        <f>[1]disc_rate!A27</f>
-        <v>0</v>
-      </c>
-      <c r="Z28" s="9">
-        <f>[1]disc_rate!B27</f>
-        <v>0</v>
-      </c>
-      <c r="AA28" s="9">
-        <f>[1]disc_rate!C27</f>
-        <v>0</v>
-      </c>
-      <c r="AC28" s="9">
-        <f>[1]prem_tax!A27</f>
-        <v>0</v>
-      </c>
-      <c r="AD28" s="9">
-        <f>[1]prem_tax!B27</f>
-        <v>0</v>
-      </c>
-      <c r="AE28" s="9">
-        <f>[1]prem_tax!C27</f>
-        <v>0</v>
-      </c>
-      <c r="AG28" s="9">
-        <f>[1]tax!A27</f>
-        <v>0</v>
-      </c>
-      <c r="AH28" s="9">
-        <f>[1]tax!B27</f>
-        <v>0</v>
-      </c>
-      <c r="AI28" s="9">
-        <f>[1]tax!C27</f>
-        <v>0</v>
-      </c>
+      <c r="A28" s="9"/>
+      <c r="B28" s="9"/>
+      <c r="C28" s="9"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="9"/>
+      <c r="G28" s="9"/>
+      <c r="I28" s="9"/>
+      <c r="J28" s="9"/>
+      <c r="K28" s="9"/>
+      <c r="M28" s="9"/>
+      <c r="N28" s="9"/>
+      <c r="O28" s="9"/>
+      <c r="Q28" s="9"/>
+      <c r="R28" s="9"/>
+      <c r="S28" s="9"/>
+      <c r="U28" s="9"/>
+      <c r="V28" s="9"/>
+      <c r="W28" s="9"/>
+      <c r="Y28" s="9"/>
+      <c r="Z28" s="9"/>
+      <c r="AA28" s="9"/>
+      <c r="AC28" s="9"/>
+      <c r="AD28" s="9"/>
+      <c r="AE28" s="9"/>
+      <c r="AG28" s="9"/>
+      <c r="AH28" s="9"/>
+      <c r="AI28" s="9"/>
     </row>
     <row r="29" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A29" s="9">
-        <f>[1]death_ben!A28</f>
-        <v>0</v>
-      </c>
-      <c r="B29" s="9">
-        <f>[1]death_ben!B28</f>
-        <v>0</v>
-      </c>
-      <c r="C29" s="9">
-        <f>[1]death_ben!C28</f>
-        <v>0</v>
-      </c>
-      <c r="E29" s="9">
-        <f>[1]surr_ben!A28</f>
-        <v>0</v>
-      </c>
-      <c r="F29" s="9">
-        <f>[1]surr_ben!B28</f>
-        <v>0</v>
-      </c>
-      <c r="G29" s="9">
-        <f>[1]surr_ben!C28</f>
-        <v>0</v>
-      </c>
-      <c r="I29" s="9">
-        <f>[1]commission!A28</f>
-        <v>0</v>
-      </c>
-      <c r="J29" s="9">
-        <f>[1]commission!B28</f>
-        <v>0</v>
-      </c>
-      <c r="K29" s="9">
-        <f>[1]commission!C28</f>
-        <v>0</v>
-      </c>
-      <c r="M29" s="9">
-        <f>[1]mortality!A28</f>
-        <v>0</v>
-      </c>
-      <c r="N29" s="9">
-        <f>[1]mortality!B28</f>
-        <v>0</v>
-      </c>
-      <c r="O29" s="9">
-        <f>[1]mortality!C28</f>
-        <v>0</v>
-      </c>
-      <c r="Q29" s="9">
-        <f>[1]lapse!A28</f>
-        <v>0</v>
-      </c>
-      <c r="R29" s="9">
-        <f>[1]lapse!B28</f>
-        <v>0</v>
-      </c>
-      <c r="S29" s="9">
-        <f>[1]lapse!C28</f>
-        <v>0</v>
-      </c>
-      <c r="U29" s="9">
-        <f>[1]expense!A28</f>
-        <v>0</v>
-      </c>
-      <c r="V29" s="9">
-        <f>[1]expense!B28</f>
-        <v>0</v>
-      </c>
-      <c r="W29" s="9">
-        <f>[1]expense!C28</f>
-        <v>0</v>
-      </c>
-      <c r="Y29" s="9">
-        <f>[1]disc_rate!A28</f>
-        <v>0</v>
-      </c>
-      <c r="Z29" s="9">
-        <f>[1]disc_rate!B28</f>
-        <v>0</v>
-      </c>
-      <c r="AA29" s="9">
-        <f>[1]disc_rate!C28</f>
-        <v>0</v>
-      </c>
-      <c r="AC29" s="9">
-        <f>[1]prem_tax!A28</f>
-        <v>0</v>
-      </c>
-      <c r="AD29" s="9">
-        <f>[1]prem_tax!B28</f>
-        <v>0</v>
-      </c>
-      <c r="AE29" s="9">
-        <f>[1]prem_tax!C28</f>
-        <v>0</v>
-      </c>
-      <c r="AG29" s="9">
-        <f>[1]tax!A28</f>
-        <v>0</v>
-      </c>
-      <c r="AH29" s="9">
-        <f>[1]tax!B28</f>
-        <v>0</v>
-      </c>
-      <c r="AI29" s="9">
-        <f>[1]tax!C28</f>
-        <v>0</v>
-      </c>
+      <c r="A29" s="9"/>
+      <c r="B29" s="9"/>
+      <c r="C29" s="9"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="9"/>
+      <c r="G29" s="9"/>
+      <c r="I29" s="9"/>
+      <c r="J29" s="9"/>
+      <c r="K29" s="9"/>
+      <c r="M29" s="9"/>
+      <c r="N29" s="9"/>
+      <c r="O29" s="9"/>
+      <c r="Q29" s="9"/>
+      <c r="R29" s="9"/>
+      <c r="S29" s="9"/>
+      <c r="U29" s="9"/>
+      <c r="V29" s="9"/>
+      <c r="W29" s="9"/>
+      <c r="Y29" s="9"/>
+      <c r="Z29" s="9"/>
+      <c r="AA29" s="9"/>
+      <c r="AC29" s="9"/>
+      <c r="AD29" s="9"/>
+      <c r="AE29" s="9"/>
+      <c r="AG29" s="9"/>
+      <c r="AH29" s="9"/>
+      <c r="AI29" s="9"/>
     </row>
     <row r="30" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A30" s="9">
-        <f>[1]death_ben!A29</f>
-        <v>0</v>
-      </c>
-      <c r="B30" s="9">
-        <f>[1]death_ben!B29</f>
-        <v>0</v>
-      </c>
-      <c r="C30" s="9">
-        <f>[1]death_ben!C29</f>
-        <v>0</v>
-      </c>
-      <c r="E30" s="9">
-        <f>[1]surr_ben!A29</f>
-        <v>0</v>
-      </c>
-      <c r="F30" s="9">
-        <f>[1]surr_ben!B29</f>
-        <v>0</v>
-      </c>
-      <c r="G30" s="9">
-        <f>[1]surr_ben!C29</f>
-        <v>0</v>
-      </c>
-      <c r="I30" s="9">
-        <f>[1]commission!A29</f>
-        <v>0</v>
-      </c>
-      <c r="J30" s="9">
-        <f>[1]commission!B29</f>
-        <v>0</v>
-      </c>
-      <c r="K30" s="9">
-        <f>[1]commission!C29</f>
-        <v>0</v>
-      </c>
-      <c r="M30" s="9">
-        <f>[1]mortality!A29</f>
-        <v>0</v>
-      </c>
-      <c r="N30" s="9">
-        <f>[1]mortality!B29</f>
-        <v>0</v>
-      </c>
-      <c r="O30" s="9">
-        <f>[1]mortality!C29</f>
-        <v>0</v>
-      </c>
-      <c r="Q30" s="9">
-        <f>[1]lapse!A29</f>
-        <v>0</v>
-      </c>
-      <c r="R30" s="9">
-        <f>[1]lapse!B29</f>
-        <v>0</v>
-      </c>
-      <c r="S30" s="9">
-        <f>[1]lapse!C29</f>
-        <v>0</v>
-      </c>
-      <c r="U30" s="9">
-        <f>[1]expense!A29</f>
-        <v>0</v>
-      </c>
-      <c r="V30" s="9">
-        <f>[1]expense!B29</f>
-        <v>0</v>
-      </c>
-      <c r="W30" s="9">
-        <f>[1]expense!C29</f>
-        <v>0</v>
-      </c>
-      <c r="Y30" s="9">
-        <f>[1]disc_rate!A29</f>
-        <v>0</v>
-      </c>
-      <c r="Z30" s="9">
-        <f>[1]disc_rate!B29</f>
-        <v>0</v>
-      </c>
-      <c r="AA30" s="9">
-        <f>[1]disc_rate!C29</f>
-        <v>0</v>
-      </c>
-      <c r="AC30" s="9">
-        <f>[1]prem_tax!A29</f>
-        <v>0</v>
-      </c>
-      <c r="AD30" s="9">
-        <f>[1]prem_tax!B29</f>
-        <v>0</v>
-      </c>
-      <c r="AE30" s="9">
-        <f>[1]prem_tax!C29</f>
-        <v>0</v>
-      </c>
-      <c r="AG30" s="9">
-        <f>[1]tax!A29</f>
-        <v>0</v>
-      </c>
-      <c r="AH30" s="9">
-        <f>[1]tax!B29</f>
-        <v>0</v>
-      </c>
-      <c r="AI30" s="9">
-        <f>[1]tax!C29</f>
-        <v>0</v>
-      </c>
+      <c r="A30" s="9"/>
+      <c r="B30" s="9"/>
+      <c r="C30" s="9"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="9"/>
+      <c r="G30" s="9"/>
+      <c r="I30" s="9"/>
+      <c r="J30" s="9"/>
+      <c r="K30" s="9"/>
+      <c r="M30" s="9"/>
+      <c r="N30" s="9"/>
+      <c r="O30" s="9"/>
+      <c r="Q30" s="9"/>
+      <c r="R30" s="9"/>
+      <c r="S30" s="9"/>
+      <c r="U30" s="9"/>
+      <c r="V30" s="9"/>
+      <c r="W30" s="9"/>
+      <c r="Y30" s="9"/>
+      <c r="Z30" s="9"/>
+      <c r="AA30" s="9"/>
+      <c r="AC30" s="9"/>
+      <c r="AD30" s="9"/>
+      <c r="AE30" s="9"/>
+      <c r="AG30" s="9"/>
+      <c r="AH30" s="9"/>
+      <c r="AI30" s="9"/>
     </row>
     <row r="31" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A31" s="9">
-        <f>[1]death_ben!A30</f>
-        <v>0</v>
-      </c>
-      <c r="B31" s="9">
-        <f>[1]death_ben!B30</f>
-        <v>0</v>
-      </c>
-      <c r="C31" s="9">
-        <f>[1]death_ben!C30</f>
-        <v>0</v>
-      </c>
-      <c r="E31" s="9">
-        <f>[1]surr_ben!A30</f>
-        <v>0</v>
-      </c>
-      <c r="F31" s="9">
-        <f>[1]surr_ben!B30</f>
-        <v>0</v>
-      </c>
-      <c r="G31" s="9">
-        <f>[1]surr_ben!C30</f>
-        <v>0</v>
-      </c>
-      <c r="I31" s="9">
-        <f>[1]commission!A30</f>
-        <v>0</v>
-      </c>
-      <c r="J31" s="9">
-        <f>[1]commission!B30</f>
-        <v>0</v>
-      </c>
-      <c r="K31" s="9">
-        <f>[1]commission!C30</f>
-        <v>0</v>
-      </c>
-      <c r="M31" s="9">
-        <f>[1]mortality!A30</f>
-        <v>0</v>
-      </c>
-      <c r="N31" s="9">
-        <f>[1]mortality!B30</f>
-        <v>0</v>
-      </c>
-      <c r="O31" s="9">
-        <f>[1]mortality!C30</f>
-        <v>0</v>
-      </c>
-      <c r="Q31" s="9">
-        <f>[1]lapse!A30</f>
-        <v>0</v>
-      </c>
-      <c r="R31" s="9">
-        <f>[1]lapse!B30</f>
-        <v>0</v>
-      </c>
-      <c r="S31" s="9">
-        <f>[1]lapse!C30</f>
-        <v>0</v>
-      </c>
-      <c r="U31" s="9">
-        <f>[1]expense!A30</f>
-        <v>0</v>
-      </c>
-      <c r="V31" s="9">
-        <f>[1]expense!B30</f>
-        <v>0</v>
-      </c>
-      <c r="W31" s="9">
-        <f>[1]expense!C30</f>
-        <v>0</v>
-      </c>
-      <c r="Y31" s="9">
-        <f>[1]disc_rate!A30</f>
-        <v>0</v>
-      </c>
-      <c r="Z31" s="9">
-        <f>[1]disc_rate!B30</f>
-        <v>0</v>
-      </c>
-      <c r="AA31" s="9">
-        <f>[1]disc_rate!C30</f>
-        <v>0</v>
-      </c>
-      <c r="AC31" s="9">
-        <f>[1]prem_tax!A30</f>
-        <v>0</v>
-      </c>
-      <c r="AD31" s="9">
-        <f>[1]prem_tax!B30</f>
-        <v>0</v>
-      </c>
-      <c r="AE31" s="9">
-        <f>[1]prem_tax!C30</f>
-        <v>0</v>
-      </c>
-      <c r="AG31" s="9">
-        <f>[1]tax!A30</f>
-        <v>0</v>
-      </c>
-      <c r="AH31" s="9">
-        <f>[1]tax!B30</f>
-        <v>0</v>
-      </c>
-      <c r="AI31" s="9">
-        <f>[1]tax!C30</f>
-        <v>0</v>
-      </c>
+      <c r="A31" s="9"/>
+      <c r="B31" s="9"/>
+      <c r="C31" s="9"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="9"/>
+      <c r="G31" s="9"/>
+      <c r="I31" s="9"/>
+      <c r="J31" s="9"/>
+      <c r="K31" s="9"/>
+      <c r="M31" s="9"/>
+      <c r="N31" s="9"/>
+      <c r="O31" s="9"/>
+      <c r="Q31" s="9"/>
+      <c r="R31" s="9"/>
+      <c r="S31" s="9"/>
+      <c r="U31" s="9"/>
+      <c r="V31" s="9"/>
+      <c r="W31" s="9"/>
+      <c r="Y31" s="9"/>
+      <c r="Z31" s="9"/>
+      <c r="AA31" s="9"/>
+      <c r="AC31" s="9"/>
+      <c r="AD31" s="9"/>
+      <c r="AE31" s="9"/>
+      <c r="AG31" s="9"/>
+      <c r="AH31" s="9"/>
+      <c r="AI31" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6816,7 +6159,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomRight" activeCell="A69" sqref="A69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
experimental stage for user defined formula
- eval(expr) seems easiest to implement compared to other methods e.g. generated functions in a separate file etc
- needs to define scope for setproperty!() and it shouldn't be global esp. since there'll be multiprocessing, hence need to revisit encapsulation with modules
</commit_message>
<xml_diff>
--- a/Input/Settings.xlsx
+++ b/Input/Settings.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Julia\TradLifeModel\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE9B40F1-AD9E-4473-80A0-AA598725AFC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75FD947A-81BA-43D2-883C-256991C97721}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="889" xr2:uid="{ADF8BBD9-0F7A-45CB-8EA8-A3D46B124E82}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="889" activeTab="1" xr2:uid="{ADF8BBD9-0F7A-45CB-8EA8-A3D46B124E82}"/>
   </bookViews>
   <sheets>
     <sheet name="general_settings" sheetId="13" r:id="rId1"/>
     <sheet name="run_settings" sheetId="12" r:id="rId2"/>
     <sheet name="product_setup" sheetId="34" r:id="rId3"/>
     <sheet name="table_listings" sheetId="35" r:id="rId4"/>
-    <sheet name="print_option" sheetId="11" r:id="rId5"/>
+    <sheet name="user_defined_formula" sheetId="36" r:id="rId5"/>
+    <sheet name="print_option" sheetId="11" r:id="rId6"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId6"/>
+    <externalReference r:id="rId7"/>
   </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">product_setup!$A$1:$C$57</definedName>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="179">
   <si>
     <t>acq_exp_per_pol</t>
   </si>
@@ -560,6 +561,27 @@
   </si>
   <si>
     <t>Number of Workers for Multiprocessing</t>
+  </si>
+  <si>
+    <t>Premium</t>
+  </si>
+  <si>
+    <t>Commission</t>
+  </si>
+  <si>
+    <t>User Defined Formula</t>
+  </si>
+  <si>
+    <t>Death_Benefit</t>
+  </si>
+  <si>
+    <t>Survival_Benefit</t>
+  </si>
+  <si>
+    <t>DB02UDT</t>
+  </si>
+  <si>
+    <t>multiple .* amount .* (1 .+ inflator) .^ (Year .- 1)</t>
   </si>
 </sst>
 </file>
@@ -611,7 +633,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -621,6 +643,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -718,7 +746,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -786,6 +814,9 @@
     <xf numFmtId="15" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -813,6 +844,7 @@
     <sheetNames>
       <sheetName val="death_ben"/>
       <sheetName val="DB01"/>
+      <sheetName val="DB02UDT"/>
       <sheetName val="surr_ben"/>
       <sheetName val="SV01"/>
       <sheetName val="commission"/>
@@ -843,9 +875,21 @@
             <v>Mult by Duration</v>
           </cell>
         </row>
+        <row r="3">
+          <cell r="A3" t="str">
+            <v>DB02UDT</v>
+          </cell>
+          <cell r="B3" t="str">
+            <v>Death Benefit Table</v>
+          </cell>
+          <cell r="C3" t="str">
+            <v>User Defined Table</v>
+          </cell>
+        </row>
       </sheetData>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2">
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3">
         <row r="2">
           <cell r="A2" t="str">
             <v>SV01</v>
@@ -858,8 +902,8 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4">
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5">
         <row r="2">
           <cell r="A2" t="str">
             <v>COMM01</v>
@@ -872,8 +916,8 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6">
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7">
         <row r="2">
           <cell r="A2" t="str">
             <v>MORT01</v>
@@ -886,8 +930,8 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="7" refreshError="1"/>
-      <sheetData sheetId="8">
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9">
         <row r="2">
           <cell r="A2" t="str">
             <v>LAPSE01</v>
@@ -900,8 +944,8 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="9" refreshError="1"/>
-      <sheetData sheetId="10">
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11">
         <row r="2">
           <cell r="A2" t="str">
             <v>EXP01</v>
@@ -914,8 +958,8 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="11" refreshError="1"/>
-      <sheetData sheetId="12">
+      <sheetData sheetId="12"/>
+      <sheetData sheetId="13">
         <row r="2">
           <cell r="A2" t="str">
             <v>DISCRT01</v>
@@ -928,8 +972,8 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="13" refreshError="1"/>
-      <sheetData sheetId="14">
+      <sheetData sheetId="14"/>
+      <sheetData sheetId="15">
         <row r="2">
           <cell r="A2" t="str">
             <v>PREMTAX01</v>
@@ -942,8 +986,8 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="15" refreshError="1"/>
-      <sheetData sheetId="16">
+      <sheetData sheetId="16"/>
+      <sheetData sheetId="17">
         <row r="2">
           <cell r="A2" t="str">
             <v>TAX01</v>
@@ -956,7 +1000,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="17" refreshError="1"/>
+      <sheetData sheetId="18"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1261,7 +1305,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F309708F-75E9-4A4E-B1AF-0EC8FC0F4256}">
   <dimension ref="A1:B25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -1323,9 +1367,7 @@
       <c r="A7" t="s">
         <v>149</v>
       </c>
-      <c r="B7" s="15" t="s">
-        <v>117</v>
-      </c>
+      <c r="B7" s="15"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
@@ -1445,11 +1487,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61890AB8-02EC-40E1-960C-9B07CCD09B96}">
   <dimension ref="A1:U19"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomRight" activeCell="F2" sqref="C2:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1513,13 +1555,13 @@
         <v>9</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F2" s="6" t="s">
         <v>10</v>
@@ -2119,7 +2161,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D4" sqref="D4"/>
+      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2183,8 +2225,8 @@
       <c r="C3" s="22" t="s">
         <v>137</v>
       </c>
-      <c r="D3" s="15" t="s">
-        <v>130</v>
+      <c r="D3" s="37" t="s">
+        <v>177</v>
       </c>
       <c r="E3" s="15" t="s">
         <v>130</v>
@@ -3796,17 +3838,17 @@
       </c>
     </row>
     <row r="4" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A4" s="9">
+      <c r="A4" s="9" t="str">
         <f>[1]death_ben!A3</f>
-        <v>0</v>
-      </c>
-      <c r="B4" s="9">
+        <v>DB02UDT</v>
+      </c>
+      <c r="B4" s="9" t="str">
         <f>[1]death_ben!B3</f>
-        <v>0</v>
-      </c>
-      <c r="C4" s="9">
+        <v>Death Benefit Table</v>
+      </c>
+      <c r="C4" s="9" t="str">
         <f>[1]death_ben!C3</f>
-        <v>0</v>
+        <v>User Defined Table</v>
       </c>
       <c r="E4" s="9">
         <f>[1]surr_ben!A3</f>
@@ -6152,6 +6194,65 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2C92756-0135-48D6-8016-1EE97220BD0B}">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="48.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>172</v>
+      </c>
+      <c r="B2" s="2"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>173</v>
+      </c>
+      <c r="B3" s="2"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>175</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>176</v>
+      </c>
+      <c r="B5" s="2"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B6" s="16"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B8" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9F298C4-02FF-4A34-A61E-BC2070858AEB}">
   <dimension ref="A1:C69"/>
   <sheetViews>

</xml_diff>

<commit_message>
udf - fix module and check calc against excel
rename Main.jl to TradLifeModel.jl to not be confused with module Main
</commit_message>
<xml_diff>
--- a/Input/Settings.xlsx
+++ b/Input/Settings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Julia\TradLifeModel\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75FD947A-81BA-43D2-883C-256991C97721}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D793083A-F998-4479-860F-DD2D8D970E34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="889" activeTab="1" xr2:uid="{ADF8BBD9-0F7A-45CB-8EA8-A3D46B124E82}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="889" activeTab="4" xr2:uid="{ADF8BBD9-0F7A-45CB-8EA8-A3D46B124E82}"/>
   </bookViews>
   <sheets>
     <sheet name="general_settings" sheetId="13" r:id="rId1"/>
@@ -581,7 +581,7 @@
     <t>DB02UDT</t>
   </si>
   <si>
-    <t>multiple .* amount .* (1 .+ inflator) .^ (Year .- 1)</t>
+    <t>min.(multiple .* amount .* (1 .+ inflator) .^ (Year .- 1), 200000)</t>
   </si>
 </sst>
 </file>
@@ -847,8 +847,10 @@
       <sheetName val="DB02UDT"/>
       <sheetName val="surr_ben"/>
       <sheetName val="SV01"/>
+      <sheetName val="SV02UDT"/>
       <sheetName val="commission"/>
       <sheetName val="COMM01"/>
+      <sheetName val="COMM02UDT"/>
       <sheetName val="mortality"/>
       <sheetName val="MORT01"/>
       <sheetName val="lapse"/>
@@ -869,7 +871,7 @@
             <v>DB01</v>
           </cell>
           <cell r="B2" t="str">
-            <v>Death Benefit Table</v>
+            <v>Death Benefit Table 01</v>
           </cell>
           <cell r="C2" t="str">
             <v>Mult by Duration</v>
@@ -880,44 +882,68 @@
             <v>DB02UDT</v>
           </cell>
           <cell r="B3" t="str">
-            <v>Death Benefit Table</v>
+            <v>Death Benefit Table 02 UDT</v>
           </cell>
           <cell r="C3" t="str">
             <v>User Defined Table</v>
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
       <sheetData sheetId="3">
         <row r="2">
           <cell r="A2" t="str">
             <v>SV01</v>
           </cell>
           <cell r="B2" t="str">
-            <v>Surrender Value Table</v>
+            <v>Surrender Value Table 01</v>
           </cell>
           <cell r="C2" t="str">
             <v>Policy Year</v>
           </cell>
         </row>
+        <row r="3">
+          <cell r="A3" t="str">
+            <v>SV02UDT</v>
+          </cell>
+          <cell r="B3" t="str">
+            <v>Surrender Value Table 02 UDT</v>
+          </cell>
+          <cell r="C3" t="str">
+            <v>User Defined Table</v>
+          </cell>
+        </row>
       </sheetData>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5">
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="6">
         <row r="2">
           <cell r="A2" t="str">
             <v>COMM01</v>
           </cell>
           <cell r="B2" t="str">
-            <v>Commission Table</v>
+            <v>Commission Table 01</v>
           </cell>
           <cell r="C2" t="str">
             <v>Policy Year</v>
           </cell>
         </row>
+        <row r="3">
+          <cell r="A3" t="str">
+            <v>COMM02UDT</v>
+          </cell>
+          <cell r="B3" t="str">
+            <v>Commission Table 02 UDT</v>
+          </cell>
+          <cell r="C3" t="str">
+            <v>User Defined Table</v>
+          </cell>
+        </row>
       </sheetData>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7">
+      <sheetData sheetId="7" refreshError="1"/>
+      <sheetData sheetId="8" refreshError="1"/>
+      <sheetData sheetId="9">
         <row r="2">
           <cell r="A2" t="str">
             <v>MORT01</v>
@@ -930,8 +956,8 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9">
+      <sheetData sheetId="10" refreshError="1"/>
+      <sheetData sheetId="11">
         <row r="2">
           <cell r="A2" t="str">
             <v>LAPSE01</v>
@@ -944,8 +970,8 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11">
+      <sheetData sheetId="12" refreshError="1"/>
+      <sheetData sheetId="13">
         <row r="2">
           <cell r="A2" t="str">
             <v>EXP01</v>
@@ -958,8 +984,8 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="12"/>
-      <sheetData sheetId="13">
+      <sheetData sheetId="14" refreshError="1"/>
+      <sheetData sheetId="15">
         <row r="2">
           <cell r="A2" t="str">
             <v>DISCRT01</v>
@@ -972,8 +998,8 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="14"/>
-      <sheetData sheetId="15">
+      <sheetData sheetId="16" refreshError="1"/>
+      <sheetData sheetId="17">
         <row r="2">
           <cell r="A2" t="str">
             <v>PREMTAX01</v>
@@ -986,8 +1012,8 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="16"/>
-      <sheetData sheetId="17">
+      <sheetData sheetId="18" refreshError="1"/>
+      <sheetData sheetId="19">
         <row r="2">
           <cell r="A2" t="str">
             <v>TAX01</v>
@@ -1000,7 +1026,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="18"/>
+      <sheetData sheetId="20" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1487,7 +1513,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61890AB8-02EC-40E1-960C-9B07CCD09B96}">
   <dimension ref="A1:U19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -2161,7 +2187,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
+      <selection pane="bottomRight" activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3556,45 +3582,47 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEDF0AF3-210A-43C6-BE28-C257ED849428}">
   <dimension ref="A1:AI31"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.77734375" customWidth="1"/>
+    <col min="2" max="2" width="26.44140625" customWidth="1"/>
+    <col min="3" max="3" width="18.44140625" customWidth="1"/>
     <col min="4" max="4" width="2.21875" customWidth="1"/>
-    <col min="5" max="5" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.77734375" customWidth="1"/>
+    <col min="6" max="6" width="26.44140625" customWidth="1"/>
+    <col min="7" max="7" width="18.44140625" customWidth="1"/>
     <col min="8" max="8" width="2.21875" customWidth="1"/>
-    <col min="9" max="9" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.77734375" customWidth="1"/>
+    <col min="10" max="10" width="26.44140625" customWidth="1"/>
+    <col min="11" max="11" width="18.44140625" customWidth="1"/>
     <col min="12" max="12" width="2.21875" customWidth="1"/>
-    <col min="13" max="13" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="23.5546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.77734375" customWidth="1"/>
+    <col min="14" max="14" width="26.44140625" customWidth="1"/>
+    <col min="15" max="15" width="18.44140625" customWidth="1"/>
     <col min="16" max="16" width="2.21875" customWidth="1"/>
-    <col min="17" max="17" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="23.5546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.77734375" customWidth="1"/>
+    <col min="18" max="18" width="26.44140625" customWidth="1"/>
+    <col min="19" max="19" width="18.44140625" customWidth="1"/>
     <col min="20" max="20" width="2.21875" customWidth="1"/>
-    <col min="21" max="21" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="23.5546875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.77734375" customWidth="1"/>
+    <col min="22" max="22" width="26.44140625" customWidth="1"/>
+    <col min="23" max="23" width="18.44140625" customWidth="1"/>
     <col min="24" max="24" width="2.21875" customWidth="1"/>
-    <col min="25" max="25" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="23.5546875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="15.77734375" customWidth="1"/>
+    <col min="26" max="26" width="26.44140625" customWidth="1"/>
+    <col min="27" max="27" width="18.44140625" customWidth="1"/>
     <col min="28" max="28" width="2.21875" customWidth="1"/>
-    <col min="29" max="29" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="23.5546875" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="15.77734375" customWidth="1"/>
+    <col min="30" max="30" width="26.44140625" customWidth="1"/>
+    <col min="31" max="31" width="18.44140625" customWidth="1"/>
     <col min="32" max="32" width="2.21875" customWidth="1"/>
-    <col min="33" max="33" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="23.5546875" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="15.77734375" customWidth="1"/>
+    <col min="34" max="34" width="26.44140625" customWidth="1"/>
+    <col min="35" max="35" width="18.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:35" s="11" customFormat="1" x14ac:dyDescent="0.3">
@@ -3734,7 +3762,7 @@
       </c>
       <c r="B3" s="9" t="str">
         <f>[1]death_ben!B2</f>
-        <v>Death Benefit Table</v>
+        <v>Death Benefit Table 01</v>
       </c>
       <c r="C3" s="9" t="str">
         <f>[1]death_ben!C2</f>
@@ -3746,7 +3774,7 @@
       </c>
       <c r="F3" s="9" t="str">
         <f>[1]surr_ben!B2</f>
-        <v>Surrender Value Table</v>
+        <v>Surrender Value Table 01</v>
       </c>
       <c r="G3" s="9" t="str">
         <f>[1]surr_ben!C2</f>
@@ -3758,7 +3786,7 @@
       </c>
       <c r="J3" s="9" t="str">
         <f>[1]commission!B2</f>
-        <v>Commission Table</v>
+        <v>Commission Table 01</v>
       </c>
       <c r="K3" s="9" t="str">
         <f>[1]commission!C2</f>
@@ -3844,35 +3872,35 @@
       </c>
       <c r="B4" s="9" t="str">
         <f>[1]death_ben!B3</f>
-        <v>Death Benefit Table</v>
+        <v>Death Benefit Table 02 UDT</v>
       </c>
       <c r="C4" s="9" t="str">
         <f>[1]death_ben!C3</f>
         <v>User Defined Table</v>
       </c>
-      <c r="E4" s="9">
+      <c r="E4" s="9" t="str">
         <f>[1]surr_ben!A3</f>
-        <v>0</v>
-      </c>
-      <c r="F4" s="9">
+        <v>SV02UDT</v>
+      </c>
+      <c r="F4" s="9" t="str">
         <f>[1]surr_ben!B3</f>
-        <v>0</v>
-      </c>
-      <c r="G4" s="9">
+        <v>Surrender Value Table 02 UDT</v>
+      </c>
+      <c r="G4" s="9" t="str">
         <f>[1]surr_ben!C3</f>
-        <v>0</v>
-      </c>
-      <c r="I4" s="9">
+        <v>User Defined Table</v>
+      </c>
+      <c r="I4" s="9" t="str">
         <f>[1]commission!A3</f>
-        <v>0</v>
-      </c>
-      <c r="J4" s="9">
+        <v>COMM02UDT</v>
+      </c>
+      <c r="J4" s="9" t="str">
         <f>[1]commission!B3</f>
-        <v>0</v>
-      </c>
-      <c r="K4" s="9">
+        <v>Commission Table 02 UDT</v>
+      </c>
+      <c r="K4" s="9" t="str">
         <f>[1]commission!C3</f>
-        <v>0</v>
+        <v>User Defined Table</v>
       </c>
       <c r="M4" s="9">
         <f>[1]mortality!A3</f>
@@ -6197,14 +6225,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2C92756-0135-48D6-8016-1EE97220BD0B}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="48.5546875" customWidth="1"/>
+    <col min="2" max="2" width="51.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
use mp struct in prod feat func and add prem term
</commit_message>
<xml_diff>
--- a/Input/Settings.xlsx
+++ b/Input/Settings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Julia\TradLifeModel\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7B5399D-33F8-40E8-96DA-992653D53C41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49825E93-8BC0-4351-AB68-00700B9ADD64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="889" activeTab="2" xr2:uid="{ADF8BBD9-0F7A-45CB-8EA8-A3D46B124E82}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="827" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="836" uniqueCount="210">
   <si>
     <t>acq_exp_per_pol</t>
   </si>
@@ -630,15 +630,9 @@
     <t>mult by duration</t>
   </si>
   <si>
-    <t>comm_rate * premium</t>
-  </si>
-  <si>
     <t>Multiple of Sum Assured by Duration</t>
   </si>
   <si>
-    <t>Rate per 1000 Sum Assured by Entry Age</t>
-  </si>
-  <si>
     <t>Product Features in product_setup</t>
   </si>
   <si>
@@ -648,31 +642,40 @@
     <t>surr_benefit_rate * mp_sum_assured</t>
   </si>
   <si>
-    <t>comm_rate</t>
-  </si>
-  <si>
-    <t>Perc by Duration</t>
-  </si>
-  <si>
     <t>Perc by Duration and Policy Term</t>
   </si>
   <si>
-    <t>Perc by Duration and Policy Term and Premium Paying Term</t>
-  </si>
-  <si>
-    <t>premium_paying_term</t>
-  </si>
-  <si>
-    <t>Rate per 1000 Sum Assured by Entry Age and Policy Term</t>
-  </si>
-  <si>
-    <t>Rate per 1000 Sum Assured by Entry Age and Policy Term and Premium Paying Term</t>
-  </si>
-  <si>
-    <t>Rate per 1000 sum assured by Policy Year and Entry Age</t>
-  </si>
-  <si>
-    <t>Rate per 1000 sum assured by Policy Year and Entry Age and Premium Paying Term</t>
+    <t>comm_perc</t>
+  </si>
+  <si>
+    <t>comm_perc * premium</t>
+  </si>
+  <si>
+    <t>Perc by Duration and Policy Term and Premium Term</t>
+  </si>
+  <si>
+    <t>prem_term</t>
+  </si>
+  <si>
+    <t>COMM03</t>
+  </si>
+  <si>
+    <t>PREM03</t>
+  </si>
+  <si>
+    <t>Rate per 1000 sum assured by Policy Year and Issue Age</t>
+  </si>
+  <si>
+    <t>Rate per 1000 Sum Assured by Issue Age and Policy Term</t>
+  </si>
+  <si>
+    <t>Rate per 1000 Sum Assured by Issue Age and Policy Term and Premium Term</t>
+  </si>
+  <si>
+    <t>Rate per 1000 sum assured by Policy Year and Issue Age and Premium Term</t>
+  </si>
+  <si>
+    <t>SV03</t>
   </si>
 </sst>
 </file>
@@ -732,7 +735,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -742,12 +745,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -845,7 +842,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -912,9 +909,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -951,15 +946,18 @@
       <sheetName val="premium"/>
       <sheetName val="PREM01"/>
       <sheetName val="PREM02"/>
+      <sheetName val="PREM03"/>
       <sheetName val="death_ben"/>
       <sheetName val="DB01"/>
       <sheetName val="DB02UDT"/>
       <sheetName val="surr_ben"/>
       <sheetName val="SV01"/>
       <sheetName val="SV02UDT"/>
+      <sheetName val="SV03"/>
       <sheetName val="commission"/>
       <sheetName val="COMM01"/>
       <sheetName val="COMM02UDT"/>
+      <sheetName val="COMM03"/>
       <sheetName val="mortality"/>
       <sheetName val="MORT01"/>
       <sheetName val="lapse"/>
@@ -980,10 +978,10 @@
             <v>PREM01</v>
           </cell>
           <cell r="B2" t="str">
-            <v>Premium Rate Table by Entry Age</v>
+            <v>Premium Rate Table by Issue Age</v>
           </cell>
           <cell r="C2" t="str">
-            <v>Premium Rate Table</v>
+            <v>Rate per 1000 SA by Age/Pol Term</v>
           </cell>
         </row>
         <row r="3">
@@ -994,13 +992,25 @@
             <v>Premium Mult to MP Premium</v>
           </cell>
           <cell r="C3" t="str">
-            <v>Mult by Duration</v>
+            <v>Mult to MP Premium by Duration</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="A4" t="str">
+            <v>PREM03</v>
+          </cell>
+          <cell r="B4" t="str">
+            <v>Premium Rate Table by Issue Age/Pol Term/Prem Term</v>
+          </cell>
+          <cell r="C4" t="str">
+            <v>Rate per 1000 SA by Issue Age/Pol Term/Prem Term</v>
           </cell>
         </row>
       </sheetData>
       <sheetData sheetId="1" refreshError="1"/>
       <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3">
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4">
         <row r="2">
           <cell r="A2" t="str">
             <v>DB01</v>
@@ -1009,7 +1019,7 @@
             <v>Multiple to MP Sum Assured</v>
           </cell>
           <cell r="C2" t="str">
-            <v>Mult by Duration</v>
+            <v>Mult to MP SA by Duration</v>
           </cell>
         </row>
         <row r="3">
@@ -1017,25 +1027,25 @@
             <v>DB02UDT</v>
           </cell>
           <cell r="B3" t="str">
-            <v>Death Benefit Table 02 UDT</v>
+            <v>Death Benefit UDT</v>
           </cell>
           <cell r="C3" t="str">
             <v>User Defined Table</v>
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="4" refreshError="1"/>
       <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6">
+      <sheetData sheetId="6" refreshError="1"/>
+      <sheetData sheetId="7">
         <row r="2">
           <cell r="A2" t="str">
             <v>SV01</v>
           </cell>
           <cell r="B2" t="str">
-            <v>Surrender Value Table 01</v>
+            <v>Surrender Value Rate Table by Policy Year/Issue Age</v>
           </cell>
           <cell r="C2" t="str">
-            <v>Year/Age</v>
+            <v>Rate per 1000 SA by Year/Age</v>
           </cell>
         </row>
         <row r="3">
@@ -1043,25 +1053,37 @@
             <v>SV02UDT</v>
           </cell>
           <cell r="B3" t="str">
-            <v>Surrender Value Table 02 UDT</v>
+            <v>Surrender Value UDT</v>
           </cell>
           <cell r="C3" t="str">
             <v>User Defined Table</v>
           </cell>
         </row>
+        <row r="4">
+          <cell r="A4" t="str">
+            <v>SV03</v>
+          </cell>
+          <cell r="B4" t="str">
+            <v>Surrender Value Rate Table by Policy Year/Issue Age/Premium Term</v>
+          </cell>
+          <cell r="C4" t="str">
+            <v>Rate per 1000 SA by Pol Year/Issue Age/Prem Term</v>
+          </cell>
+        </row>
       </sheetData>
-      <sheetData sheetId="7" refreshError="1"/>
       <sheetData sheetId="8" refreshError="1"/>
-      <sheetData sheetId="9">
+      <sheetData sheetId="9" refreshError="1"/>
+      <sheetData sheetId="10" refreshError="1"/>
+      <sheetData sheetId="11">
         <row r="2">
           <cell r="A2" t="str">
             <v>COMM01</v>
           </cell>
           <cell r="B2" t="str">
-            <v>Commission Rates</v>
+            <v>Commission Percentage by Policy Year/Policy Term</v>
           </cell>
           <cell r="C2" t="str">
-            <v>Policy Year</v>
+            <v>Perc by Year/Pol Term</v>
           </cell>
         </row>
         <row r="3">
@@ -1069,16 +1091,28 @@
             <v>COMM02UDT</v>
           </cell>
           <cell r="B3" t="str">
-            <v>Commission Table 02 UDT</v>
+            <v>Commission Percentage UDT</v>
           </cell>
           <cell r="C3" t="str">
             <v>User Defined Table</v>
           </cell>
         </row>
+        <row r="4">
+          <cell r="A4" t="str">
+            <v>COMM03</v>
+          </cell>
+          <cell r="B4" t="str">
+            <v>Commission Percentage by Policy Year/Policy Term/Prem Paying Term</v>
+          </cell>
+          <cell r="C4" t="str">
+            <v>Perc by Pol Year/Pol Term/Prem Term</v>
+          </cell>
+        </row>
       </sheetData>
-      <sheetData sheetId="10" refreshError="1"/>
-      <sheetData sheetId="11" refreshError="1"/>
-      <sheetData sheetId="12">
+      <sheetData sheetId="12" refreshError="1"/>
+      <sheetData sheetId="13" refreshError="1"/>
+      <sheetData sheetId="14" refreshError="1"/>
+      <sheetData sheetId="15">
         <row r="2">
           <cell r="A2" t="str">
             <v>MORT01</v>
@@ -1091,8 +1125,8 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="13" refreshError="1"/>
-      <sheetData sheetId="14">
+      <sheetData sheetId="16" refreshError="1"/>
+      <sheetData sheetId="17">
         <row r="2">
           <cell r="A2" t="str">
             <v>LAPSE01</v>
@@ -1105,8 +1139,8 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="15" refreshError="1"/>
-      <sheetData sheetId="16">
+      <sheetData sheetId="18" refreshError="1"/>
+      <sheetData sheetId="19">
         <row r="2">
           <cell r="A2" t="str">
             <v>EXP01</v>
@@ -1119,8 +1153,8 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="17" refreshError="1"/>
-      <sheetData sheetId="18">
+      <sheetData sheetId="20" refreshError="1"/>
+      <sheetData sheetId="21">
         <row r="2">
           <cell r="A2" t="str">
             <v>DISCRT01</v>
@@ -1133,8 +1167,8 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="19" refreshError="1"/>
-      <sheetData sheetId="20">
+      <sheetData sheetId="22" refreshError="1"/>
+      <sheetData sheetId="23">
         <row r="2">
           <cell r="A2" t="str">
             <v>PREMTAX01</v>
@@ -1147,8 +1181,8 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="21" refreshError="1"/>
-      <sheetData sheetId="22">
+      <sheetData sheetId="24" refreshError="1"/>
+      <sheetData sheetId="25">
         <row r="2">
           <cell r="A2" t="str">
             <v>TAX01</v>
@@ -1161,7 +1195,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="23" refreshError="1"/>
+      <sheetData sheetId="26" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1467,7 +1501,7 @@
   <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1528,7 +1562,9 @@
       <c r="A7" t="s">
         <v>148</v>
       </c>
-      <c r="B7" s="12"/>
+      <c r="B7" s="12" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
@@ -2322,7 +2358,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C11" sqref="C11"/>
+      <selection pane="bottomRight" activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2386,7 +2422,7 @@
         <v>136</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>176</v>
+        <v>204</v>
       </c>
       <c r="E3" s="13" t="s">
         <v>176</v>
@@ -2409,11 +2445,11 @@
       </c>
       <c r="D4" s="34" t="str">
         <f>_xlfn.XLOOKUP(D3,table_listings!$B$2:$B$201,table_listings!$D$2:$D$201,,0)</f>
-        <v>Premium Rate Table</v>
+        <v>Rate per 1000 SA by Issue Age/Pol Term/Prem Term</v>
       </c>
       <c r="E4" s="34" t="str">
         <f>_xlfn.XLOOKUP(E3,table_listings!$B$2:$B$201,table_listings!$D$2:$D$201,,0)</f>
-        <v>Premium Rate Table</v>
+        <v>Rate per 1000 SA by Age/Pol Term</v>
       </c>
       <c r="F4" s="13"/>
       <c r="G4" s="13"/>
@@ -2495,7 +2531,7 @@
       </c>
       <c r="D8" s="34" t="str">
         <f>_xlfn.XLOOKUP(D7,table_listings!$B$2:$B$201,table_listings!$D$2:$D$201,,0)</f>
-        <v>Mult by Duration</v>
+        <v>Mult to MP SA by Duration</v>
       </c>
       <c r="E8" s="34" t="str">
         <f>_xlfn.XLOOKUP(E7,table_listings!$B$2:$B$201,table_listings!$D$2:$D$201,,0)</f>
@@ -2560,7 +2596,7 @@
         <v>136</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>130</v>
+        <v>209</v>
       </c>
       <c r="E11" s="12" t="s">
         <v>130</v>
@@ -2583,11 +2619,11 @@
       </c>
       <c r="D12" s="34" t="str">
         <f>_xlfn.XLOOKUP(D11,table_listings!$B$2:$B$201,table_listings!$D$2:$D$201,,0)</f>
-        <v>Year/Age</v>
+        <v>Rate per 1000 SA by Pol Year/Issue Age/Prem Term</v>
       </c>
       <c r="E12" s="34" t="str">
         <f>_xlfn.XLOOKUP(E11,table_listings!$B$2:$B$201,table_listings!$D$2:$D$201,,0)</f>
-        <v>Year/Age</v>
+        <v>Rate per 1000 SA by Year/Age</v>
       </c>
       <c r="F12" s="13"/>
       <c r="G12" s="13"/>
@@ -2646,7 +2682,7 @@
         <v>136</v>
       </c>
       <c r="D15" s="13" t="s">
-        <v>124</v>
+        <v>203</v>
       </c>
       <c r="E15" s="13" t="s">
         <v>124</v>
@@ -2669,11 +2705,11 @@
       </c>
       <c r="D16" s="34" t="str">
         <f>_xlfn.XLOOKUP(D15,table_listings!$B$2:$B$201,table_listings!$D$2:$D$201,,0)</f>
-        <v>Policy Year</v>
+        <v>Perc by Pol Year/Pol Term/Prem Term</v>
       </c>
       <c r="E16" s="34" t="str">
         <f>_xlfn.XLOOKUP(E15,table_listings!$B$2:$B$201,table_listings!$D$2:$D$201,,0)</f>
-        <v>Policy Year</v>
+        <v>Perc by Year/Pol Term</v>
       </c>
       <c r="F16" s="13"/>
       <c r="G16" s="13"/>
@@ -4272,9 +4308,9 @@
           </x14:formula1>
           <xm:sqref>D7:E7</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{47ABC217-4045-44B4-9DB7-9C5FFDF571D1}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{3276693A-87D7-4A8D-9CCA-C2D88FEF16C3}">
           <x14:formula1>
-            <xm:f>table_listings!B63:B82</xm:f>
+            <xm:f>table_listings!$B$62:$B$81</xm:f>
           </x14:formula1>
           <xm:sqref>D15:E15</xm:sqref>
         </x14:dataValidation>
@@ -4326,11 +4362,11 @@
       </c>
       <c r="C2" s="9" t="str">
         <f>[1]premium!B2</f>
-        <v>Premium Rate Table by Entry Age</v>
+        <v>Premium Rate Table by Issue Age</v>
       </c>
       <c r="D2" s="9" t="str">
         <f>[1]premium!C2</f>
-        <v>Premium Rate Table</v>
+        <v>Rate per 1000 SA by Age/Pol Term</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -4347,24 +4383,24 @@
       </c>
       <c r="D3" s="9" t="str">
         <f>[1]premium!C3</f>
-        <v>Mult by Duration</v>
+        <v>Mult to MP Premium by Duration</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
         <v>174</v>
       </c>
-      <c r="B4" s="9">
+      <c r="B4" s="9" t="str">
         <f>[1]premium!A4</f>
-        <v>0</v>
-      </c>
-      <c r="C4" s="9">
+        <v>PREM03</v>
+      </c>
+      <c r="C4" s="9" t="str">
         <f>[1]premium!B4</f>
-        <v>0</v>
-      </c>
-      <c r="D4" s="9">
+        <v>Premium Rate Table by Issue Age/Pol Term/Prem Term</v>
+      </c>
+      <c r="D4" s="9" t="str">
         <f>[1]premium!C4</f>
-        <v>0</v>
+        <v>Rate per 1000 SA by Issue Age/Pol Term/Prem Term</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -4670,7 +4706,7 @@
       </c>
       <c r="D22" s="9" t="str">
         <f>[1]death_ben!C2</f>
-        <v>Mult by Duration</v>
+        <v>Mult to MP SA by Duration</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
@@ -4683,7 +4719,7 @@
       </c>
       <c r="C23" s="9" t="str">
         <f>[1]death_ben!B3</f>
-        <v>Death Benefit Table 02 UDT</v>
+        <v>Death Benefit UDT</v>
       </c>
       <c r="D23" s="9" t="str">
         <f>[1]death_ben!C3</f>
@@ -5006,11 +5042,11 @@
       </c>
       <c r="C42" s="9" t="str">
         <f>[1]surr_ben!B2</f>
-        <v>Surrender Value Table 01</v>
+        <v>Surrender Value Rate Table by Policy Year/Issue Age</v>
       </c>
       <c r="D42" s="9" t="str">
         <f>[1]surr_ben!C2</f>
-        <v>Year/Age</v>
+        <v>Rate per 1000 SA by Year/Age</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
@@ -5023,7 +5059,7 @@
       </c>
       <c r="C43" s="9" t="str">
         <f>[1]surr_ben!B3</f>
-        <v>Surrender Value Table 02 UDT</v>
+        <v>Surrender Value UDT</v>
       </c>
       <c r="D43" s="9" t="str">
         <f>[1]surr_ben!C3</f>
@@ -5034,17 +5070,17 @@
       <c r="A44" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="B44" s="9">
+      <c r="B44" s="9" t="str">
         <f>[1]surr_ben!A4</f>
-        <v>0</v>
-      </c>
-      <c r="C44" s="9">
+        <v>SV03</v>
+      </c>
+      <c r="C44" s="9" t="str">
         <f>[1]surr_ben!B4</f>
-        <v>0</v>
-      </c>
-      <c r="D44" s="9">
+        <v>Surrender Value Rate Table by Policy Year/Issue Age/Premium Term</v>
+      </c>
+      <c r="D44" s="9" t="str">
         <f>[1]surr_ben!C4</f>
-        <v>0</v>
+        <v>Rate per 1000 SA by Pol Year/Issue Age/Prem Term</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
@@ -5346,11 +5382,11 @@
       </c>
       <c r="C62" s="9" t="str">
         <f>[1]commission!B2</f>
-        <v>Commission Rates</v>
+        <v>Commission Percentage by Policy Year/Policy Term</v>
       </c>
       <c r="D62" s="9" t="str">
         <f>[1]commission!C2</f>
-        <v>Policy Year</v>
+        <v>Perc by Year/Pol Term</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
@@ -5363,7 +5399,7 @@
       </c>
       <c r="C63" s="9" t="str">
         <f>[1]commission!B3</f>
-        <v>Commission Table 02 UDT</v>
+        <v>Commission Percentage UDT</v>
       </c>
       <c r="D63" s="9" t="str">
         <f>[1]commission!C3</f>
@@ -5374,17 +5410,17 @@
       <c r="A64" s="9" t="s">
         <v>144</v>
       </c>
-      <c r="B64" s="9">
+      <c r="B64" s="9" t="str">
         <f>[1]commission!A4</f>
-        <v>0</v>
-      </c>
-      <c r="C64" s="9">
+        <v>COMM03</v>
+      </c>
+      <c r="C64" s="9" t="str">
         <f>[1]commission!B4</f>
-        <v>0</v>
-      </c>
-      <c r="D64" s="9">
+        <v>Commission Percentage by Policy Year/Policy Term/Prem Paying Term</v>
+      </c>
+      <c r="D64" s="9" t="str">
         <f>[1]commission!C4</f>
-        <v>0</v>
+        <v>Perc by Pol Year/Pol Term/Prem Term</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
@@ -8500,7 +8536,7 @@
   <dimension ref="B1:E23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8512,16 +8548,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B1" s="37" t="s">
-        <v>197</v>
-      </c>
-      <c r="C1" s="37" t="s">
+      <c r="B1" s="36" t="s">
+        <v>195</v>
+      </c>
+      <c r="C1" s="36" t="s">
         <v>188</v>
       </c>
-      <c r="D1" s="37" t="s">
+      <c r="D1" s="36" t="s">
         <v>190</v>
       </c>
-      <c r="E1" s="37" t="s">
+      <c r="E1" s="36" t="s">
         <v>189</v>
       </c>
     </row>
@@ -8530,48 +8566,69 @@
         <v>174</v>
       </c>
       <c r="C2" t="s">
+        <v>206</v>
+      </c>
+      <c r="D2" t="s">
         <v>196</v>
-      </c>
-      <c r="D2" t="s">
-        <v>198</v>
       </c>
       <c r="E2" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C3" s="36" t="s">
-        <v>205</v>
+      <c r="B3" t="s">
+        <v>174</v>
+      </c>
+      <c r="C3" t="s">
+        <v>207</v>
+      </c>
+      <c r="D3" t="s">
+        <v>196</v>
+      </c>
+      <c r="E3" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C4" s="36" t="s">
-        <v>206</v>
+      <c r="B4" t="s">
+        <v>174</v>
+      </c>
+      <c r="C4" t="s">
+        <v>193</v>
+      </c>
+      <c r="D4" t="s">
+        <v>191</v>
+      </c>
+      <c r="E4" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>177</v>
+      </c>
       <c r="C5" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="D5" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="E5" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C6" t="s">
-        <v>195</v>
+        <v>205</v>
       </c>
       <c r="D6" t="s">
-        <v>192</v>
+        <v>197</v>
       </c>
       <c r="E6" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.3">
@@ -8579,18 +8636,27 @@
         <v>178</v>
       </c>
       <c r="C7" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="D7" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E7" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C8" s="36" t="s">
-        <v>208</v>
+      <c r="B8" t="s">
+        <v>144</v>
+      </c>
+      <c r="C8" t="s">
+        <v>198</v>
+      </c>
+      <c r="D8" t="s">
+        <v>199</v>
+      </c>
+      <c r="E8" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.3">
@@ -8600,27 +8666,15 @@
       <c r="C9" t="s">
         <v>201</v>
       </c>
-      <c r="D9" s="38" t="s">
+      <c r="D9" t="s">
+        <v>199</v>
+      </c>
+      <c r="E9" t="s">
         <v>200</v>
       </c>
-      <c r="E9" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C10" s="36" t="s">
-        <v>202</v>
-      </c>
-      <c r="D10" s="38"/>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C11" s="36" t="s">
-        <v>203</v>
-      </c>
-      <c r="D11" s="38"/>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B13" s="37" t="s">
+      <c r="B13" s="36" t="s">
         <v>179</v>
       </c>
     </row>
@@ -8656,22 +8710,22 @@
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
-        <v>175</v>
+        <v>202</v>
       </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B23" t="s">
         <v>186</v>
-      </c>
-    </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B23" s="36" t="s">
-        <v>204</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add mort tables and use MortalityTables package (WIP)
</commit_message>
<xml_diff>
--- a/Input/Settings.xlsx
+++ b/Input/Settings.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Julia\TradLifeModel\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49825E93-8BC0-4351-AB68-00700B9ADD64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D5C1085-8478-458B-83E8-39D8D1C0D7D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="889" activeTab="2" xr2:uid="{ADF8BBD9-0F7A-45CB-8EA8-A3D46B124E82}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="836" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="854" uniqueCount="221">
   <si>
     <t>acq_exp_per_pol</t>
   </si>
@@ -676,6 +676,39 @@
   </si>
   <si>
     <t>SV03</t>
+  </si>
+  <si>
+    <t>Assumptions in product_setup</t>
+  </si>
+  <si>
+    <t>moratlity</t>
+  </si>
+  <si>
+    <t>smoking_status</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Base</t>
+  </si>
+  <si>
+    <t>Attained Age Aggregate Rate</t>
+  </si>
+  <si>
+    <t>Attained Age Sex Distinct</t>
+  </si>
+  <si>
+    <t>Attained Age Sex Smoker Distinct</t>
+  </si>
+  <si>
+    <t>Rate by Policy Year and Policy Term</t>
+  </si>
+  <si>
+    <t>Rate by Policy Year and Policy Term and Premium Term</t>
+  </si>
+  <si>
+    <t>MORT04</t>
   </si>
 </sst>
 </file>
@@ -960,6 +993,10 @@
       <sheetName val="COMM03"/>
       <sheetName val="mortality"/>
       <sheetName val="MORT01"/>
+      <sheetName val="MORT02"/>
+      <sheetName val="MORT03"/>
+      <sheetName val="MORT04"/>
+      <sheetName val="MORT05"/>
       <sheetName val="lapse"/>
       <sheetName val="LAPSE01"/>
       <sheetName val="expense"/>
@@ -1007,9 +1044,9 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
       <sheetData sheetId="4">
         <row r="2">
           <cell r="A2" t="str">
@@ -1034,8 +1071,8 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
       <sheetData sheetId="7">
         <row r="2">
           <cell r="A2" t="str">
@@ -1071,9 +1108,9 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="8" refreshError="1"/>
-      <sheetData sheetId="9" refreshError="1"/>
-      <sheetData sheetId="10" refreshError="1"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
       <sheetData sheetId="11">
         <row r="2">
           <cell r="A2" t="str">
@@ -1109,24 +1146,78 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="12" refreshError="1"/>
-      <sheetData sheetId="13" refreshError="1"/>
-      <sheetData sheetId="14" refreshError="1"/>
+      <sheetData sheetId="12"/>
+      <sheetData sheetId="13"/>
+      <sheetData sheetId="14"/>
       <sheetData sheetId="15">
         <row r="2">
           <cell r="A2" t="str">
             <v>MORT01</v>
           </cell>
           <cell r="B2" t="str">
-            <v>Mortality Table Sex Distinct</v>
+            <v>Attained Age Aggregate Mortality Table</v>
           </cell>
           <cell r="C2" t="str">
-            <v>Sex Distinct</v>
+            <v>Attained Age Aggregate</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="A3" t="str">
+            <v>MORT02</v>
+          </cell>
+          <cell r="B3" t="str">
+            <v>Attained Age Sex Distinct Mortality Table</v>
+          </cell>
+          <cell r="C3" t="str">
+            <v>Attained Age Sex Distinct</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="A4" t="str">
+            <v>MORT03</v>
+          </cell>
+          <cell r="B4" t="str">
+            <v>Attained Age Sex Smoker Distinct Mortality Table</v>
+          </cell>
+          <cell r="C4" t="str">
+            <v>Attained Age Sex Smoker Distinct</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="A5" t="str">
+            <v>MORT04</v>
+          </cell>
+          <cell r="B5" t="str">
+            <v>Attained Age Select and Ultimate Table</v>
+          </cell>
+          <cell r="C5" t="str">
+            <v>Select and Ultimate Aggregate</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="A6" t="str">
+            <v>MORT05</v>
+          </cell>
+          <cell r="B6" t="str">
+            <v>Reference Table for CSO Composite Select and Ultimate Table</v>
+          </cell>
+          <cell r="C6" t="str">
+            <v>Reference Table for SOA Select and Ultimate Table</v>
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="16" refreshError="1"/>
-      <sheetData sheetId="17">
+      <sheetData sheetId="16"/>
+      <sheetData sheetId="17"/>
+      <sheetData sheetId="18"/>
+      <sheetData sheetId="19">
+        <row r="1">
+          <cell r="B1">
+            <v>1</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="20"/>
+      <sheetData sheetId="21">
         <row r="2">
           <cell r="A2" t="str">
             <v>LAPSE01</v>
@@ -1139,8 +1230,8 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="18" refreshError="1"/>
-      <sheetData sheetId="19">
+      <sheetData sheetId="22"/>
+      <sheetData sheetId="23">
         <row r="2">
           <cell r="A2" t="str">
             <v>EXP01</v>
@@ -1153,8 +1244,8 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="20" refreshError="1"/>
-      <sheetData sheetId="21">
+      <sheetData sheetId="24"/>
+      <sheetData sheetId="25">
         <row r="2">
           <cell r="A2" t="str">
             <v>DISCRT01</v>
@@ -1167,8 +1258,8 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="22" refreshError="1"/>
-      <sheetData sheetId="23">
+      <sheetData sheetId="26"/>
+      <sheetData sheetId="27">
         <row r="2">
           <cell r="A2" t="str">
             <v>PREMTAX01</v>
@@ -1181,8 +1272,8 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="24" refreshError="1"/>
-      <sheetData sheetId="25">
+      <sheetData sheetId="28"/>
+      <sheetData sheetId="29">
         <row r="2">
           <cell r="A2" t="str">
             <v>TAX01</v>
@@ -1195,7 +1286,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="26" refreshError="1"/>
+      <sheetData sheetId="30"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1501,7 +1592,7 @@
   <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1523,7 +1614,7 @@
         <v>168</v>
       </c>
       <c r="B2" s="33">
-        <v>45291</v>
+        <v>45230</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -1547,7 +1638,7 @@
         <v>170</v>
       </c>
       <c r="B5" s="12">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -1562,9 +1653,7 @@
       <c r="A7" t="s">
         <v>148</v>
       </c>
-      <c r="B7" s="12" t="s">
-        <v>116</v>
-      </c>
+      <c r="B7" s="12"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
@@ -1688,7 +1777,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomRight" activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1794,18 +1883,20 @@
         <v>81</v>
       </c>
       <c r="B3" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="C3" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="D3" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="E3" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="F3" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="F3" s="7"/>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
       <c r="I3" s="7"/>
@@ -1827,10 +1918,10 @@
         <v>94</v>
       </c>
       <c r="B4" s="4">
+        <v>1</v>
+      </c>
+      <c r="C4" s="4">
         <v>1.1000000000000001</v>
-      </c>
-      <c r="C4" s="4">
-        <v>1</v>
       </c>
       <c r="D4" s="4">
         <v>1</v>
@@ -1838,7 +1929,9 @@
       <c r="E4" s="4">
         <v>1</v>
       </c>
-      <c r="F4" s="4"/>
+      <c r="F4" s="4">
+        <v>1</v>
+      </c>
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
@@ -1863,15 +1956,17 @@
         <v>1</v>
       </c>
       <c r="C5" s="4">
+        <v>1</v>
+      </c>
+      <c r="D5" s="4">
         <v>0.9</v>
-      </c>
-      <c r="D5" s="4">
-        <v>1</v>
       </c>
       <c r="E5" s="4">
         <v>1</v>
       </c>
-      <c r="F5" s="4"/>
+      <c r="F5" s="4">
+        <v>1</v>
+      </c>
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
@@ -1899,12 +1994,14 @@
         <v>1</v>
       </c>
       <c r="D6" s="4">
+        <v>1</v>
+      </c>
+      <c r="E6" s="4">
         <v>1.1000000000000001</v>
       </c>
-      <c r="E6" s="4">
+      <c r="F6" s="4">
         <v>1</v>
       </c>
-      <c r="F6" s="4"/>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
@@ -1935,9 +2032,11 @@
         <v>0</v>
       </c>
       <c r="E7" s="8">
+        <v>0</v>
+      </c>
+      <c r="F7" s="8">
         <v>-0.01</v>
       </c>
-      <c r="F7" s="4"/>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
@@ -1968,9 +2067,11 @@
         <v>0</v>
       </c>
       <c r="E8" s="8">
+        <v>0</v>
+      </c>
+      <c r="F8" s="8">
         <v>-0.01</v>
       </c>
-      <c r="F8" s="4"/>
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
@@ -1995,17 +2096,19 @@
         <v>1</v>
       </c>
       <c r="C9" s="4">
-        <f t="shared" ref="C9:D11" si="0">C4</f>
         <v>1</v>
       </c>
       <c r="D9" s="4">
+        <f t="shared" ref="D9:E9" si="0">D4</f>
+        <v>1</v>
+      </c>
+      <c r="E9" s="4">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="E9" s="4">
+      <c r="F9" s="4">
         <v>1</v>
       </c>
-      <c r="F9" s="4"/>
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
@@ -2027,21 +2130,24 @@
         <v>100</v>
       </c>
       <c r="B10" s="4">
-        <f>B5</f>
+        <f t="shared" ref="B10:C12" si="1">B5</f>
         <v>1</v>
       </c>
       <c r="C10" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D10" s="4">
+        <f t="shared" ref="D10:E10" si="2">D5</f>
         <v>0.9</v>
       </c>
-      <c r="D10" s="4">
-        <f t="shared" si="0"/>
+      <c r="E10" s="4">
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="E10" s="4">
+      <c r="F10" s="4">
         <v>1</v>
       </c>
-      <c r="F10" s="4"/>
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
@@ -2063,21 +2169,24 @@
         <v>101</v>
       </c>
       <c r="B11" s="4">
-        <f>B6</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="C11" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="D11" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="D11:E11" si="3">D6</f>
+        <v>1</v>
+      </c>
+      <c r="E11" s="4">
+        <f t="shared" si="3"/>
         <v>1.1000000000000001</v>
       </c>
-      <c r="E11" s="4">
+      <c r="F11" s="4">
         <v>1</v>
       </c>
-      <c r="F11" s="4"/>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
@@ -2099,11 +2208,11 @@
         <v>102</v>
       </c>
       <c r="B12" s="8">
-        <f>B7</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="C12" s="8">
-        <f>C7</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D12" s="8">
@@ -2111,9 +2220,12 @@
         <v>0</v>
       </c>
       <c r="E12" s="8">
+        <f>E7</f>
+        <v>0</v>
+      </c>
+      <c r="F12" s="8">
         <v>-0.01</v>
       </c>
-      <c r="F12" s="4"/>
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
@@ -2135,21 +2247,24 @@
         <v>103</v>
       </c>
       <c r="B13" s="4">
-        <f t="shared" ref="B13:D15" si="1">B9</f>
+        <f t="shared" ref="B13:B15" si="4">B9</f>
         <v>1</v>
       </c>
       <c r="C13" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="C13:E13" si="5">C9</f>
         <v>1</v>
       </c>
       <c r="D13" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="E13" s="4">
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
-      <c r="F13" s="4"/>
+      <c r="F13" s="4">
+        <v>1</v>
+      </c>
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
@@ -2171,21 +2286,24 @@
         <v>104</v>
       </c>
       <c r="B14" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="C14" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="C14:E14" si="6">C10</f>
+        <v>1</v>
+      </c>
+      <c r="D14" s="4">
+        <f t="shared" si="6"/>
         <v>0.9</v>
       </c>
-      <c r="D14" s="4">
-        <f t="shared" si="1"/>
+      <c r="E14" s="4">
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
-      <c r="E14" s="4">
+      <c r="F14" s="4">
         <v>1</v>
       </c>
-      <c r="F14" s="4"/>
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
@@ -2207,21 +2325,24 @@
         <v>105</v>
       </c>
       <c r="B15" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="C15" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="C15:E15" si="7">C11</f>
         <v>1</v>
       </c>
       <c r="D15" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E15" s="4">
+        <f t="shared" si="7"/>
         <v>1.1000000000000001</v>
       </c>
-      <c r="E15" s="4">
+      <c r="F15" s="4">
         <v>1</v>
       </c>
-      <c r="F15" s="4"/>
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
@@ -2255,9 +2376,12 @@
         <v>0</v>
       </c>
       <c r="E16" s="8">
+        <f>E12</f>
+        <v>0</v>
+      </c>
+      <c r="F16" s="8">
         <v>-0.01</v>
       </c>
-      <c r="F16" s="4"/>
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
@@ -2352,13 +2476,14 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1E729B3-29BA-40F1-80D4-2208DEC4BA85}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:J84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E4" sqref="E4"/>
+      <selection pane="bottomRight" activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2389,7 +2514,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>141</v>
       </c>
@@ -2411,7 +2536,7 @@
       <c r="I2" s="13"/>
       <c r="J2" s="13"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>141</v>
       </c>
@@ -2433,7 +2558,7 @@
       <c r="I3" s="13"/>
       <c r="J3" s="13"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>141</v>
       </c>
@@ -2457,7 +2582,7 @@
       <c r="I4" s="13"/>
       <c r="J4" s="13"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>141</v>
       </c>
@@ -2475,7 +2600,7 @@
       <c r="I5" s="12"/>
       <c r="J5" s="12"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6" s="15" t="s">
         <v>141</v>
       </c>
@@ -2497,7 +2622,7 @@
       <c r="I6" s="13"/>
       <c r="J6" s="13"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7" s="15" t="s">
         <v>141</v>
       </c>
@@ -2519,7 +2644,7 @@
       <c r="I7" s="13"/>
       <c r="J7" s="13"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8" s="15" t="s">
         <v>141</v>
       </c>
@@ -2543,7 +2668,7 @@
       <c r="I8" s="13"/>
       <c r="J8" s="13"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" s="15" t="s">
         <v>141</v>
       </c>
@@ -2563,7 +2688,7 @@
       <c r="I9" s="12"/>
       <c r="J9" s="12"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" s="24" t="s">
         <v>141</v>
       </c>
@@ -2585,7 +2710,7 @@
       <c r="I10" s="13"/>
       <c r="J10" s="13"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" s="24" t="s">
         <v>141</v>
       </c>
@@ -2607,7 +2732,7 @@
       <c r="I11" s="12"/>
       <c r="J11" s="12"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" s="24" t="s">
         <v>141</v>
       </c>
@@ -2631,7 +2756,7 @@
       <c r="I12" s="13"/>
       <c r="J12" s="13"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13" s="24" t="s">
         <v>141</v>
       </c>
@@ -2649,7 +2774,7 @@
       <c r="I13" s="12"/>
       <c r="J13" s="12"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14" s="15" t="s">
         <v>141</v>
       </c>
@@ -2671,7 +2796,7 @@
       <c r="I14" s="13"/>
       <c r="J14" s="13"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15" s="15" t="s">
         <v>141</v>
       </c>
@@ -2693,7 +2818,7 @@
       <c r="I15" s="13"/>
       <c r="J15" s="13"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16" s="15" t="s">
         <v>141</v>
       </c>
@@ -2717,7 +2842,7 @@
       <c r="I16" s="13"/>
       <c r="J16" s="13"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17" s="15" t="s">
         <v>141</v>
       </c>
@@ -2746,7 +2871,7 @@
         <v>137</v>
       </c>
       <c r="D18" s="13">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="E18" s="13">
         <v>0.8</v>
@@ -2768,7 +2893,7 @@
         <v>136</v>
       </c>
       <c r="D19" s="12" t="s">
-        <v>109</v>
+        <v>220</v>
       </c>
       <c r="E19" s="12" t="s">
         <v>109</v>
@@ -2791,11 +2916,11 @@
       </c>
       <c r="D20" s="34" t="str">
         <f>_xlfn.XLOOKUP(D19,table_listings!$B$2:$B$201,table_listings!$D$2:$D$201,,0)</f>
-        <v>Sex Distinct</v>
+        <v>Select and Ultimate Aggregate</v>
       </c>
       <c r="E20" s="34" t="str">
         <f>_xlfn.XLOOKUP(E19,table_listings!$B$2:$B$201,table_listings!$D$2:$D$201,,0)</f>
-        <v>Sex Distinct</v>
+        <v>Attained Age Aggregate</v>
       </c>
       <c r="F20" s="13"/>
       <c r="G20" s="13"/>
@@ -2803,7 +2928,7 @@
       <c r="I20" s="13"/>
       <c r="J20" s="13"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21" s="15" t="s">
         <v>133</v>
       </c>
@@ -2825,7 +2950,7 @@
       <c r="I21" s="13"/>
       <c r="J21" s="13"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22" s="15" t="s">
         <v>133</v>
       </c>
@@ -2847,7 +2972,7 @@
       <c r="I22" s="12"/>
       <c r="J22" s="12"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23" s="15" t="s">
         <v>133</v>
       </c>
@@ -2871,7 +2996,7 @@
       <c r="I23" s="13"/>
       <c r="J23" s="13"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24" s="24" t="s">
         <v>133</v>
       </c>
@@ -2893,7 +3018,7 @@
       <c r="I24" s="13"/>
       <c r="J24" s="13"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25" s="24" t="s">
         <v>133</v>
       </c>
@@ -2915,7 +3040,7 @@
       <c r="I25" s="12"/>
       <c r="J25" s="12"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26" s="24" t="s">
         <v>133</v>
       </c>
@@ -2939,7 +3064,7 @@
       <c r="I26" s="13"/>
       <c r="J26" s="13"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27" s="15" t="s">
         <v>133</v>
       </c>
@@ -2961,7 +3086,7 @@
       <c r="I27" s="13"/>
       <c r="J27" s="13"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28" s="15" t="s">
         <v>133</v>
       </c>
@@ -2983,7 +3108,7 @@
       <c r="I28" s="12"/>
       <c r="J28" s="12"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29" s="15" t="s">
         <v>133</v>
       </c>
@@ -3007,7 +3132,7 @@
       <c r="I29" s="13"/>
       <c r="J29" s="13"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30" s="15" t="s">
         <v>133</v>
       </c>
@@ -3029,7 +3154,7 @@
       <c r="I30" s="12"/>
       <c r="J30" s="12"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31" s="24" t="s">
         <v>133</v>
       </c>
@@ -3051,7 +3176,7 @@
       <c r="I31" s="13"/>
       <c r="J31" s="13"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A32" s="24" t="s">
         <v>133</v>
       </c>
@@ -3073,7 +3198,7 @@
       <c r="I32" s="12"/>
       <c r="J32" s="12"/>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33" s="24" t="s">
         <v>133</v>
       </c>
@@ -3097,7 +3222,7 @@
       <c r="I33" s="13"/>
       <c r="J33" s="13"/>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34" s="24" t="s">
         <v>133</v>
       </c>
@@ -3119,7 +3244,7 @@
       <c r="I34" s="12"/>
       <c r="J34" s="12"/>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A35" s="15" t="s">
         <v>133</v>
       </c>
@@ -3141,7 +3266,7 @@
       <c r="I35" s="13"/>
       <c r="J35" s="13"/>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A36" s="15" t="s">
         <v>133</v>
       </c>
@@ -3163,7 +3288,7 @@
       <c r="I36" s="12"/>
       <c r="J36" s="12"/>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A37" s="15" t="s">
         <v>133</v>
       </c>
@@ -3187,7 +3312,7 @@
       <c r="I37" s="13"/>
       <c r="J37" s="13"/>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A38" s="15" t="s">
         <v>133</v>
       </c>
@@ -3209,7 +3334,7 @@
       <c r="I38" s="12"/>
       <c r="J38" s="12"/>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A39" s="24" t="s">
         <v>133</v>
       </c>
@@ -3231,7 +3356,7 @@
       <c r="I39" s="13"/>
       <c r="J39" s="13"/>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A40" s="24" t="s">
         <v>133</v>
       </c>
@@ -3253,7 +3378,7 @@
       <c r="I40" s="13"/>
       <c r="J40" s="13"/>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A41" s="24" t="s">
         <v>133</v>
       </c>
@@ -3277,7 +3402,7 @@
       <c r="I41" s="13"/>
       <c r="J41" s="13"/>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A42" s="24" t="s">
         <v>133</v>
       </c>
@@ -3310,7 +3435,7 @@
         <v>137</v>
       </c>
       <c r="D43" s="13">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="E43" s="13">
         <v>0.8</v>
@@ -3332,7 +3457,7 @@
         <v>136</v>
       </c>
       <c r="D44" s="12" t="s">
-        <v>109</v>
+        <v>220</v>
       </c>
       <c r="E44" s="12" t="s">
         <v>109</v>
@@ -3355,11 +3480,11 @@
       </c>
       <c r="D45" s="34" t="str">
         <f>_xlfn.XLOOKUP(D44,table_listings!$B$2:$B$201,table_listings!$D$2:$D$201,,0)</f>
-        <v>Sex Distinct</v>
+        <v>Select and Ultimate Aggregate</v>
       </c>
       <c r="E45" s="34" t="str">
         <f>_xlfn.XLOOKUP(E44,table_listings!$B$2:$B$201,table_listings!$D$2:$D$201,,0)</f>
-        <v>Sex Distinct</v>
+        <v>Attained Age Aggregate</v>
       </c>
       <c r="F45" s="13"/>
       <c r="G45" s="13"/>
@@ -3389,7 +3514,7 @@
       <c r="I46" s="12"/>
       <c r="J46" s="12"/>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A47" s="24" t="s">
         <v>132</v>
       </c>
@@ -3411,7 +3536,7 @@
       <c r="I47" s="13"/>
       <c r="J47" s="13"/>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A48" s="24" t="s">
         <v>132</v>
       </c>
@@ -3433,7 +3558,7 @@
       <c r="I48" s="12"/>
       <c r="J48" s="12"/>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A49" s="24" t="s">
         <v>132</v>
       </c>
@@ -3457,7 +3582,7 @@
       <c r="I49" s="13"/>
       <c r="J49" s="13"/>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A50" s="24" t="s">
         <v>132</v>
       </c>
@@ -3479,7 +3604,7 @@
       <c r="I50" s="12"/>
       <c r="J50" s="12"/>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A51" s="15" t="s">
         <v>132</v>
       </c>
@@ -3501,7 +3626,7 @@
       <c r="I51" s="13"/>
       <c r="J51" s="13"/>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A52" s="15" t="s">
         <v>132</v>
       </c>
@@ -3523,7 +3648,7 @@
       <c r="I52" s="12"/>
       <c r="J52" s="12"/>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A53" s="15" t="s">
         <v>132</v>
       </c>
@@ -3547,7 +3672,7 @@
       <c r="I53" s="13"/>
       <c r="J53" s="13"/>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A54" s="15" t="s">
         <v>132</v>
       </c>
@@ -3569,7 +3694,7 @@
       <c r="I54" s="12"/>
       <c r="J54" s="12"/>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A55" s="24" t="s">
         <v>132</v>
       </c>
@@ -3591,7 +3716,7 @@
       <c r="I55" s="13"/>
       <c r="J55" s="13"/>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A56" s="24" t="s">
         <v>132</v>
       </c>
@@ -3613,7 +3738,7 @@
       <c r="I56" s="12"/>
       <c r="J56" s="12"/>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A57" s="24" t="s">
         <v>132</v>
       </c>
@@ -3637,7 +3762,7 @@
       <c r="I57" s="13"/>
       <c r="J57" s="13"/>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A58" s="24" t="s">
         <v>132</v>
       </c>
@@ -3659,7 +3784,7 @@
       <c r="I58" s="13"/>
       <c r="J58" s="13"/>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A59" s="24" t="s">
         <v>132</v>
       </c>
@@ -3681,7 +3806,7 @@
       <c r="I59" s="14"/>
       <c r="J59" s="14"/>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A60" s="15" t="s">
         <v>132</v>
       </c>
@@ -3703,7 +3828,7 @@
       <c r="I60" s="13"/>
       <c r="J60" s="13"/>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A61" s="15" t="s">
         <v>132</v>
       </c>
@@ -3725,7 +3850,7 @@
       <c r="I61" s="12"/>
       <c r="J61" s="12"/>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A62" s="15" t="s">
         <v>132</v>
       </c>
@@ -3749,7 +3874,7 @@
       <c r="I62" s="13"/>
       <c r="J62" s="13"/>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A63" s="27" t="s">
         <v>132</v>
       </c>
@@ -3782,7 +3907,7 @@
         <v>137</v>
       </c>
       <c r="D64" s="13">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="E64" s="13">
         <v>0.8</v>
@@ -3804,7 +3929,7 @@
         <v>136</v>
       </c>
       <c r="D65" s="12" t="s">
-        <v>109</v>
+        <v>220</v>
       </c>
       <c r="E65" s="12" t="s">
         <v>109</v>
@@ -3827,11 +3952,11 @@
       </c>
       <c r="D66" s="34" t="str">
         <f>_xlfn.XLOOKUP(D65,table_listings!$B$2:$B$201,table_listings!$D$2:$D$201,,0)</f>
-        <v>Sex Distinct</v>
+        <v>Select and Ultimate Aggregate</v>
       </c>
       <c r="E66" s="34" t="str">
         <f>_xlfn.XLOOKUP(E65,table_listings!$B$2:$B$201,table_listings!$D$2:$D$201,,0)</f>
-        <v>Sex Distinct</v>
+        <v>Attained Age Aggregate</v>
       </c>
       <c r="F66" s="13"/>
       <c r="G66" s="13"/>
@@ -3861,7 +3986,7 @@
       <c r="I67" s="12"/>
       <c r="J67" s="12"/>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A68" s="15" t="s">
         <v>131</v>
       </c>
@@ -3883,7 +4008,7 @@
       <c r="I68" s="13"/>
       <c r="J68" s="13"/>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A69" s="15" t="s">
         <v>131</v>
       </c>
@@ -3905,7 +4030,7 @@
       <c r="I69" s="13"/>
       <c r="J69" s="13"/>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A70" s="15" t="s">
         <v>131</v>
       </c>
@@ -3929,7 +4054,7 @@
       <c r="I70" s="13"/>
       <c r="J70" s="13"/>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A71" s="15" t="s">
         <v>131</v>
       </c>
@@ -3951,7 +4076,7 @@
       <c r="I71" s="13"/>
       <c r="J71" s="13"/>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A72" s="24" t="s">
         <v>131</v>
       </c>
@@ -3973,7 +4098,7 @@
       <c r="I72" s="13"/>
       <c r="J72" s="13"/>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A73" s="24" t="s">
         <v>131</v>
       </c>
@@ -3995,7 +4120,7 @@
       <c r="I73" s="12"/>
       <c r="J73" s="12"/>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A74" s="24" t="s">
         <v>131</v>
       </c>
@@ -4019,7 +4144,7 @@
       <c r="I74" s="13"/>
       <c r="J74" s="13"/>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A75" s="24" t="s">
         <v>131</v>
       </c>
@@ -4041,7 +4166,7 @@
       <c r="I75" s="12"/>
       <c r="J75" s="12"/>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A76" s="15" t="s">
         <v>131</v>
       </c>
@@ -4063,7 +4188,7 @@
       <c r="I76" s="13"/>
       <c r="J76" s="13"/>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A77" s="15" t="s">
         <v>131</v>
       </c>
@@ -4085,7 +4210,7 @@
       <c r="I77" s="13"/>
       <c r="J77" s="13"/>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A78" s="15" t="s">
         <v>131</v>
       </c>
@@ -4109,7 +4234,7 @@
       <c r="I78" s="13"/>
       <c r="J78" s="13"/>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A79" s="15" t="s">
         <v>131</v>
       </c>
@@ -4131,7 +4256,7 @@
       <c r="I79" s="13"/>
       <c r="J79" s="13"/>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A80" s="15" t="s">
         <v>131</v>
       </c>
@@ -4153,7 +4278,7 @@
       <c r="I80" s="13"/>
       <c r="J80" s="13"/>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A81" s="24" t="s">
         <v>131</v>
       </c>
@@ -4175,7 +4300,7 @@
       <c r="I81" s="13"/>
       <c r="J81" s="13"/>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A82" s="24" t="s">
         <v>131</v>
       </c>
@@ -4197,7 +4322,7 @@
       <c r="I82" s="13"/>
       <c r="J82" s="13"/>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A83" s="24" t="s">
         <v>131</v>
       </c>
@@ -4221,7 +4346,7 @@
       <c r="I83" s="13"/>
       <c r="J83" s="13"/>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A84" s="30" t="s">
         <v>131</v>
       </c>
@@ -4244,7 +4369,13 @@
       <c r="J84" s="12"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C84" xr:uid="{C1E729B3-29BA-40F1-80D4-2208DEC4BA85}"/>
+  <autoFilter ref="A1:C84" xr:uid="{C1E729B3-29BA-40F1-80D4-2208DEC4BA85}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="mortality"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <conditionalFormatting sqref="D5:E5 D9:E9 D13:E13 D17:E17">
     <cfRule type="expression" dxfId="0" priority="4">
       <formula>D4&lt;&gt;"User Defined Table"</formula>
@@ -4325,17 +4456,17 @@
   <dimension ref="A1:D201"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B74" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2:XFD21"/>
+      <selection pane="bottomRight" activeCell="D82" sqref="D82:D84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="15.77734375" customWidth="1"/>
-    <col min="3" max="3" width="29.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.44140625" customWidth="1"/>
+    <col min="3" max="3" width="60.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="45" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.3">
@@ -5722,79 +5853,79 @@
       </c>
       <c r="C82" s="9" t="str">
         <f>[1]mortality!B2</f>
-        <v>Mortality Table Sex Distinct</v>
+        <v>Attained Age Aggregate Mortality Table</v>
       </c>
       <c r="D82" s="9" t="str">
         <f>[1]mortality!C2</f>
-        <v>Sex Distinct</v>
+        <v>Attained Age Aggregate</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="B83" s="9">
+      <c r="B83" s="9" t="str">
         <f>[1]mortality!A3</f>
-        <v>0</v>
-      </c>
-      <c r="C83" s="9">
+        <v>MORT02</v>
+      </c>
+      <c r="C83" s="9" t="str">
         <f>[1]mortality!B3</f>
-        <v>0</v>
-      </c>
-      <c r="D83" s="9">
+        <v>Attained Age Sex Distinct Mortality Table</v>
+      </c>
+      <c r="D83" s="9" t="str">
         <f>[1]mortality!C3</f>
-        <v>0</v>
+        <v>Attained Age Sex Distinct</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="B84" s="9">
+      <c r="B84" s="9" t="str">
         <f>[1]mortality!A4</f>
-        <v>0</v>
-      </c>
-      <c r="C84" s="9">
+        <v>MORT03</v>
+      </c>
+      <c r="C84" s="9" t="str">
         <f>[1]mortality!B4</f>
-        <v>0</v>
-      </c>
-      <c r="D84" s="9">
+        <v>Attained Age Sex Smoker Distinct Mortality Table</v>
+      </c>
+      <c r="D84" s="9" t="str">
         <f>[1]mortality!C4</f>
-        <v>0</v>
+        <v>Attained Age Sex Smoker Distinct</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="B85" s="9">
+      <c r="B85" s="9" t="str">
         <f>[1]mortality!A5</f>
-        <v>0</v>
-      </c>
-      <c r="C85" s="9">
+        <v>MORT04</v>
+      </c>
+      <c r="C85" s="9" t="str">
         <f>[1]mortality!B5</f>
-        <v>0</v>
-      </c>
-      <c r="D85" s="9">
+        <v>Attained Age Select and Ultimate Table</v>
+      </c>
+      <c r="D85" s="9" t="str">
         <f>[1]mortality!C5</f>
-        <v>0</v>
+        <v>Select and Ultimate Aggregate</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="B86" s="9">
+      <c r="B86" s="9" t="str">
         <f>[1]mortality!A6</f>
-        <v>0</v>
-      </c>
-      <c r="C86" s="9">
+        <v>MORT05</v>
+      </c>
+      <c r="C86" s="9" t="str">
         <f>[1]mortality!B6</f>
-        <v>0</v>
-      </c>
-      <c r="D86" s="9">
+        <v>Reference Table for CSO Composite Select and Ultimate Table</v>
+      </c>
+      <c r="D86" s="9" t="str">
         <f>[1]mortality!C6</f>
-        <v>0</v>
+        <v>Reference Table for SOA Select and Ultimate Table</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.3">
@@ -8533,18 +8664,18 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA1111D6-CFD5-472E-AAF0-AF6E36C438B2}">
-  <dimension ref="B1:E23"/>
+  <dimension ref="B1:E36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="30.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="69.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="63.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="31.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="46.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:5" x14ac:dyDescent="0.3">
@@ -8673,58 +8804,139 @@
         <v>200</v>
       </c>
     </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B12" s="36" t="s">
+        <v>210</v>
+      </c>
+      <c r="C12" s="36" t="s">
+        <v>188</v>
+      </c>
+      <c r="D12" s="36"/>
+      <c r="E12" s="36"/>
+    </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B13" s="36" t="s">
-        <v>179</v>
+      <c r="B13" t="s">
+        <v>211</v>
+      </c>
+      <c r="C13" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>180</v>
+        <v>211</v>
+      </c>
+      <c r="C14" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>181</v>
+        <v>211</v>
+      </c>
+      <c r="C15" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
+        <v>118</v>
+      </c>
+      <c r="C16" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C17" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B25" s="36" t="s">
+        <v>179</v>
+      </c>
+      <c r="C25" s="36" t="s">
+        <v>213</v>
+      </c>
+      <c r="D25" s="36"/>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B26" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B27" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B28" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B17" t="s">
+    <row r="29" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B29" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B18" t="s">
+    <row r="30" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B30" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B19" t="s">
+    <row r="31" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B31" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B32" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B20" t="s">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B33" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B21" t="s">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B34" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B22" t="s">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B35" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B23" t="s">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B36" t="s">
         <v>186</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add mort and lapse table types
</commit_message>
<xml_diff>
--- a/Input/Settings.xlsx
+++ b/Input/Settings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Julia\TradLifeModel\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D5C1085-8478-458B-83E8-39D8D1C0D7D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67A34FA1-E508-4F14-975B-51164B34A48B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="889" activeTab="2" xr2:uid="{ADF8BBD9-0F7A-45CB-8EA8-A3D46B124E82}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="889" activeTab="5" xr2:uid="{ADF8BBD9-0F7A-45CB-8EA8-A3D46B124E82}"/>
   </bookViews>
   <sheets>
     <sheet name="general_settings" sheetId="13" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="854" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="878" uniqueCount="230">
   <si>
     <t>acq_exp_per_pol</t>
   </si>
@@ -657,9 +657,6 @@
     <t>prem_term</t>
   </si>
   <si>
-    <t>COMM03</t>
-  </si>
-  <si>
     <t>PREM03</t>
   </si>
   <si>
@@ -681,9 +678,6 @@
     <t>Assumptions in product_setup</t>
   </si>
   <si>
-    <t>moratlity</t>
-  </si>
-  <si>
     <t>smoking_status</t>
   </si>
   <si>
@@ -693,9 +687,6 @@
     <t>Base</t>
   </si>
   <si>
-    <t>Attained Age Aggregate Rate</t>
-  </si>
-  <si>
     <t>Attained Age Sex Distinct</t>
   </si>
   <si>
@@ -708,7 +699,43 @@
     <t>Rate by Policy Year and Policy Term and Premium Term</t>
   </si>
   <si>
-    <t>MORT04</t>
+    <t>Select and Ultimate - Sex Distinct - SOA Table ID</t>
+  </si>
+  <si>
+    <t>Select and Ultimate - Sex Smoker Distinct - SOA Table ID</t>
+  </si>
+  <si>
+    <t>Applied in accordance to the sex field of each model point.</t>
+  </si>
+  <si>
+    <t>Applied in accordance to the sex and smoker fields of each model point.</t>
+  </si>
+  <si>
+    <t>Applied to all model points regardless of sex or smoker status of each model point.</t>
+  </si>
+  <si>
+    <t>LAPSE02</t>
+  </si>
+  <si>
+    <t>Multi-Index Tables</t>
+  </si>
+  <si>
+    <t>Other Notes</t>
+  </si>
+  <si>
+    <t>MORT05</t>
+  </si>
+  <si>
+    <t>Attained Age</t>
+  </si>
+  <si>
+    <t>Select and Ultimate</t>
+  </si>
+  <si>
+    <t>Select and Ultimate - Sex Distinct</t>
+  </si>
+  <si>
+    <t>Select and Ultimate - Sex Smoker Distinct</t>
   </si>
 </sst>
 </file>
@@ -871,11 +898,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -943,10 +971,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -997,12 +1030,17 @@
       <sheetName val="MORT03"/>
       <sheetName val="MORT04"/>
       <sheetName val="MORT05"/>
+      <sheetName val="MORT06"/>
+      <sheetName val="MORT07"/>
+      <sheetName val="MORT08"/>
       <sheetName val="lapse"/>
       <sheetName val="LAPSE01"/>
+      <sheetName val="LAPSE02"/>
       <sheetName val="expense"/>
       <sheetName val="EXP01"/>
       <sheetName val="disc_rate"/>
       <sheetName val="DISCRT01"/>
+      <sheetName val="DISCRT02"/>
       <sheetName val="prem_tax"/>
       <sheetName val="PREMTAX01"/>
       <sheetName val="tax"/>
@@ -1117,10 +1155,10 @@
             <v>COMM01</v>
           </cell>
           <cell r="B2" t="str">
-            <v>Commission Percentage by Policy Year/Policy Term</v>
+            <v>Commission % by Policy Year/Policy Term</v>
           </cell>
           <cell r="C2" t="str">
-            <v>Perc by Year/Pol Term</v>
+            <v>Perc by Pol Year/Pol Term</v>
           </cell>
         </row>
         <row r="3">
@@ -1128,7 +1166,7 @@
             <v>COMM02UDT</v>
           </cell>
           <cell r="B3" t="str">
-            <v>Commission Percentage UDT</v>
+            <v>Commission % UDT</v>
           </cell>
           <cell r="C3" t="str">
             <v>User Defined Table</v>
@@ -1139,7 +1177,7 @@
             <v>COMM03</v>
           </cell>
           <cell r="B4" t="str">
-            <v>Commission Percentage by Policy Year/Policy Term/Prem Paying Term</v>
+            <v>Commission % by Policy Year/Policy Term/Prem Paying Term</v>
           </cell>
           <cell r="C4" t="str">
             <v>Perc by Pol Year/Pol Term/Prem Term</v>
@@ -1155,10 +1193,10 @@
             <v>MORT01</v>
           </cell>
           <cell r="B2" t="str">
-            <v>Attained Age Aggregate Mortality Table</v>
+            <v>Attained Age Unisex Mortality Table</v>
           </cell>
           <cell r="C2" t="str">
-            <v>Attained Age Aggregate</v>
+            <v>Attained Age</v>
           </cell>
         </row>
         <row r="3">
@@ -1188,10 +1226,10 @@
             <v>MORT04</v>
           </cell>
           <cell r="B5" t="str">
-            <v>Attained Age Select and Ultimate Table</v>
+            <v>Select and Ultimate Table - Unisex</v>
           </cell>
           <cell r="C5" t="str">
-            <v>Select and Ultimate Aggregate</v>
+            <v>Select and Ultimate</v>
           </cell>
         </row>
         <row r="6">
@@ -1199,25 +1237,55 @@
             <v>MORT05</v>
           </cell>
           <cell r="B6" t="str">
-            <v>Reference Table for CSO Composite Select and Ultimate Table</v>
+            <v xml:space="preserve">Select and Ultimate Table - Sex Distinct </v>
           </cell>
           <cell r="C6" t="str">
-            <v>Reference Table for SOA Select and Ultimate Table</v>
+            <v>Select and Ultimate - Sex Distinct</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="A7" t="str">
+            <v>MORT06</v>
+          </cell>
+          <cell r="B7" t="str">
+            <v xml:space="preserve">Select and Ultimate Table - Sex Smoker Distinct </v>
+          </cell>
+          <cell r="C7" t="str">
+            <v>Select and Ultimate - Sex Smoker Distinct</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="A8" t="str">
+            <v>MORT07</v>
+          </cell>
+          <cell r="B8" t="str">
+            <v>2001 CSO Select and Ultimate - Male &amp; Female</v>
+          </cell>
+          <cell r="C8" t="str">
+            <v>Select and Ultimate - Sex Distinct - SOA Table ID</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="A9" t="str">
+            <v>MORT08</v>
+          </cell>
+          <cell r="B9" t="str">
+            <v>2001 CSO Select and Ultimate - MN, FN, MS, FS</v>
+          </cell>
+          <cell r="C9" t="str">
+            <v>Select and Ultimate - Sex Smoker Distinct - SOA Table ID</v>
           </cell>
         </row>
       </sheetData>
       <sheetData sheetId="16"/>
       <sheetData sheetId="17"/>
       <sheetData sheetId="18"/>
-      <sheetData sheetId="19">
-        <row r="1">
-          <cell r="B1">
-            <v>1</v>
-          </cell>
-        </row>
-      </sheetData>
+      <sheetData sheetId="19"/>
       <sheetData sheetId="20"/>
-      <sheetData sheetId="21">
+      <sheetData sheetId="21"/>
+      <sheetData sheetId="22"/>
+      <sheetData sheetId="23"/>
+      <sheetData sheetId="24">
         <row r="2">
           <cell r="A2" t="str">
             <v>LAPSE01</v>
@@ -1226,12 +1294,24 @@
             <v>Lapse Table</v>
           </cell>
           <cell r="C2" t="str">
-            <v>Policy Year</v>
+            <v>Pol Year/Pol Term</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="A3" t="str">
+            <v>LAPSE02</v>
+          </cell>
+          <cell r="B3" t="str">
+            <v>Lapse Table</v>
+          </cell>
+          <cell r="C3" t="str">
+            <v>Pol Year/Pol Term/Prem Term</v>
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="22"/>
-      <sheetData sheetId="23">
+      <sheetData sheetId="25"/>
+      <sheetData sheetId="26"/>
+      <sheetData sheetId="27">
         <row r="2">
           <cell r="A2" t="str">
             <v>EXP01</v>
@@ -1244,8 +1324,8 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="24"/>
-      <sheetData sheetId="25">
+      <sheetData sheetId="28"/>
+      <sheetData sheetId="29">
         <row r="2">
           <cell r="A2" t="str">
             <v>DISCRT01</v>
@@ -1258,8 +1338,9 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="26"/>
-      <sheetData sheetId="27">
+      <sheetData sheetId="30"/>
+      <sheetData sheetId="31"/>
+      <sheetData sheetId="32">
         <row r="2">
           <cell r="A2" t="str">
             <v>PREMTAX01</v>
@@ -1272,8 +1353,8 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="28"/>
-      <sheetData sheetId="29">
+      <sheetData sheetId="33"/>
+      <sheetData sheetId="34">
         <row r="2">
           <cell r="A2" t="str">
             <v>TAX01</v>
@@ -1286,7 +1367,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="30"/>
+      <sheetData sheetId="35"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1622,7 +1703,7 @@
         <v>167</v>
       </c>
       <c r="B3" s="12">
-        <v>120</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -1883,7 +1964,7 @@
         <v>81</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>80</v>
@@ -2479,11 +2560,11 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:J84"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D45" sqref="D45"/>
+      <selection pane="bottomRight" activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2547,7 +2628,7 @@
         <v>136</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E3" s="13" t="s">
         <v>176</v>
@@ -2721,7 +2802,7 @@
         <v>136</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E11" s="12" t="s">
         <v>130</v>
@@ -2807,7 +2888,7 @@
         <v>136</v>
       </c>
       <c r="D15" s="13" t="s">
-        <v>203</v>
+        <v>124</v>
       </c>
       <c r="E15" s="13" t="s">
         <v>124</v>
@@ -2830,11 +2911,11 @@
       </c>
       <c r="D16" s="34" t="str">
         <f>_xlfn.XLOOKUP(D15,table_listings!$B$2:$B$201,table_listings!$D$2:$D$201,,0)</f>
-        <v>Perc by Pol Year/Pol Term/Prem Term</v>
+        <v>Perc by Pol Year/Pol Term</v>
       </c>
       <c r="E16" s="34" t="str">
         <f>_xlfn.XLOOKUP(E15,table_listings!$B$2:$B$201,table_listings!$D$2:$D$201,,0)</f>
-        <v>Perc by Year/Pol Term</v>
+        <v>Perc by Pol Year/Pol Term</v>
       </c>
       <c r="F16" s="13"/>
       <c r="G16" s="13"/>
@@ -2860,7 +2941,7 @@
       <c r="I17" s="12"/>
       <c r="J17" s="12"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18" s="21" t="s">
         <v>133</v>
       </c>
@@ -2882,7 +2963,7 @@
       <c r="I18" s="13"/>
       <c r="J18" s="13"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19" s="24" t="s">
         <v>133</v>
       </c>
@@ -2893,7 +2974,7 @@
         <v>136</v>
       </c>
       <c r="D19" s="12" t="s">
-        <v>220</v>
+        <v>225</v>
       </c>
       <c r="E19" s="12" t="s">
         <v>109</v>
@@ -2904,7 +2985,7 @@
       <c r="I19" s="12"/>
       <c r="J19" s="12"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20" s="24" t="s">
         <v>133</v>
       </c>
@@ -2916,11 +2997,11 @@
       </c>
       <c r="D20" s="34" t="str">
         <f>_xlfn.XLOOKUP(D19,table_listings!$B$2:$B$201,table_listings!$D$2:$D$201,,0)</f>
-        <v>Select and Ultimate Aggregate</v>
+        <v>Select and Ultimate - Sex Distinct</v>
       </c>
       <c r="E20" s="34" t="str">
         <f>_xlfn.XLOOKUP(E19,table_listings!$B$2:$B$201,table_listings!$D$2:$D$201,,0)</f>
-        <v>Attained Age Aggregate</v>
+        <v>Attained Age</v>
       </c>
       <c r="F20" s="13"/>
       <c r="G20" s="13"/>
@@ -2961,7 +3042,7 @@
         <v>136</v>
       </c>
       <c r="D22" s="12" t="s">
-        <v>123</v>
+        <v>222</v>
       </c>
       <c r="E22" s="12" t="s">
         <v>123</v>
@@ -2984,11 +3065,11 @@
       </c>
       <c r="D23" s="34" t="str">
         <f>_xlfn.XLOOKUP(D22,table_listings!$B$2:$B$201,table_listings!$D$2:$D$201,,0)</f>
-        <v>Policy Year</v>
+        <v>Pol Year/Pol Term/Prem Term</v>
       </c>
       <c r="E23" s="34" t="str">
         <f>_xlfn.XLOOKUP(E22,table_listings!$B$2:$B$201,table_listings!$D$2:$D$201,,0)</f>
-        <v>Policy Year</v>
+        <v>Pol Year/Pol Term</v>
       </c>
       <c r="F23" s="13"/>
       <c r="G23" s="13"/>
@@ -3064,7 +3145,7 @@
       <c r="I26" s="13"/>
       <c r="J26" s="13"/>
     </row>
-    <row r="27" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" s="15" t="s">
         <v>133</v>
       </c>
@@ -3086,7 +3167,7 @@
       <c r="I27" s="13"/>
       <c r="J27" s="13"/>
     </row>
-    <row r="28" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" s="15" t="s">
         <v>133</v>
       </c>
@@ -3108,7 +3189,7 @@
       <c r="I28" s="12"/>
       <c r="J28" s="12"/>
     </row>
-    <row r="29" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" s="15" t="s">
         <v>133</v>
       </c>
@@ -3132,7 +3213,7 @@
       <c r="I29" s="13"/>
       <c r="J29" s="13"/>
     </row>
-    <row r="30" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" s="15" t="s">
         <v>133</v>
       </c>
@@ -3424,7 +3505,7 @@
       <c r="I42" s="12"/>
       <c r="J42" s="12"/>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A43" s="17" t="s">
         <v>132</v>
       </c>
@@ -3446,7 +3527,7 @@
       <c r="I43" s="13"/>
       <c r="J43" s="13"/>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A44" s="15" t="s">
         <v>132</v>
       </c>
@@ -3457,7 +3538,7 @@
         <v>136</v>
       </c>
       <c r="D44" s="12" t="s">
-        <v>220</v>
+        <v>225</v>
       </c>
       <c r="E44" s="12" t="s">
         <v>109</v>
@@ -3468,7 +3549,7 @@
       <c r="I44" s="12"/>
       <c r="J44" s="12"/>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A45" s="15" t="s">
         <v>132</v>
       </c>
@@ -3480,11 +3561,11 @@
       </c>
       <c r="D45" s="34" t="str">
         <f>_xlfn.XLOOKUP(D44,table_listings!$B$2:$B$201,table_listings!$D$2:$D$201,,0)</f>
-        <v>Select and Ultimate Aggregate</v>
+        <v>Select and Ultimate - Sex Distinct</v>
       </c>
       <c r="E45" s="34" t="str">
         <f>_xlfn.XLOOKUP(E44,table_listings!$B$2:$B$201,table_listings!$D$2:$D$201,,0)</f>
-        <v>Attained Age Aggregate</v>
+        <v>Attained Age</v>
       </c>
       <c r="F45" s="13"/>
       <c r="G45" s="13"/>
@@ -3492,7 +3573,7 @@
       <c r="I45" s="13"/>
       <c r="J45" s="13"/>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A46" s="15" t="s">
         <v>132</v>
       </c>
@@ -3547,7 +3628,7 @@
         <v>136</v>
       </c>
       <c r="D48" s="12" t="s">
-        <v>123</v>
+        <v>222</v>
       </c>
       <c r="E48" s="12" t="s">
         <v>123</v>
@@ -3570,11 +3651,11 @@
       </c>
       <c r="D49" s="34" t="str">
         <f>_xlfn.XLOOKUP(D48,table_listings!$B$2:$B$201,table_listings!$D$2:$D$201,,0)</f>
-        <v>Policy Year</v>
+        <v>Pol Year/Pol Term/Prem Term</v>
       </c>
       <c r="E49" s="34" t="str">
         <f>_xlfn.XLOOKUP(E48,table_listings!$B$2:$B$201,table_listings!$D$2:$D$201,,0)</f>
-        <v>Policy Year</v>
+        <v>Pol Year/Pol Term</v>
       </c>
       <c r="F49" s="13"/>
       <c r="G49" s="13"/>
@@ -3592,10 +3673,10 @@
       <c r="C50" s="25" t="s">
         <v>134</v>
       </c>
-      <c r="D50" s="12">
+      <c r="D50" s="37">
         <v>0.2</v>
       </c>
-      <c r="E50" s="12">
+      <c r="E50" s="37">
         <v>0.2</v>
       </c>
       <c r="F50" s="12"/>
@@ -3694,7 +3775,7 @@
       <c r="I54" s="12"/>
       <c r="J54" s="12"/>
     </row>
-    <row r="55" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A55" s="24" t="s">
         <v>132</v>
       </c>
@@ -3716,7 +3797,7 @@
       <c r="I55" s="13"/>
       <c r="J55" s="13"/>
     </row>
-    <row r="56" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A56" s="24" t="s">
         <v>132</v>
       </c>
@@ -3738,7 +3819,7 @@
       <c r="I56" s="12"/>
       <c r="J56" s="12"/>
     </row>
-    <row r="57" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A57" s="24" t="s">
         <v>132</v>
       </c>
@@ -3762,7 +3843,7 @@
       <c r="I57" s="13"/>
       <c r="J57" s="13"/>
     </row>
-    <row r="58" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A58" s="24" t="s">
         <v>132</v>
       </c>
@@ -3784,7 +3865,7 @@
       <c r="I58" s="13"/>
       <c r="J58" s="13"/>
     </row>
-    <row r="59" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A59" s="24" t="s">
         <v>132</v>
       </c>
@@ -3896,7 +3977,7 @@
       <c r="I63" s="12"/>
       <c r="J63" s="12"/>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A64" s="24" t="s">
         <v>131</v>
       </c>
@@ -3918,7 +3999,7 @@
       <c r="I64" s="13"/>
       <c r="J64" s="13"/>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A65" s="24" t="s">
         <v>131</v>
       </c>
@@ -3929,7 +4010,7 @@
         <v>136</v>
       </c>
       <c r="D65" s="12" t="s">
-        <v>220</v>
+        <v>225</v>
       </c>
       <c r="E65" s="12" t="s">
         <v>109</v>
@@ -3940,7 +4021,7 @@
       <c r="I65" s="12"/>
       <c r="J65" s="12"/>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A66" s="24" t="s">
         <v>131</v>
       </c>
@@ -3952,11 +4033,11 @@
       </c>
       <c r="D66" s="34" t="str">
         <f>_xlfn.XLOOKUP(D65,table_listings!$B$2:$B$201,table_listings!$D$2:$D$201,,0)</f>
-        <v>Select and Ultimate Aggregate</v>
+        <v>Select and Ultimate - Sex Distinct</v>
       </c>
       <c r="E66" s="34" t="str">
         <f>_xlfn.XLOOKUP(E65,table_listings!$B$2:$B$201,table_listings!$D$2:$D$201,,0)</f>
-        <v>Attained Age Aggregate</v>
+        <v>Attained Age</v>
       </c>
       <c r="F66" s="13"/>
       <c r="G66" s="13"/>
@@ -3964,7 +4045,7 @@
       <c r="I66" s="13"/>
       <c r="J66" s="13"/>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A67" s="24" t="s">
         <v>131</v>
       </c>
@@ -4019,7 +4100,7 @@
         <v>136</v>
       </c>
       <c r="D69" s="12" t="s">
-        <v>123</v>
+        <v>222</v>
       </c>
       <c r="E69" s="12" t="s">
         <v>123</v>
@@ -4042,11 +4123,11 @@
       </c>
       <c r="D70" s="34" t="str">
         <f>_xlfn.XLOOKUP(D69,table_listings!$B$2:$B$201,table_listings!$D$2:$D$201,,0)</f>
-        <v>Policy Year</v>
+        <v>Pol Year/Pol Term/Prem Term</v>
       </c>
       <c r="E70" s="34" t="str">
         <f>_xlfn.XLOOKUP(E69,table_listings!$B$2:$B$201,table_listings!$D$2:$D$201,,0)</f>
-        <v>Policy Year</v>
+        <v>Pol Year/Pol Term</v>
       </c>
       <c r="F70" s="13"/>
       <c r="G70" s="13"/>
@@ -4166,7 +4247,7 @@
       <c r="I75" s="12"/>
       <c r="J75" s="12"/>
     </row>
-    <row r="76" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A76" s="15" t="s">
         <v>131</v>
       </c>
@@ -4188,7 +4269,7 @@
       <c r="I76" s="13"/>
       <c r="J76" s="13"/>
     </row>
-    <row r="77" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A77" s="15" t="s">
         <v>131</v>
       </c>
@@ -4210,7 +4291,7 @@
       <c r="I77" s="13"/>
       <c r="J77" s="13"/>
     </row>
-    <row r="78" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A78" s="15" t="s">
         <v>131</v>
       </c>
@@ -4234,7 +4315,7 @@
       <c r="I78" s="13"/>
       <c r="J78" s="13"/>
     </row>
-    <row r="79" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A79" s="15" t="s">
         <v>131</v>
       </c>
@@ -4256,7 +4337,7 @@
       <c r="I79" s="13"/>
       <c r="J79" s="13"/>
     </row>
-    <row r="80" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A80" s="15" t="s">
         <v>131</v>
       </c>
@@ -4372,7 +4453,7 @@
   <autoFilter ref="A1:C84" xr:uid="{C1E729B3-29BA-40F1-80D4-2208DEC4BA85}">
     <filterColumn colId="1">
       <filters>
-        <filter val="mortality"/>
+        <filter val="disc_rate"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -4395,13 +4476,13 @@
           <x14:formula1>
             <xm:f>table_listings!$B$82:$B$101</xm:f>
           </x14:formula1>
-          <xm:sqref>D44:E44 D65:E65 D19:E19</xm:sqref>
+          <xm:sqref>D19:E19 D44:E44 D65:E65</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{9B11AC40-BA78-465E-A8C2-ABDE8DC86665}">
           <x14:formula1>
             <xm:f>table_listings!$B$102:$B$121</xm:f>
           </x14:formula1>
-          <xm:sqref>D48:E48 D69:E69 D22:E22</xm:sqref>
+          <xm:sqref>D22:E22 D48:E48 D69:E69</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{AE6B13E0-3C67-444A-9E02-E0311D9C7B6B}">
           <x14:formula1>
@@ -4459,14 +4540,14 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B74" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D82" sqref="D82:D84"/>
+      <selection pane="bottomRight" activeCell="C114" sqref="C114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="15.77734375" customWidth="1"/>
     <col min="3" max="3" width="60.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="45" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="59.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.3">
@@ -5513,11 +5594,11 @@
       </c>
       <c r="C62" s="9" t="str">
         <f>[1]commission!B2</f>
-        <v>Commission Percentage by Policy Year/Policy Term</v>
+        <v>Commission % by Policy Year/Policy Term</v>
       </c>
       <c r="D62" s="9" t="str">
         <f>[1]commission!C2</f>
-        <v>Perc by Year/Pol Term</v>
+        <v>Perc by Pol Year/Pol Term</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
@@ -5530,7 +5611,7 @@
       </c>
       <c r="C63" s="9" t="str">
         <f>[1]commission!B3</f>
-        <v>Commission Percentage UDT</v>
+        <v>Commission % UDT</v>
       </c>
       <c r="D63" s="9" t="str">
         <f>[1]commission!C3</f>
@@ -5547,7 +5628,7 @@
       </c>
       <c r="C64" s="9" t="str">
         <f>[1]commission!B4</f>
-        <v>Commission Percentage by Policy Year/Policy Term/Prem Paying Term</v>
+        <v>Commission % by Policy Year/Policy Term/Prem Paying Term</v>
       </c>
       <c r="D64" s="9" t="str">
         <f>[1]commission!C4</f>
@@ -5853,11 +5934,11 @@
       </c>
       <c r="C82" s="9" t="str">
         <f>[1]mortality!B2</f>
-        <v>Attained Age Aggregate Mortality Table</v>
+        <v>Attained Age Unisex Mortality Table</v>
       </c>
       <c r="D82" s="9" t="str">
         <f>[1]mortality!C2</f>
-        <v>Attained Age Aggregate</v>
+        <v>Attained Age</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.3">
@@ -5904,11 +5985,11 @@
       </c>
       <c r="C85" s="9" t="str">
         <f>[1]mortality!B5</f>
-        <v>Attained Age Select and Ultimate Table</v>
+        <v>Select and Ultimate Table - Unisex</v>
       </c>
       <c r="D85" s="9" t="str">
         <f>[1]mortality!C5</f>
-        <v>Select and Ultimate Aggregate</v>
+        <v>Select and Ultimate</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
@@ -5921,62 +6002,62 @@
       </c>
       <c r="C86" s="9" t="str">
         <f>[1]mortality!B6</f>
-        <v>Reference Table for CSO Composite Select and Ultimate Table</v>
+        <v xml:space="preserve">Select and Ultimate Table - Sex Distinct </v>
       </c>
       <c r="D86" s="9" t="str">
         <f>[1]mortality!C6</f>
-        <v>Reference Table for SOA Select and Ultimate Table</v>
+        <v>Select and Ultimate - Sex Distinct</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="B87" s="9">
+      <c r="B87" s="9" t="str">
         <f>[1]mortality!A7</f>
-        <v>0</v>
-      </c>
-      <c r="C87" s="9">
+        <v>MORT06</v>
+      </c>
+      <c r="C87" s="9" t="str">
         <f>[1]mortality!B7</f>
-        <v>0</v>
-      </c>
-      <c r="D87" s="9">
+        <v xml:space="preserve">Select and Ultimate Table - Sex Smoker Distinct </v>
+      </c>
+      <c r="D87" s="9" t="str">
         <f>[1]mortality!C7</f>
-        <v>0</v>
+        <v>Select and Ultimate - Sex Smoker Distinct</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="B88" s="9">
+      <c r="B88" s="9" t="str">
         <f>[1]mortality!A8</f>
-        <v>0</v>
-      </c>
-      <c r="C88" s="9">
+        <v>MORT07</v>
+      </c>
+      <c r="C88" s="9" t="str">
         <f>[1]mortality!B8</f>
-        <v>0</v>
-      </c>
-      <c r="D88" s="9">
+        <v>2001 CSO Select and Ultimate - Male &amp; Female</v>
+      </c>
+      <c r="D88" s="9" t="str">
         <f>[1]mortality!C8</f>
-        <v>0</v>
+        <v>Select and Ultimate - Sex Distinct - SOA Table ID</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="B89" s="9">
+      <c r="B89" s="9" t="str">
         <f>[1]mortality!A9</f>
-        <v>0</v>
-      </c>
-      <c r="C89" s="9">
+        <v>MORT08</v>
+      </c>
+      <c r="C89" s="9" t="str">
         <f>[1]mortality!B9</f>
-        <v>0</v>
-      </c>
-      <c r="D89" s="9">
+        <v>2001 CSO Select and Ultimate - MN, FN, MS, FS</v>
+      </c>
+      <c r="D89" s="9" t="str">
         <f>[1]mortality!C9</f>
-        <v>0</v>
+        <v>Select and Ultimate - Sex Smoker Distinct - SOA Table ID</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.3">
@@ -6197,24 +6278,24 @@
       </c>
       <c r="D102" s="9" t="str">
         <f>[1]lapse!C2</f>
-        <v>Policy Year</v>
+        <v>Pol Year/Pol Term</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="B103" s="9">
+      <c r="B103" s="9" t="str">
         <f>[1]lapse!A3</f>
-        <v>0</v>
-      </c>
-      <c r="C103" s="9">
+        <v>LAPSE02</v>
+      </c>
+      <c r="C103" s="9" t="str">
         <f>[1]lapse!B3</f>
-        <v>0</v>
-      </c>
-      <c r="D103" s="9">
+        <v>Lapse Table</v>
+      </c>
+      <c r="D103" s="9" t="str">
         <f>[1]lapse!C3</f>
-        <v>0</v>
+        <v>Pol Year/Pol Term/Prem Term</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.3">
@@ -8664,10 +8745,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA1111D6-CFD5-472E-AAF0-AF6E36C438B2}">
-  <dimension ref="B1:E36"/>
+  <dimension ref="B1:F41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8676,9 +8757,10 @@
     <col min="3" max="3" width="63.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="31.77734375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B1" s="36" t="s">
         <v>195</v>
       </c>
@@ -8691,13 +8773,16 @@
       <c r="E1" s="36" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="F1" s="36" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>174</v>
       </c>
       <c r="C2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D2" t="s">
         <v>196</v>
@@ -8706,12 +8791,12 @@
         <v>174</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>174</v>
       </c>
       <c r="C3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D3" t="s">
         <v>196</v>
@@ -8719,8 +8804,11 @@
       <c r="E3" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="F3" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>174</v>
       </c>
@@ -8734,7 +8822,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>177</v>
       </c>
@@ -8748,12 +8836,12 @@
         <v>177</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>178</v>
       </c>
       <c r="C6" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D6" t="s">
         <v>197</v>
@@ -8762,12 +8850,12 @@
         <v>178</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>178</v>
       </c>
       <c r="C7" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D7" t="s">
         <v>197</v>
@@ -8775,8 +8863,11 @@
       <c r="E7" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="F7" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>144</v>
       </c>
@@ -8790,7 +8881,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>144</v>
       </c>
@@ -8803,10 +8894,13 @@
       <c r="E9" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="F9" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B12" s="36" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C12" s="36" t="s">
         <v>188</v>
@@ -8814,129 +8908,199 @@
       <c r="D12" s="36"/>
       <c r="E12" s="36"/>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>211</v>
-      </c>
-      <c r="C13" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
+        <v>117</v>
+      </c>
+      <c r="C13" s="38" t="s">
+        <v>226</v>
+      </c>
+      <c r="D13" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>211</v>
-      </c>
-      <c r="C14" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
+        <v>117</v>
+      </c>
+      <c r="C14" s="38" t="s">
+        <v>213</v>
+      </c>
+      <c r="D14" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>211</v>
-      </c>
-      <c r="C15" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.3">
+        <v>117</v>
+      </c>
+      <c r="C15" s="38" t="s">
+        <v>214</v>
+      </c>
+      <c r="D15" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>118</v>
-      </c>
-      <c r="C16" t="s">
-        <v>218</v>
+        <v>117</v>
+      </c>
+      <c r="C16" s="38" t="s">
+        <v>227</v>
+      </c>
+      <c r="D16" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C17" t="s">
+      <c r="B17" t="s">
+        <v>117</v>
+      </c>
+      <c r="C17" s="38" t="s">
+        <v>228</v>
+      </c>
+      <c r="D17" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
-        <v>119</v>
+        <v>117</v>
+      </c>
+      <c r="C18" s="38" t="s">
+        <v>229</v>
+      </c>
+      <c r="D18" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>112</v>
+        <v>117</v>
+      </c>
+      <c r="C19" t="s">
+        <v>217</v>
+      </c>
+      <c r="D19" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
-        <v>120</v>
+        <v>117</v>
+      </c>
+      <c r="C20" t="s">
+        <v>218</v>
+      </c>
+      <c r="D20" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
-        <v>121</v>
+        <v>118</v>
+      </c>
+      <c r="C21" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
-        <v>122</v>
+        <v>118</v>
+      </c>
+      <c r="C22" t="s">
+        <v>216</v>
+      </c>
+      <c r="D22" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B23" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B24" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B25" s="36" t="s">
-        <v>179</v>
-      </c>
-      <c r="C25" s="36" t="s">
-        <v>213</v>
-      </c>
-      <c r="D25" s="36"/>
+      <c r="B25" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
-        <v>180</v>
+        <v>121</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B28" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B29" t="s">
-        <v>183</v>
+        <v>122</v>
       </c>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B30" t="s">
-        <v>184</v>
-      </c>
+      <c r="B30" s="36" t="s">
+        <v>179</v>
+      </c>
+      <c r="C30" s="36" t="s">
+        <v>211</v>
+      </c>
+      <c r="D30" s="36"/>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
-        <v>212</v>
+        <v>180</v>
       </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
-        <v>202</v>
+        <v>182</v>
       </c>
     </row>
     <row r="34" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
-        <v>175</v>
+        <v>183</v>
       </c>
     </row>
     <row r="35" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
-        <v>174</v>
+        <v>184</v>
       </c>
     </row>
     <row r="36" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="37" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B37" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="38" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B38" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="39" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B39" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="40" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B40" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="41" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B41" t="s">
         <v>186</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add projection and calendar year int rate tables
</commit_message>
<xml_diff>
--- a/Input/Settings.xlsx
+++ b/Input/Settings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Julia\TradLifeModel\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67A34FA1-E508-4F14-975B-51164B34A48B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71BDB82F-966C-46B2-8987-74033DC86EEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="889" activeTab="5" xr2:uid="{ADF8BBD9-0F7A-45CB-8EA8-A3D46B124E82}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="878" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="898" uniqueCount="237">
   <si>
     <t>acq_exp_per_pol</t>
   </si>
@@ -736,6 +736,27 @@
   </si>
   <si>
     <t>Select and Ultimate - Sex Smoker Distinct</t>
+  </si>
+  <si>
+    <t>proj_year</t>
+  </si>
+  <si>
+    <t>DISCRT03</t>
+  </si>
+  <si>
+    <t>Prj Year</t>
+  </si>
+  <si>
+    <t>Cal Year</t>
+  </si>
+  <si>
+    <t>Mix of Prj Year and Cal Year</t>
+  </si>
+  <si>
+    <t>Scalar</t>
+  </si>
+  <si>
+    <t>Per Policy and Perc of Premium by Policy Year</t>
   </si>
 </sst>
 </file>
@@ -795,7 +816,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -805,6 +826,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -974,7 +1001,7 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1041,6 +1068,7 @@
       <sheetName val="disc_rate"/>
       <sheetName val="DISCRT01"/>
       <sheetName val="DISCRT02"/>
+      <sheetName val="DISCRT03"/>
       <sheetName val="prem_tax"/>
       <sheetName val="PREMTAX01"/>
       <sheetName val="tax"/>
@@ -1331,16 +1359,39 @@
             <v>DISCRT01</v>
           </cell>
           <cell r="B2" t="str">
-            <v>Discount Rate Table</v>
+            <v>Policy Year Discount Rate Table</v>
           </cell>
           <cell r="C2" t="str">
-            <v>Policy Year</v>
+            <v>Prj Year</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="A3" t="str">
+            <v>DISCRT02</v>
+          </cell>
+          <cell r="B3" t="str">
+            <v>Calendar Year Discount Rate Table</v>
+          </cell>
+          <cell r="C3" t="str">
+            <v>Cal Year</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="A4" t="str">
+            <v>DISCRT03</v>
+          </cell>
+          <cell r="B4" t="str">
+            <v>CY: Invt Return and Disc Rate, PRJ_Y: Val Int Rate</v>
+          </cell>
+          <cell r="C4" t="str">
+            <v>Mix of Prj Year and Cal Year</v>
           </cell>
         </row>
       </sheetData>
       <sheetData sheetId="30"/>
       <sheetData sheetId="31"/>
-      <sheetData sheetId="32">
+      <sheetData sheetId="32"/>
+      <sheetData sheetId="33">
         <row r="2">
           <cell r="A2" t="str">
             <v>PREMTAX01</v>
@@ -1353,8 +1404,8 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="33"/>
-      <sheetData sheetId="34">
+      <sheetData sheetId="34"/>
+      <sheetData sheetId="35">
         <row r="2">
           <cell r="A2" t="str">
             <v>TAX01</v>
@@ -1367,7 +1418,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="35"/>
+      <sheetData sheetId="36"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1695,7 +1746,7 @@
         <v>168</v>
       </c>
       <c r="B2" s="33">
-        <v>45230</v>
+        <v>44561</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -2564,7 +2615,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D36" sqref="D36"/>
+      <selection pane="bottomRight" activeCell="D77" sqref="D77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3145,7 +3196,7 @@
       <c r="I26" s="13"/>
       <c r="J26" s="13"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27" s="15" t="s">
         <v>133</v>
       </c>
@@ -3178,7 +3229,7 @@
         <v>136</v>
       </c>
       <c r="D28" s="12" t="s">
-        <v>126</v>
+        <v>231</v>
       </c>
       <c r="E28" s="12" t="s">
         <v>126</v>
@@ -3201,11 +3252,11 @@
       </c>
       <c r="D29" s="34" t="str">
         <f>_xlfn.XLOOKUP(D28,table_listings!$B$2:$B$201,table_listings!$D$2:$D$201,,0)</f>
-        <v>Policy Year</v>
+        <v>Mix of Prj Year and Cal Year</v>
       </c>
       <c r="E29" s="34" t="str">
         <f>_xlfn.XLOOKUP(E28,table_listings!$B$2:$B$201,table_listings!$D$2:$D$201,,0)</f>
-        <v>Policy Year</v>
+        <v>Prj Year</v>
       </c>
       <c r="F29" s="13"/>
       <c r="G29" s="13"/>
@@ -3257,7 +3308,7 @@
       <c r="I31" s="13"/>
       <c r="J31" s="13"/>
     </row>
-    <row r="32" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" s="24" t="s">
         <v>133</v>
       </c>
@@ -3268,7 +3319,7 @@
         <v>136</v>
       </c>
       <c r="D32" s="12" t="s">
-        <v>126</v>
+        <v>231</v>
       </c>
       <c r="E32" s="12" t="s">
         <v>126</v>
@@ -3279,7 +3330,7 @@
       <c r="I32" s="12"/>
       <c r="J32" s="12"/>
     </row>
-    <row r="33" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" s="24" t="s">
         <v>133</v>
       </c>
@@ -3291,11 +3342,11 @@
       </c>
       <c r="D33" s="34" t="str">
         <f>_xlfn.XLOOKUP(D32,table_listings!$B$2:$B$201,table_listings!$D$2:$D$201,,0)</f>
-        <v>Policy Year</v>
+        <v>Mix of Prj Year and Cal Year</v>
       </c>
       <c r="E33" s="34" t="str">
         <f>_xlfn.XLOOKUP(E32,table_listings!$B$2:$B$201,table_listings!$D$2:$D$201,,0)</f>
-        <v>Policy Year</v>
+        <v>Prj Year</v>
       </c>
       <c r="F33" s="13"/>
       <c r="G33" s="13"/>
@@ -3303,7 +3354,7 @@
       <c r="I33" s="13"/>
       <c r="J33" s="13"/>
     </row>
-    <row r="34" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34" s="24" t="s">
         <v>133</v>
       </c>
@@ -3775,7 +3826,7 @@
       <c r="I54" s="12"/>
       <c r="J54" s="12"/>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A55" s="24" t="s">
         <v>132</v>
       </c>
@@ -3808,7 +3859,7 @@
         <v>136</v>
       </c>
       <c r="D56" s="12" t="s">
-        <v>126</v>
+        <v>231</v>
       </c>
       <c r="E56" s="12" t="s">
         <v>126</v>
@@ -3831,11 +3882,11 @@
       </c>
       <c r="D57" s="34" t="str">
         <f>_xlfn.XLOOKUP(D56,table_listings!$B$2:$B$201,table_listings!$D$2:$D$201,,0)</f>
-        <v>Policy Year</v>
+        <v>Mix of Prj Year and Cal Year</v>
       </c>
       <c r="E57" s="34" t="str">
         <f>_xlfn.XLOOKUP(E56,table_listings!$B$2:$B$201,table_listings!$D$2:$D$201,,0)</f>
-        <v>Policy Year</v>
+        <v>Prj Year</v>
       </c>
       <c r="F57" s="13"/>
       <c r="G57" s="13"/>
@@ -3865,7 +3916,7 @@
       <c r="I58" s="13"/>
       <c r="J58" s="13"/>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A59" s="24" t="s">
         <v>132</v>
       </c>
@@ -4247,7 +4298,7 @@
       <c r="I75" s="12"/>
       <c r="J75" s="12"/>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A76" s="15" t="s">
         <v>131</v>
       </c>
@@ -4280,7 +4331,7 @@
         <v>136</v>
       </c>
       <c r="D77" s="12" t="s">
-        <v>126</v>
+        <v>231</v>
       </c>
       <c r="E77" s="12" t="s">
         <v>126</v>
@@ -4303,11 +4354,11 @@
       </c>
       <c r="D78" s="34" t="str">
         <f>_xlfn.XLOOKUP(D77,table_listings!$B$2:$B$201,table_listings!$D$2:$D$201,,0)</f>
-        <v>Policy Year</v>
+        <v>Mix of Prj Year and Cal Year</v>
       </c>
       <c r="E78" s="34" t="str">
         <f>_xlfn.XLOOKUP(E77,table_listings!$B$2:$B$201,table_listings!$D$2:$D$201,,0)</f>
-        <v>Policy Year</v>
+        <v>Prj Year</v>
       </c>
       <c r="F78" s="13"/>
       <c r="G78" s="13"/>
@@ -4337,7 +4388,7 @@
       <c r="I79" s="13"/>
       <c r="J79" s="13"/>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A80" s="15" t="s">
         <v>131</v>
       </c>
@@ -4454,6 +4505,14 @@
     <filterColumn colId="1">
       <filters>
         <filter val="disc_rate"/>
+        <filter val="invt_return"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="2">
+      <filters>
+        <filter val="Table"/>
+        <filter val="Table Column"/>
+        <filter val="Table Type"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -4494,7 +4553,7 @@
           <x14:formula1>
             <xm:f>table_listings!$B$142:$B$161</xm:f>
           </x14:formula1>
-          <xm:sqref>D28:E28 D77:E77 D56:E56 D32:E32</xm:sqref>
+          <xm:sqref>D28:E28 D56:E56 D32:E32 D77:E77</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{9147491E-BAE9-4A7D-A399-337FB5EBD658}">
           <x14:formula1>
@@ -4537,10 +4596,10 @@
   <dimension ref="A1:D201"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B74" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B122" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C114" sqref="C114"/>
+      <selection pane="bottomRight" activeCell="D142" sqref="D142:D144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6954,45 +7013,45 @@
       </c>
       <c r="C142" s="9" t="str">
         <f>[1]disc_rate!B2</f>
-        <v>Discount Rate Table</v>
+        <v>Policy Year Discount Rate Table</v>
       </c>
       <c r="D142" s="9" t="str">
         <f>[1]disc_rate!C2</f>
-        <v>Policy Year</v>
+        <v>Prj Year</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A143" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="B143" s="9">
+      <c r="B143" s="9" t="str">
         <f>[1]disc_rate!A3</f>
-        <v>0</v>
-      </c>
-      <c r="C143" s="9">
+        <v>DISCRT02</v>
+      </c>
+      <c r="C143" s="9" t="str">
         <f>[1]disc_rate!B3</f>
-        <v>0</v>
-      </c>
-      <c r="D143" s="9">
+        <v>Calendar Year Discount Rate Table</v>
+      </c>
+      <c r="D143" s="9" t="str">
         <f>[1]disc_rate!C3</f>
-        <v>0</v>
+        <v>Cal Year</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A144" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="B144" s="9">
+      <c r="B144" s="9" t="str">
         <f>[1]disc_rate!A4</f>
-        <v>0</v>
-      </c>
-      <c r="C144" s="9">
+        <v>DISCRT03</v>
+      </c>
+      <c r="C144" s="9" t="str">
         <f>[1]disc_rate!B4</f>
-        <v>0</v>
-      </c>
-      <c r="D144" s="9">
+        <v>CY: Invt Return and Disc Rate, PRJ_Y: Val Int Rate</v>
+      </c>
+      <c r="D144" s="9" t="str">
         <f>[1]disc_rate!C4</f>
-        <v>0</v>
+        <v>Mix of Prj Year and Cal Year</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.3">
@@ -7972,13 +8031,13 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9F298C4-02FF-4A34-A61E-BC2070858AEB}">
-  <dimension ref="A1:C68"/>
+  <dimension ref="A1:C69"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G29" sqref="G29"/>
+      <selection pane="bottomRight" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8025,18 +8084,18 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>12</v>
+        <v>230</v>
       </c>
       <c r="B4" t="s">
         <v>49</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="38" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B5" t="s">
         <v>49</v>
@@ -8047,7 +8106,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B6" t="s">
         <v>49</v>
@@ -8058,10 +8117,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>70</v>
+        <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>10</v>
@@ -8069,7 +8128,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="B8" t="s">
         <v>50</v>
@@ -8080,7 +8139,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="B9" t="s">
         <v>50</v>
@@ -8091,7 +8150,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B10" t="s">
         <v>50</v>
@@ -8102,7 +8161,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>0</v>
+        <v>76</v>
       </c>
       <c r="B11" t="s">
         <v>50</v>
@@ -8113,7 +8172,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B12" t="s">
         <v>50</v>
@@ -8124,7 +8183,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B13" t="s">
         <v>50</v>
@@ -8135,7 +8194,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B14" t="s">
         <v>50</v>
@@ -8146,7 +8205,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>72</v>
+        <v>3</v>
       </c>
       <c r="B15" t="s">
         <v>50</v>
@@ -8157,7 +8216,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B16" t="s">
         <v>50</v>
@@ -8168,7 +8227,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B17" t="s">
         <v>50</v>
@@ -8179,7 +8238,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B18" t="s">
         <v>50</v>
@@ -8190,7 +8249,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>4</v>
+        <v>74</v>
       </c>
       <c r="B19" t="s">
         <v>50</v>
@@ -8201,7 +8260,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>69</v>
+        <v>4</v>
       </c>
       <c r="B20" t="s">
         <v>50</v>
@@ -8212,18 +8271,18 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>15</v>
+        <v>69</v>
       </c>
       <c r="B21" t="s">
-        <v>51</v>
-      </c>
-      <c r="C21" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B22" t="s">
         <v>51</v>
@@ -8234,7 +8293,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B23" t="s">
         <v>51</v>
@@ -8245,7 +8304,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B24" t="s">
         <v>51</v>
@@ -8256,7 +8315,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B25" t="s">
         <v>51</v>
@@ -8267,7 +8326,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B26" t="s">
         <v>51</v>
@@ -8278,7 +8337,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B27" t="s">
         <v>51</v>
@@ -8289,7 +8348,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B28" t="s">
         <v>51</v>
@@ -8300,7 +8359,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B29" t="s">
         <v>51</v>
@@ -8311,18 +8370,18 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B30" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B31" t="s">
         <v>52</v>
@@ -8333,7 +8392,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B32" t="s">
         <v>52</v>
@@ -8344,7 +8403,7 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B33" t="s">
         <v>52</v>
@@ -8355,10 +8414,10 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B34" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>9</v>
@@ -8366,7 +8425,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B35" t="s">
         <v>53</v>
@@ -8377,7 +8436,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B36" t="s">
         <v>53</v>
@@ -8388,7 +8447,7 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B37" t="s">
         <v>53</v>
@@ -8399,7 +8458,7 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B38" t="s">
         <v>53</v>
@@ -8410,7 +8469,7 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B39" t="s">
         <v>53</v>
@@ -8421,7 +8480,7 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B40" t="s">
         <v>53</v>
@@ -8432,7 +8491,7 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B41" t="s">
         <v>53</v>
@@ -8443,7 +8502,7 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B42" t="s">
         <v>53</v>
@@ -8454,7 +8513,7 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
-        <v>55</v>
+        <v>36</v>
       </c>
       <c r="B43" t="s">
         <v>53</v>
@@ -8465,7 +8524,7 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B44" t="s">
         <v>53</v>
@@ -8476,7 +8535,7 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B45" t="s">
         <v>53</v>
@@ -8487,7 +8546,7 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B46" t="s">
         <v>53</v>
@@ -8498,7 +8557,7 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
-        <v>37</v>
+        <v>58</v>
       </c>
       <c r="B47" t="s">
         <v>53</v>
@@ -8509,7 +8568,7 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B48" t="s">
         <v>53</v>
@@ -8520,7 +8579,7 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
-        <v>59</v>
+        <v>38</v>
       </c>
       <c r="B49" t="s">
         <v>53</v>
@@ -8531,7 +8590,7 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B50" t="s">
         <v>53</v>
@@ -8542,7 +8601,7 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B51" t="s">
         <v>53</v>
@@ -8553,10 +8612,10 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
-        <v>39</v>
+        <v>61</v>
       </c>
       <c r="B52" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>9</v>
@@ -8564,7 +8623,7 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B53" t="s">
         <v>54</v>
@@ -8575,7 +8634,7 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B54" t="s">
         <v>54</v>
@@ -8586,7 +8645,7 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B55" t="s">
         <v>54</v>
@@ -8597,7 +8656,7 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B56" t="s">
         <v>54</v>
@@ -8608,7 +8667,7 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B57" t="s">
         <v>54</v>
@@ -8619,7 +8678,7 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B58" t="s">
         <v>54</v>
@@ -8630,7 +8689,7 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B59" t="s">
         <v>54</v>
@@ -8641,7 +8700,7 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B60" t="s">
         <v>54</v>
@@ -8652,7 +8711,7 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="B61" t="s">
         <v>54</v>
@@ -8663,7 +8722,7 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B62" t="s">
         <v>54</v>
@@ -8674,7 +8733,7 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B63" t="s">
         <v>54</v>
@@ -8685,7 +8744,7 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B64" t="s">
         <v>54</v>
@@ -8696,7 +8755,7 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
-        <v>48</v>
+        <v>65</v>
       </c>
       <c r="B65" t="s">
         <v>54</v>
@@ -8707,7 +8766,7 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="B66" t="s">
         <v>54</v>
@@ -8718,7 +8777,7 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B67" t="s">
         <v>54</v>
@@ -8729,12 +8788,23 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B68" t="s">
         <v>54</v>
       </c>
       <c r="C68" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A69" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B69" t="s">
+        <v>54</v>
+      </c>
+      <c r="C69" s="2" t="s">
         <v>9</v>
       </c>
     </row>
@@ -8745,10 +8815,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA1111D6-CFD5-472E-AAF0-AF6E36C438B2}">
-  <dimension ref="B1:F41"/>
+  <dimension ref="B1:F46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8912,7 +8982,7 @@
       <c r="B13" t="s">
         <v>117</v>
       </c>
-      <c r="C13" s="38" t="s">
+      <c r="C13" t="s">
         <v>226</v>
       </c>
       <c r="D13" t="s">
@@ -8923,7 +8993,7 @@
       <c r="B14" t="s">
         <v>117</v>
       </c>
-      <c r="C14" s="38" t="s">
+      <c r="C14" t="s">
         <v>213</v>
       </c>
       <c r="D14" t="s">
@@ -8934,7 +9004,7 @@
       <c r="B15" t="s">
         <v>117</v>
       </c>
-      <c r="C15" s="38" t="s">
+      <c r="C15" t="s">
         <v>214</v>
       </c>
       <c r="D15" t="s">
@@ -8945,7 +9015,7 @@
       <c r="B16" t="s">
         <v>117</v>
       </c>
-      <c r="C16" s="38" t="s">
+      <c r="C16" t="s">
         <v>227</v>
       </c>
       <c r="D16" t="s">
@@ -8956,7 +9026,7 @@
       <c r="B17" t="s">
         <v>117</v>
       </c>
-      <c r="C17" s="38" t="s">
+      <c r="C17" t="s">
         <v>228</v>
       </c>
       <c r="D17" t="s">
@@ -8967,7 +9037,7 @@
       <c r="B18" t="s">
         <v>117</v>
       </c>
-      <c r="C18" s="38" t="s">
+      <c r="C18" t="s">
         <v>229</v>
       </c>
       <c r="D18" t="s">
@@ -9019,88 +9089,151 @@
       <c r="B23" t="s">
         <v>119</v>
       </c>
+      <c r="C23" t="s">
+        <v>236</v>
+      </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>112</v>
       </c>
+      <c r="C24" t="s">
+        <v>232</v>
+      </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
-        <v>120</v>
+        <v>112</v>
+      </c>
+      <c r="C25" t="s">
+        <v>233</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
-        <v>121</v>
+        <v>112</v>
+      </c>
+      <c r="C26" t="s">
+        <v>234</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
-        <v>122</v>
+        <v>120</v>
+      </c>
+      <c r="C27" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B28" t="s">
+        <v>120</v>
+      </c>
+      <c r="C28" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B29" t="s">
+        <v>120</v>
+      </c>
+      <c r="C29" t="s">
+        <v>234</v>
       </c>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B30" s="36" t="s">
-        <v>179</v>
-      </c>
-      <c r="C30" s="36" t="s">
-        <v>211</v>
-      </c>
-      <c r="D30" s="36"/>
+      <c r="B30" t="s">
+        <v>121</v>
+      </c>
+      <c r="C30" t="s">
+        <v>235</v>
+      </c>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
-        <v>180</v>
+        <v>121</v>
+      </c>
+      <c r="C31" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
+        <v>122</v>
+      </c>
+      <c r="C32" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B33" t="s">
+        <v>122</v>
+      </c>
+      <c r="C33" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B35" s="36" t="s">
+        <v>179</v>
+      </c>
+      <c r="C35" s="36" t="s">
+        <v>211</v>
+      </c>
+      <c r="D35" s="36"/>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B36" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B37" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B33" t="s">
+    <row r="38" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B38" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B34" t="s">
+    <row r="39" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B39" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B35" t="s">
+    <row r="40" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B40" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B36" t="s">
+    <row r="41" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B41" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B37" t="s">
+    <row r="42" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B42" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B38" t="s">
+    <row r="43" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B43" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B39" t="s">
+    <row r="44" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B44" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B40" t="s">
+    <row r="45" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B45" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B41" t="s">
+    <row r="46" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B46" t="s">
         <v>186</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add new table types for prem tax and tax
</commit_message>
<xml_diff>
--- a/Input/Settings.xlsx
+++ b/Input/Settings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Julia\TradLifeModel\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71BDB82F-966C-46B2-8987-74033DC86EEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F407EDF-4683-4738-AB26-56557784BFA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="889" activeTab="5" xr2:uid="{ADF8BBD9-0F7A-45CB-8EA8-A3D46B124E82}"/>
   </bookViews>
@@ -24,7 +24,7 @@
     <externalReference r:id="rId7"/>
   </externalReferences>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">product_setup!$A$1:$C$84</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">product_setup!$A$1:$C$80</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">table_listings!$A$1:$D$201</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="898" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="882" uniqueCount="242">
   <si>
     <t>acq_exp_per_pol</t>
   </si>
@@ -757,6 +757,33 @@
   </si>
   <si>
     <t>Per Policy and Perc of Premium by Policy Year</t>
+  </si>
+  <si>
+    <t>PREMTAX02</t>
+  </si>
+  <si>
+    <t>TAX02</t>
+  </si>
+  <si>
+    <t>Age setback</t>
+  </si>
+  <si>
+    <t>Pol Year</t>
+  </si>
+  <si>
+    <r>
+      <t>Mix of Prj Year or Cal Year</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> or Pol Year</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -979,9 +1006,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1002,6 +1026,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1071,8 +1096,10 @@
       <sheetName val="DISCRT03"/>
       <sheetName val="prem_tax"/>
       <sheetName val="PREMTAX01"/>
+      <sheetName val="PREMTAX02"/>
       <sheetName val="tax"/>
       <sheetName val="TAX01"/>
+      <sheetName val="TAX02"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
@@ -1110,9 +1137,9 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
       <sheetData sheetId="4">
         <row r="2">
           <cell r="A2" t="str">
@@ -1137,8 +1164,8 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
+      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="6" refreshError="1"/>
       <sheetData sheetId="7">
         <row r="2">
           <cell r="A2" t="str">
@@ -1174,9 +1201,9 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
+      <sheetData sheetId="8" refreshError="1"/>
+      <sheetData sheetId="9" refreshError="1"/>
+      <sheetData sheetId="10" refreshError="1"/>
       <sheetData sheetId="11">
         <row r="2">
           <cell r="A2" t="str">
@@ -1212,9 +1239,9 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="12"/>
-      <sheetData sheetId="13"/>
-      <sheetData sheetId="14"/>
+      <sheetData sheetId="12" refreshError="1"/>
+      <sheetData sheetId="13" refreshError="1"/>
+      <sheetData sheetId="14" refreshError="1"/>
       <sheetData sheetId="15">
         <row r="2">
           <cell r="A2" t="str">
@@ -1305,14 +1332,14 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="16"/>
-      <sheetData sheetId="17"/>
-      <sheetData sheetId="18"/>
-      <sheetData sheetId="19"/>
-      <sheetData sheetId="20"/>
-      <sheetData sheetId="21"/>
-      <sheetData sheetId="22"/>
-      <sheetData sheetId="23"/>
+      <sheetData sheetId="16" refreshError="1"/>
+      <sheetData sheetId="17" refreshError="1"/>
+      <sheetData sheetId="18" refreshError="1"/>
+      <sheetData sheetId="19" refreshError="1"/>
+      <sheetData sheetId="20" refreshError="1"/>
+      <sheetData sheetId="21" refreshError="1"/>
+      <sheetData sheetId="22" refreshError="1"/>
+      <sheetData sheetId="23" refreshError="1"/>
       <sheetData sheetId="24">
         <row r="2">
           <cell r="A2" t="str">
@@ -1337,8 +1364,8 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="25"/>
-      <sheetData sheetId="26"/>
+      <sheetData sheetId="25" refreshError="1"/>
+      <sheetData sheetId="26" refreshError="1"/>
       <sheetData sheetId="27">
         <row r="2">
           <cell r="A2" t="str">
@@ -1352,7 +1379,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="28"/>
+      <sheetData sheetId="28" refreshError="1"/>
       <sheetData sheetId="29">
         <row r="2">
           <cell r="A2" t="str">
@@ -1388,9 +1415,9 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="30"/>
-      <sheetData sheetId="31"/>
-      <sheetData sheetId="32"/>
+      <sheetData sheetId="30" refreshError="1"/>
+      <sheetData sheetId="31" refreshError="1"/>
+      <sheetData sheetId="32" refreshError="1"/>
       <sheetData sheetId="33">
         <row r="2">
           <cell r="A2" t="str">
@@ -1400,12 +1427,24 @@
             <v>Premium Tax Rate</v>
           </cell>
           <cell r="C2" t="str">
+            <v>Scalar</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="A3" t="str">
+            <v>PREMTAX02</v>
+          </cell>
+          <cell r="B3" t="str">
+            <v>Premium Tax Rate Table</v>
+          </cell>
+          <cell r="C3" t="str">
             <v>Policy Year</v>
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="34"/>
-      <sheetData sheetId="35">
+      <sheetData sheetId="34" refreshError="1"/>
+      <sheetData sheetId="35" refreshError="1"/>
+      <sheetData sheetId="36">
         <row r="2">
           <cell r="A2" t="str">
             <v>TAX01</v>
@@ -1414,11 +1453,23 @@
             <v>Tax Rate</v>
           </cell>
           <cell r="C2" t="str">
+            <v>Scalar</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="A3" t="str">
+            <v>TAX02</v>
+          </cell>
+          <cell r="B3" t="str">
+            <v>Tax Rate Table</v>
+          </cell>
+          <cell r="C3" t="str">
             <v>Policy Year</v>
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="36"/>
+      <sheetData sheetId="37" refreshError="1"/>
+      <sheetData sheetId="38" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1745,7 +1796,7 @@
       <c r="A2" t="s">
         <v>168</v>
       </c>
-      <c r="B2" s="33">
+      <c r="B2" s="32">
         <v>44561</v>
       </c>
     </row>
@@ -2609,13 +2660,13 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1E729B3-29BA-40F1-80D4-2208DEC4BA85}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:J84"/>
+  <dimension ref="A1:J80"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D77" sqref="D77"/>
+      <selection pane="bottomRight" activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2700,11 +2751,11 @@
       <c r="C4" t="s">
         <v>110</v>
       </c>
-      <c r="D4" s="34" t="str">
+      <c r="D4" s="33" t="str">
         <f>_xlfn.XLOOKUP(D3,table_listings!$B$2:$B$201,table_listings!$D$2:$D$201,,0)</f>
         <v>Rate per 1000 SA by Issue Age/Pol Term/Prem Term</v>
       </c>
-      <c r="E4" s="34" t="str">
+      <c r="E4" s="33" t="str">
         <f>_xlfn.XLOOKUP(E3,table_listings!$B$2:$B$201,table_listings!$D$2:$D$201,,0)</f>
         <v>Rate per 1000 SA by Age/Pol Term</v>
       </c>
@@ -2786,11 +2837,11 @@
       <c r="C8" s="19" t="s">
         <v>110</v>
       </c>
-      <c r="D8" s="34" t="str">
+      <c r="D8" s="33" t="str">
         <f>_xlfn.XLOOKUP(D7,table_listings!$B$2:$B$201,table_listings!$D$2:$D$201,,0)</f>
         <v>Mult to MP SA by Duration</v>
       </c>
-      <c r="E8" s="34" t="str">
+      <c r="E8" s="33" t="str">
         <f>_xlfn.XLOOKUP(E7,table_listings!$B$2:$B$201,table_listings!$D$2:$D$201,,0)</f>
         <v>User Defined Table</v>
       </c>
@@ -2874,11 +2925,11 @@
       <c r="C12" s="25" t="s">
         <v>110</v>
       </c>
-      <c r="D12" s="34" t="str">
+      <c r="D12" s="33" t="str">
         <f>_xlfn.XLOOKUP(D11,table_listings!$B$2:$B$201,table_listings!$D$2:$D$201,,0)</f>
         <v>Rate per 1000 SA by Pol Year/Issue Age/Prem Term</v>
       </c>
-      <c r="E12" s="34" t="str">
+      <c r="E12" s="33" t="str">
         <f>_xlfn.XLOOKUP(E11,table_listings!$B$2:$B$201,table_listings!$D$2:$D$201,,0)</f>
         <v>Rate per 1000 SA by Year/Age</v>
       </c>
@@ -2960,11 +3011,11 @@
       <c r="C16" s="19" t="s">
         <v>110</v>
       </c>
-      <c r="D16" s="34" t="str">
+      <c r="D16" s="33" t="str">
         <f>_xlfn.XLOOKUP(D15,table_listings!$B$2:$B$201,table_listings!$D$2:$D$201,,0)</f>
         <v>Perc by Pol Year/Pol Term</v>
       </c>
-      <c r="E16" s="34" t="str">
+      <c r="E16" s="33" t="str">
         <f>_xlfn.XLOOKUP(E15,table_listings!$B$2:$B$201,table_listings!$D$2:$D$201,,0)</f>
         <v>Perc by Pol Year/Pol Term</v>
       </c>
@@ -3046,11 +3097,11 @@
       <c r="C20" s="25" t="s">
         <v>110</v>
       </c>
-      <c r="D20" s="34" t="str">
+      <c r="D20" s="33" t="str">
         <f>_xlfn.XLOOKUP(D19,table_listings!$B$2:$B$201,table_listings!$D$2:$D$201,,0)</f>
         <v>Select and Ultimate - Sex Distinct</v>
       </c>
-      <c r="E20" s="34" t="str">
+      <c r="E20" s="33" t="str">
         <f>_xlfn.XLOOKUP(E19,table_listings!$B$2:$B$201,table_listings!$D$2:$D$201,,0)</f>
         <v>Attained Age</v>
       </c>
@@ -3114,11 +3165,11 @@
       <c r="C23" s="19" t="s">
         <v>110</v>
       </c>
-      <c r="D23" s="34" t="str">
+      <c r="D23" s="33" t="str">
         <f>_xlfn.XLOOKUP(D22,table_listings!$B$2:$B$201,table_listings!$D$2:$D$201,,0)</f>
         <v>Pol Year/Pol Term/Prem Term</v>
       </c>
-      <c r="E23" s="34" t="str">
+      <c r="E23" s="33" t="str">
         <f>_xlfn.XLOOKUP(E22,table_listings!$B$2:$B$201,table_listings!$D$2:$D$201,,0)</f>
         <v>Pol Year/Pol Term</v>
       </c>
@@ -3182,11 +3233,11 @@
       <c r="C26" s="25" t="s">
         <v>110</v>
       </c>
-      <c r="D26" s="34" t="str">
+      <c r="D26" s="33" t="str">
         <f>_xlfn.XLOOKUP(D25,table_listings!$B$2:$B$201,table_listings!$D$2:$D$201,,0)</f>
         <v>Policy Year</v>
       </c>
-      <c r="E26" s="34" t="str">
+      <c r="E26" s="33" t="str">
         <f>_xlfn.XLOOKUP(E25,table_listings!$B$2:$B$201,table_listings!$D$2:$D$201,,0)</f>
         <v>Policy Year</v>
       </c>
@@ -3218,7 +3269,7 @@
       <c r="I27" s="13"/>
       <c r="J27" s="13"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28" s="15" t="s">
         <v>133</v>
       </c>
@@ -3240,7 +3291,7 @@
       <c r="I28" s="12"/>
       <c r="J28" s="12"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29" s="15" t="s">
         <v>133</v>
       </c>
@@ -3250,11 +3301,11 @@
       <c r="C29" s="19" t="s">
         <v>110</v>
       </c>
-      <c r="D29" s="34" t="str">
+      <c r="D29" s="33" t="str">
         <f>_xlfn.XLOOKUP(D28,table_listings!$B$2:$B$201,table_listings!$D$2:$D$201,,0)</f>
         <v>Mix of Prj Year and Cal Year</v>
       </c>
-      <c r="E29" s="34" t="str">
+      <c r="E29" s="33" t="str">
         <f>_xlfn.XLOOKUP(E28,table_listings!$B$2:$B$201,table_listings!$D$2:$D$201,,0)</f>
         <v>Prj Year</v>
       </c>
@@ -3264,7 +3315,7 @@
       <c r="I29" s="13"/>
       <c r="J29" s="13"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30" s="15" t="s">
         <v>133</v>
       </c>
@@ -3308,7 +3359,7 @@
       <c r="I31" s="13"/>
       <c r="J31" s="13"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A32" s="24" t="s">
         <v>133</v>
       </c>
@@ -3330,7 +3381,7 @@
       <c r="I32" s="12"/>
       <c r="J32" s="12"/>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33" s="24" t="s">
         <v>133</v>
       </c>
@@ -3340,11 +3391,11 @@
       <c r="C33" s="25" t="s">
         <v>110</v>
       </c>
-      <c r="D33" s="34" t="str">
+      <c r="D33" s="33" t="str">
         <f>_xlfn.XLOOKUP(D32,table_listings!$B$2:$B$201,table_listings!$D$2:$D$201,,0)</f>
         <v>Mix of Prj Year and Cal Year</v>
       </c>
-      <c r="E33" s="34" t="str">
+      <c r="E33" s="33" t="str">
         <f>_xlfn.XLOOKUP(E32,table_listings!$B$2:$B$201,table_listings!$D$2:$D$201,,0)</f>
         <v>Prj Year</v>
       </c>
@@ -3354,7 +3405,7 @@
       <c r="I33" s="13"/>
       <c r="J33" s="13"/>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34" s="24" t="s">
         <v>133</v>
       </c>
@@ -3376,7 +3427,7 @@
       <c r="I34" s="12"/>
       <c r="J34" s="12"/>
     </row>
-    <row r="35" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" s="15" t="s">
         <v>133</v>
       </c>
@@ -3398,7 +3449,7 @@
       <c r="I35" s="13"/>
       <c r="J35" s="13"/>
     </row>
-    <row r="36" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" s="15" t="s">
         <v>133</v>
       </c>
@@ -3409,7 +3460,7 @@
         <v>136</v>
       </c>
       <c r="D36" s="12" t="s">
-        <v>127</v>
+        <v>237</v>
       </c>
       <c r="E36" s="12" t="s">
         <v>127</v>
@@ -3420,7 +3471,7 @@
       <c r="I36" s="12"/>
       <c r="J36" s="12"/>
     </row>
-    <row r="37" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37" s="15" t="s">
         <v>133</v>
       </c>
@@ -3430,13 +3481,13 @@
       <c r="C37" s="19" t="s">
         <v>110</v>
       </c>
-      <c r="D37" s="34" t="str">
+      <c r="D37" s="33" t="str">
         <f>_xlfn.XLOOKUP(D36,table_listings!$B$2:$B$201,table_listings!$D$2:$D$201,,0)</f>
         <v>Policy Year</v>
       </c>
-      <c r="E37" s="34" t="str">
+      <c r="E37" s="33" t="str">
         <f>_xlfn.XLOOKUP(E36,table_listings!$B$2:$B$201,table_listings!$D$2:$D$201,,0)</f>
-        <v>Policy Year</v>
+        <v>Scalar</v>
       </c>
       <c r="F37" s="13"/>
       <c r="G37" s="13"/>
@@ -3444,29 +3495,29 @@
       <c r="I37" s="13"/>
       <c r="J37" s="13"/>
     </row>
-    <row r="38" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="15" t="s">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A38" s="24" t="s">
         <v>133</v>
       </c>
-      <c r="B38" s="16" t="s">
-        <v>121</v>
-      </c>
-      <c r="C38" s="19" t="s">
-        <v>135</v>
-      </c>
-      <c r="D38" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="E38" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="F38" s="12"/>
-      <c r="G38" s="12"/>
-      <c r="H38" s="12"/>
-      <c r="I38" s="12"/>
-      <c r="J38" s="12"/>
-    </row>
-    <row r="39" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="B38" t="s">
+        <v>122</v>
+      </c>
+      <c r="C38" s="25" t="s">
+        <v>137</v>
+      </c>
+      <c r="D38" s="13">
+        <v>1</v>
+      </c>
+      <c r="E38" s="13">
+        <v>1</v>
+      </c>
+      <c r="F38" s="13"/>
+      <c r="G38" s="13"/>
+      <c r="H38" s="13"/>
+      <c r="I38" s="13"/>
+      <c r="J38" s="13"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" s="24" t="s">
         <v>133</v>
       </c>
@@ -3474,13 +3525,13 @@
         <v>122</v>
       </c>
       <c r="C39" s="25" t="s">
-        <v>137</v>
-      </c>
-      <c r="D39" s="13">
-        <v>1</v>
-      </c>
-      <c r="E39" s="13">
-        <v>1</v>
+        <v>136</v>
+      </c>
+      <c r="D39" s="12" t="s">
+        <v>238</v>
+      </c>
+      <c r="E39" s="12" t="s">
+        <v>128</v>
       </c>
       <c r="F39" s="13"/>
       <c r="G39" s="13"/>
@@ -3488,7 +3539,7 @@
       <c r="I39" s="13"/>
       <c r="J39" s="13"/>
     </row>
-    <row r="40" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" s="24" t="s">
         <v>133</v>
       </c>
@@ -3496,13 +3547,15 @@
         <v>122</v>
       </c>
       <c r="C40" s="25" t="s">
-        <v>136</v>
-      </c>
-      <c r="D40" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="E40" s="12" t="s">
-        <v>128</v>
+        <v>110</v>
+      </c>
+      <c r="D40" s="33" t="str">
+        <f>_xlfn.XLOOKUP(D39,table_listings!$B$2:$B$201,table_listings!$D$2:$D$201,,0)</f>
+        <v>Policy Year</v>
+      </c>
+      <c r="E40" s="33" t="str">
+        <f>_xlfn.XLOOKUP(E39,table_listings!$B$2:$B$201,table_listings!$D$2:$D$201,,0)</f>
+        <v>Scalar</v>
       </c>
       <c r="F40" s="13"/>
       <c r="G40" s="13"/>
@@ -3511,22 +3564,20 @@
       <c r="J40" s="13"/>
     </row>
     <row r="41" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="24" t="s">
-        <v>133</v>
-      </c>
-      <c r="B41" t="s">
-        <v>122</v>
-      </c>
-      <c r="C41" s="25" t="s">
-        <v>110</v>
-      </c>
-      <c r="D41" s="34" t="str">
-        <f>_xlfn.XLOOKUP(D40,table_listings!$B$2:$B$201,table_listings!$D$2:$D$201,,0)</f>
-        <v>Policy Year</v>
-      </c>
-      <c r="E41" s="34" t="str">
-        <f>_xlfn.XLOOKUP(E40,table_listings!$B$2:$B$201,table_listings!$D$2:$D$201,,0)</f>
-        <v>Policy Year</v>
+      <c r="A41" s="17" t="s">
+        <v>132</v>
+      </c>
+      <c r="B41" s="18" t="s">
+        <v>117</v>
+      </c>
+      <c r="C41" s="20" t="s">
+        <v>137</v>
+      </c>
+      <c r="D41" s="13">
+        <v>1</v>
+      </c>
+      <c r="E41" s="13">
+        <v>0.8</v>
       </c>
       <c r="F41" s="13"/>
       <c r="G41" s="13"/>
@@ -3535,20 +3586,20 @@
       <c r="J41" s="13"/>
     </row>
     <row r="42" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="24" t="s">
-        <v>133</v>
-      </c>
-      <c r="B42" t="s">
-        <v>122</v>
-      </c>
-      <c r="C42" s="25" t="s">
-        <v>135</v>
-      </c>
-      <c r="D42" s="26" t="s">
-        <v>69</v>
-      </c>
-      <c r="E42" s="26" t="s">
-        <v>69</v>
+      <c r="A42" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="B42" s="16" t="s">
+        <v>117</v>
+      </c>
+      <c r="C42" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="D42" s="12" t="s">
+        <v>225</v>
+      </c>
+      <c r="E42" s="12" t="s">
+        <v>109</v>
       </c>
       <c r="F42" s="12"/>
       <c r="G42" s="12"/>
@@ -3557,20 +3608,22 @@
       <c r="J42" s="12"/>
     </row>
     <row r="43" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="17" t="s">
+      <c r="A43" s="15" t="s">
         <v>132</v>
       </c>
-      <c r="B43" s="18" t="s">
+      <c r="B43" s="16" t="s">
         <v>117</v>
       </c>
-      <c r="C43" s="20" t="s">
-        <v>137</v>
-      </c>
-      <c r="D43" s="13">
-        <v>1</v>
-      </c>
-      <c r="E43" s="13">
-        <v>0.8</v>
+      <c r="C43" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="D43" s="33" t="str">
+        <f>_xlfn.XLOOKUP(D42,table_listings!$B$2:$B$201,table_listings!$D$2:$D$201,,0)</f>
+        <v>Select and Ultimate - Sex Distinct</v>
+      </c>
+      <c r="E43" s="33" t="str">
+        <f>_xlfn.XLOOKUP(E42,table_listings!$B$2:$B$201,table_listings!$D$2:$D$201,,0)</f>
+        <v>Attained Age</v>
       </c>
       <c r="F43" s="13"/>
       <c r="G43" s="13"/>
@@ -3586,13 +3639,13 @@
         <v>117</v>
       </c>
       <c r="C44" s="19" t="s">
-        <v>136</v>
-      </c>
-      <c r="D44" s="12" t="s">
-        <v>225</v>
-      </c>
-      <c r="E44" s="12" t="s">
-        <v>109</v>
+        <v>134</v>
+      </c>
+      <c r="D44" s="12">
+        <v>0.1</v>
+      </c>
+      <c r="E44" s="12">
+        <v>0.1</v>
       </c>
       <c r="F44" s="12"/>
       <c r="G44" s="12"/>
@@ -3601,22 +3654,20 @@
       <c r="J44" s="12"/>
     </row>
     <row r="45" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="15" t="s">
+      <c r="A45" s="24" t="s">
         <v>132</v>
       </c>
-      <c r="B45" s="16" t="s">
-        <v>117</v>
-      </c>
-      <c r="C45" s="19" t="s">
-        <v>110</v>
-      </c>
-      <c r="D45" s="34" t="str">
-        <f>_xlfn.XLOOKUP(D44,table_listings!$B$2:$B$201,table_listings!$D$2:$D$201,,0)</f>
-        <v>Select and Ultimate - Sex Distinct</v>
-      </c>
-      <c r="E45" s="34" t="str">
-        <f>_xlfn.XLOOKUP(E44,table_listings!$B$2:$B$201,table_listings!$D$2:$D$201,,0)</f>
-        <v>Attained Age</v>
+      <c r="B45" t="s">
+        <v>118</v>
+      </c>
+      <c r="C45" s="25" t="s">
+        <v>137</v>
+      </c>
+      <c r="D45" s="13">
+        <v>1</v>
+      </c>
+      <c r="E45" s="13">
+        <v>1</v>
       </c>
       <c r="F45" s="13"/>
       <c r="G45" s="13"/>
@@ -3625,20 +3676,20 @@
       <c r="J45" s="13"/>
     </row>
     <row r="46" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="15" t="s">
+      <c r="A46" s="24" t="s">
         <v>132</v>
       </c>
-      <c r="B46" s="16" t="s">
-        <v>117</v>
-      </c>
-      <c r="C46" s="19" t="s">
-        <v>134</v>
-      </c>
-      <c r="D46" s="12">
-        <v>0.1</v>
-      </c>
-      <c r="E46" s="12">
-        <v>0.1</v>
+      <c r="B46" t="s">
+        <v>118</v>
+      </c>
+      <c r="C46" s="25" t="s">
+        <v>136</v>
+      </c>
+      <c r="D46" s="12" t="s">
+        <v>222</v>
+      </c>
+      <c r="E46" s="12" t="s">
+        <v>123</v>
       </c>
       <c r="F46" s="12"/>
       <c r="G46" s="12"/>
@@ -3654,13 +3705,15 @@
         <v>118</v>
       </c>
       <c r="C47" s="25" t="s">
-        <v>137</v>
-      </c>
-      <c r="D47" s="13">
-        <v>1</v>
-      </c>
-      <c r="E47" s="13">
-        <v>1</v>
+        <v>110</v>
+      </c>
+      <c r="D47" s="33" t="str">
+        <f>_xlfn.XLOOKUP(D46,table_listings!$B$2:$B$201,table_listings!$D$2:$D$201,,0)</f>
+        <v>Pol Year/Pol Term/Prem Term</v>
+      </c>
+      <c r="E47" s="33" t="str">
+        <f>_xlfn.XLOOKUP(E46,table_listings!$B$2:$B$201,table_listings!$D$2:$D$201,,0)</f>
+        <v>Pol Year/Pol Term</v>
       </c>
       <c r="F47" s="13"/>
       <c r="G47" s="13"/>
@@ -3676,13 +3729,13 @@
         <v>118</v>
       </c>
       <c r="C48" s="25" t="s">
-        <v>136</v>
-      </c>
-      <c r="D48" s="12" t="s">
-        <v>222</v>
-      </c>
-      <c r="E48" s="12" t="s">
-        <v>123</v>
+        <v>134</v>
+      </c>
+      <c r="D48" s="36">
+        <v>0.2</v>
+      </c>
+      <c r="E48" s="36">
+        <v>0.2</v>
       </c>
       <c r="F48" s="12"/>
       <c r="G48" s="12"/>
@@ -3691,22 +3744,20 @@
       <c r="J48" s="12"/>
     </row>
     <row r="49" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="24" t="s">
+      <c r="A49" s="15" t="s">
         <v>132</v>
       </c>
-      <c r="B49" t="s">
-        <v>118</v>
-      </c>
-      <c r="C49" s="25" t="s">
-        <v>110</v>
-      </c>
-      <c r="D49" s="34" t="str">
-        <f>_xlfn.XLOOKUP(D48,table_listings!$B$2:$B$201,table_listings!$D$2:$D$201,,0)</f>
-        <v>Pol Year/Pol Term/Prem Term</v>
-      </c>
-      <c r="E49" s="34" t="str">
-        <f>_xlfn.XLOOKUP(E48,table_listings!$B$2:$B$201,table_listings!$D$2:$D$201,,0)</f>
-        <v>Pol Year/Pol Term</v>
+      <c r="B49" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="C49" s="19" t="s">
+        <v>137</v>
+      </c>
+      <c r="D49" s="13">
+        <v>1</v>
+      </c>
+      <c r="E49" s="13">
+        <v>1</v>
       </c>
       <c r="F49" s="13"/>
       <c r="G49" s="13"/>
@@ -3715,20 +3766,20 @@
       <c r="J49" s="13"/>
     </row>
     <row r="50" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="24" t="s">
+      <c r="A50" s="15" t="s">
         <v>132</v>
       </c>
-      <c r="B50" t="s">
-        <v>118</v>
-      </c>
-      <c r="C50" s="25" t="s">
-        <v>134</v>
-      </c>
-      <c r="D50" s="37">
-        <v>0.2</v>
-      </c>
-      <c r="E50" s="37">
-        <v>0.2</v>
+      <c r="B50" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="C50" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="D50" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="E50" s="12" t="s">
+        <v>125</v>
       </c>
       <c r="F50" s="12"/>
       <c r="G50" s="12"/>
@@ -3744,13 +3795,15 @@
         <v>119</v>
       </c>
       <c r="C51" s="19" t="s">
-        <v>137</v>
-      </c>
-      <c r="D51" s="13">
-        <v>1</v>
-      </c>
-      <c r="E51" s="13">
-        <v>1</v>
+        <v>110</v>
+      </c>
+      <c r="D51" s="33" t="str">
+        <f>_xlfn.XLOOKUP(D50,table_listings!$B$2:$B$201,table_listings!$D$2:$D$201,,0)</f>
+        <v>Policy Year</v>
+      </c>
+      <c r="E51" s="33" t="str">
+        <f>_xlfn.XLOOKUP(E50,table_listings!$B$2:$B$201,table_listings!$D$2:$D$201,,0)</f>
+        <v>Policy Year</v>
       </c>
       <c r="F51" s="13"/>
       <c r="G51" s="13"/>
@@ -3766,13 +3819,13 @@
         <v>119</v>
       </c>
       <c r="C52" s="19" t="s">
-        <v>136</v>
-      </c>
-      <c r="D52" s="12" t="s">
-        <v>125</v>
-      </c>
-      <c r="E52" s="12" t="s">
-        <v>125</v>
+        <v>134</v>
+      </c>
+      <c r="D52" s="12">
+        <v>0.1</v>
+      </c>
+      <c r="E52" s="12">
+        <v>0.1</v>
       </c>
       <c r="F52" s="12"/>
       <c r="G52" s="12"/>
@@ -3781,22 +3834,20 @@
       <c r="J52" s="12"/>
     </row>
     <row r="53" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="15" t="s">
+      <c r="A53" s="24" t="s">
         <v>132</v>
       </c>
-      <c r="B53" s="16" t="s">
-        <v>119</v>
-      </c>
-      <c r="C53" s="19" t="s">
-        <v>110</v>
-      </c>
-      <c r="D53" s="34" t="str">
-        <f>_xlfn.XLOOKUP(D52,table_listings!$B$2:$B$201,table_listings!$D$2:$D$201,,0)</f>
-        <v>Policy Year</v>
-      </c>
-      <c r="E53" s="34" t="str">
-        <f>_xlfn.XLOOKUP(E52,table_listings!$B$2:$B$201,table_listings!$D$2:$D$201,,0)</f>
-        <v>Policy Year</v>
+      <c r="B53" t="s">
+        <v>112</v>
+      </c>
+      <c r="C53" s="25" t="s">
+        <v>137</v>
+      </c>
+      <c r="D53" s="13">
+        <v>1</v>
+      </c>
+      <c r="E53" s="13">
+        <v>1</v>
       </c>
       <c r="F53" s="13"/>
       <c r="G53" s="13"/>
@@ -3805,20 +3856,20 @@
       <c r="J53" s="13"/>
     </row>
     <row r="54" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="15" t="s">
+      <c r="A54" s="24" t="s">
         <v>132</v>
       </c>
-      <c r="B54" s="16" t="s">
-        <v>119</v>
-      </c>
-      <c r="C54" s="19" t="s">
-        <v>134</v>
-      </c>
-      <c r="D54" s="12">
-        <v>0.1</v>
-      </c>
-      <c r="E54" s="12">
-        <v>0.1</v>
+      <c r="B54" t="s">
+        <v>112</v>
+      </c>
+      <c r="C54" s="25" t="s">
+        <v>136</v>
+      </c>
+      <c r="D54" s="12" t="s">
+        <v>231</v>
+      </c>
+      <c r="E54" s="12" t="s">
+        <v>126</v>
       </c>
       <c r="F54" s="12"/>
       <c r="G54" s="12"/>
@@ -3834,13 +3885,15 @@
         <v>112</v>
       </c>
       <c r="C55" s="25" t="s">
-        <v>137</v>
-      </c>
-      <c r="D55" s="13">
-        <v>1</v>
-      </c>
-      <c r="E55" s="13">
-        <v>1</v>
+        <v>110</v>
+      </c>
+      <c r="D55" s="33" t="str">
+        <f>_xlfn.XLOOKUP(D54,table_listings!$B$2:$B$201,table_listings!$D$2:$D$201,,0)</f>
+        <v>Mix of Prj Year and Cal Year</v>
+      </c>
+      <c r="E55" s="33" t="str">
+        <f>_xlfn.XLOOKUP(E54,table_listings!$B$2:$B$201,table_listings!$D$2:$D$201,,0)</f>
+        <v>Prj Year</v>
       </c>
       <c r="F55" s="13"/>
       <c r="G55" s="13"/>
@@ -3848,7 +3901,7 @@
       <c r="I55" s="13"/>
       <c r="J55" s="13"/>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A56" s="24" t="s">
         <v>132</v>
       </c>
@@ -3856,21 +3909,21 @@
         <v>112</v>
       </c>
       <c r="C56" s="25" t="s">
-        <v>136</v>
-      </c>
-      <c r="D56" s="12" t="s">
-        <v>231</v>
-      </c>
-      <c r="E56" s="12" t="s">
-        <v>126</v>
-      </c>
-      <c r="F56" s="12"/>
-      <c r="G56" s="12"/>
-      <c r="H56" s="12"/>
-      <c r="I56" s="12"/>
-      <c r="J56" s="12"/>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
+        <v>135</v>
+      </c>
+      <c r="D56" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="E56" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="F56" s="13"/>
+      <c r="G56" s="13"/>
+      <c r="H56" s="13"/>
+      <c r="I56" s="13"/>
+      <c r="J56" s="13"/>
+    </row>
+    <row r="57" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A57" s="24" t="s">
         <v>132</v>
       </c>
@@ -3878,37 +3931,35 @@
         <v>112</v>
       </c>
       <c r="C57" s="25" t="s">
-        <v>110</v>
-      </c>
-      <c r="D57" s="34" t="str">
-        <f>_xlfn.XLOOKUP(D56,table_listings!$B$2:$B$201,table_listings!$D$2:$D$201,,0)</f>
-        <v>Mix of Prj Year and Cal Year</v>
-      </c>
-      <c r="E57" s="34" t="str">
-        <f>_xlfn.XLOOKUP(E56,table_listings!$B$2:$B$201,table_listings!$D$2:$D$201,,0)</f>
-        <v>Prj Year</v>
-      </c>
-      <c r="F57" s="13"/>
-      <c r="G57" s="13"/>
-      <c r="H57" s="13"/>
-      <c r="I57" s="13"/>
-      <c r="J57" s="13"/>
+        <v>134</v>
+      </c>
+      <c r="D57" s="14">
+        <v>0</v>
+      </c>
+      <c r="E57" s="14">
+        <v>0</v>
+      </c>
+      <c r="F57" s="14"/>
+      <c r="G57" s="14"/>
+      <c r="H57" s="14"/>
+      <c r="I57" s="14"/>
+      <c r="J57" s="14"/>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A58" s="24" t="s">
+      <c r="A58" s="15" t="s">
         <v>132</v>
       </c>
-      <c r="B58" t="s">
-        <v>112</v>
-      </c>
-      <c r="C58" s="25" t="s">
-        <v>135</v>
-      </c>
-      <c r="D58" s="13" t="s">
-        <v>113</v>
-      </c>
-      <c r="E58" s="13" t="s">
-        <v>113</v>
+      <c r="B58" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="C58" s="19" t="s">
+        <v>137</v>
+      </c>
+      <c r="D58" s="13">
+        <v>1</v>
+      </c>
+      <c r="E58" s="13">
+        <v>1</v>
       </c>
       <c r="F58" s="13"/>
       <c r="G58" s="13"/>
@@ -3916,43 +3967,45 @@
       <c r="I58" s="13"/>
       <c r="J58" s="13"/>
     </row>
-    <row r="59" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="24" t="s">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A59" s="15" t="s">
         <v>132</v>
       </c>
-      <c r="B59" t="s">
-        <v>112</v>
-      </c>
-      <c r="C59" s="25" t="s">
-        <v>134</v>
-      </c>
-      <c r="D59" s="14">
-        <v>0</v>
-      </c>
-      <c r="E59" s="14">
-        <v>0</v>
-      </c>
-      <c r="F59" s="14"/>
-      <c r="G59" s="14"/>
-      <c r="H59" s="14"/>
-      <c r="I59" s="14"/>
-      <c r="J59" s="14"/>
-    </row>
-    <row r="60" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="15" t="s">
+      <c r="B59" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="C59" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="D59" s="12" t="s">
+        <v>237</v>
+      </c>
+      <c r="E59" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="F59" s="12"/>
+      <c r="G59" s="12"/>
+      <c r="H59" s="12"/>
+      <c r="I59" s="12"/>
+      <c r="J59" s="12"/>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A60" s="26" t="s">
         <v>132</v>
       </c>
-      <c r="B60" s="16" t="s">
+      <c r="B60" s="27" t="s">
         <v>121</v>
       </c>
-      <c r="C60" s="19" t="s">
-        <v>137</v>
-      </c>
-      <c r="D60" s="13">
-        <v>1</v>
-      </c>
-      <c r="E60" s="13">
-        <v>1</v>
+      <c r="C60" s="28" t="s">
+        <v>110</v>
+      </c>
+      <c r="D60" s="33" t="str">
+        <f>_xlfn.XLOOKUP(D59,table_listings!$B$2:$B$201,table_listings!$D$2:$D$201,,0)</f>
+        <v>Policy Year</v>
+      </c>
+      <c r="E60" s="33" t="str">
+        <f>_xlfn.XLOOKUP(E59,table_listings!$B$2:$B$201,table_listings!$D$2:$D$201,,0)</f>
+        <v>Scalar</v>
       </c>
       <c r="F60" s="13"/>
       <c r="G60" s="13"/>
@@ -3961,72 +4014,72 @@
       <c r="J60" s="13"/>
     </row>
     <row r="61" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="15" t="s">
-        <v>132</v>
-      </c>
-      <c r="B61" s="16" t="s">
-        <v>121</v>
-      </c>
-      <c r="C61" s="19" t="s">
+      <c r="A61" s="24" t="s">
+        <v>131</v>
+      </c>
+      <c r="B61" t="s">
+        <v>117</v>
+      </c>
+      <c r="C61" s="25" t="s">
+        <v>137</v>
+      </c>
+      <c r="D61" s="13">
+        <v>1</v>
+      </c>
+      <c r="E61" s="13">
+        <v>0.8</v>
+      </c>
+      <c r="F61" s="13"/>
+      <c r="G61" s="13"/>
+      <c r="H61" s="13"/>
+      <c r="I61" s="13"/>
+      <c r="J61" s="13"/>
+    </row>
+    <row r="62" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="24" t="s">
+        <v>131</v>
+      </c>
+      <c r="B62" t="s">
+        <v>117</v>
+      </c>
+      <c r="C62" s="25" t="s">
         <v>136</v>
       </c>
-      <c r="D61" s="12" t="s">
-        <v>127</v>
-      </c>
-      <c r="E61" s="12" t="s">
-        <v>127</v>
-      </c>
-      <c r="F61" s="12"/>
-      <c r="G61" s="12"/>
-      <c r="H61" s="12"/>
-      <c r="I61" s="12"/>
-      <c r="J61" s="12"/>
-    </row>
-    <row r="62" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="15" t="s">
-        <v>132</v>
-      </c>
-      <c r="B62" s="16" t="s">
-        <v>121</v>
-      </c>
-      <c r="C62" s="19" t="s">
+      <c r="D62" s="12" t="s">
+        <v>225</v>
+      </c>
+      <c r="E62" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="F62" s="12"/>
+      <c r="G62" s="12"/>
+      <c r="H62" s="12"/>
+      <c r="I62" s="12"/>
+      <c r="J62" s="12"/>
+    </row>
+    <row r="63" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="24" t="s">
+        <v>131</v>
+      </c>
+      <c r="B63" t="s">
+        <v>117</v>
+      </c>
+      <c r="C63" s="25" t="s">
         <v>110</v>
       </c>
-      <c r="D62" s="34" t="str">
-        <f>_xlfn.XLOOKUP(D61,table_listings!$B$2:$B$201,table_listings!$D$2:$D$201,,0)</f>
-        <v>Policy Year</v>
-      </c>
-      <c r="E62" s="34" t="str">
-        <f>_xlfn.XLOOKUP(E61,table_listings!$B$2:$B$201,table_listings!$D$2:$D$201,,0)</f>
-        <v>Policy Year</v>
-      </c>
-      <c r="F62" s="13"/>
-      <c r="G62" s="13"/>
-      <c r="H62" s="13"/>
-      <c r="I62" s="13"/>
-      <c r="J62" s="13"/>
-    </row>
-    <row r="63" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="27" t="s">
-        <v>132</v>
-      </c>
-      <c r="B63" s="28" t="s">
-        <v>121</v>
-      </c>
-      <c r="C63" s="29" t="s">
-        <v>135</v>
-      </c>
-      <c r="D63" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="E63" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="F63" s="12"/>
-      <c r="G63" s="12"/>
-      <c r="H63" s="12"/>
-      <c r="I63" s="12"/>
-      <c r="J63" s="12"/>
+      <c r="D63" s="33" t="str">
+        <f>_xlfn.XLOOKUP(D62,table_listings!$B$2:$B$201,table_listings!$D$2:$D$201,,0)</f>
+        <v>Select and Ultimate - Sex Distinct</v>
+      </c>
+      <c r="E63" s="33" t="str">
+        <f>_xlfn.XLOOKUP(E62,table_listings!$B$2:$B$201,table_listings!$D$2:$D$201,,0)</f>
+        <v>Attained Age</v>
+      </c>
+      <c r="F63" s="13"/>
+      <c r="G63" s="13"/>
+      <c r="H63" s="13"/>
+      <c r="I63" s="13"/>
+      <c r="J63" s="13"/>
     </row>
     <row r="64" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A64" s="24" t="s">
@@ -4036,87 +4089,87 @@
         <v>117</v>
       </c>
       <c r="C64" s="25" t="s">
+        <v>134</v>
+      </c>
+      <c r="D64" s="12">
+        <v>0.15</v>
+      </c>
+      <c r="E64" s="12">
+        <v>0.15</v>
+      </c>
+      <c r="F64" s="12"/>
+      <c r="G64" s="12"/>
+      <c r="H64" s="12"/>
+      <c r="I64" s="12"/>
+      <c r="J64" s="12"/>
+    </row>
+    <row r="65" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="B65" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="C65" s="19" t="s">
         <v>137</v>
       </c>
-      <c r="D64" s="13">
+      <c r="D65" s="13">
         <v>1</v>
       </c>
-      <c r="E64" s="13">
-        <v>0.8</v>
-      </c>
-      <c r="F64" s="13"/>
-      <c r="G64" s="13"/>
-      <c r="H64" s="13"/>
-      <c r="I64" s="13"/>
-      <c r="J64" s="13"/>
-    </row>
-    <row r="65" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="24" t="s">
+      <c r="E65" s="13">
+        <v>1</v>
+      </c>
+      <c r="F65" s="13"/>
+      <c r="G65" s="13"/>
+      <c r="H65" s="13"/>
+      <c r="I65" s="13"/>
+      <c r="J65" s="13"/>
+    </row>
+    <row r="66" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="B65" t="s">
-        <v>117</v>
-      </c>
-      <c r="C65" s="25" t="s">
+      <c r="B66" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="C66" s="19" t="s">
         <v>136</v>
       </c>
-      <c r="D65" s="12" t="s">
-        <v>225</v>
-      </c>
-      <c r="E65" s="12" t="s">
-        <v>109</v>
-      </c>
-      <c r="F65" s="12"/>
-      <c r="G65" s="12"/>
-      <c r="H65" s="12"/>
-      <c r="I65" s="12"/>
-      <c r="J65" s="12"/>
-    </row>
-    <row r="66" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="24" t="s">
-        <v>131</v>
-      </c>
-      <c r="B66" t="s">
-        <v>117</v>
-      </c>
-      <c r="C66" s="25" t="s">
-        <v>110</v>
-      </c>
-      <c r="D66" s="34" t="str">
-        <f>_xlfn.XLOOKUP(D65,table_listings!$B$2:$B$201,table_listings!$D$2:$D$201,,0)</f>
-        <v>Select and Ultimate - Sex Distinct</v>
-      </c>
-      <c r="E66" s="34" t="str">
-        <f>_xlfn.XLOOKUP(E65,table_listings!$B$2:$B$201,table_listings!$D$2:$D$201,,0)</f>
-        <v>Attained Age</v>
-      </c>
-      <c r="F66" s="13"/>
+      <c r="D66" s="12" t="s">
+        <v>222</v>
+      </c>
+      <c r="E66" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="F66" s="12"/>
       <c r="G66" s="13"/>
       <c r="H66" s="13"/>
       <c r="I66" s="13"/>
       <c r="J66" s="13"/>
     </row>
     <row r="67" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="24" t="s">
+      <c r="A67" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="B67" t="s">
-        <v>117</v>
-      </c>
-      <c r="C67" s="25" t="s">
-        <v>134</v>
-      </c>
-      <c r="D67" s="12">
-        <v>0.15</v>
-      </c>
-      <c r="E67" s="12">
-        <v>0.15</v>
-      </c>
-      <c r="F67" s="12"/>
-      <c r="G67" s="12"/>
-      <c r="H67" s="12"/>
-      <c r="I67" s="12"/>
-      <c r="J67" s="12"/>
+      <c r="B67" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="C67" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="D67" s="33" t="str">
+        <f>_xlfn.XLOOKUP(D66,table_listings!$B$2:$B$201,table_listings!$D$2:$D$201,,0)</f>
+        <v>Pol Year/Pol Term/Prem Term</v>
+      </c>
+      <c r="E67" s="33" t="str">
+        <f>_xlfn.XLOOKUP(E66,table_listings!$B$2:$B$201,table_listings!$D$2:$D$201,,0)</f>
+        <v>Pol Year/Pol Term</v>
+      </c>
+      <c r="F67" s="13"/>
+      <c r="G67" s="13"/>
+      <c r="H67" s="13"/>
+      <c r="I67" s="13"/>
+      <c r="J67" s="13"/>
     </row>
     <row r="68" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A68" s="15" t="s">
@@ -4126,13 +4179,13 @@
         <v>118</v>
       </c>
       <c r="C68" s="19" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D68" s="13">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="E68" s="13">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="F68" s="13"/>
       <c r="G68" s="13"/>
@@ -4141,66 +4194,66 @@
       <c r="J68" s="13"/>
     </row>
     <row r="69" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="15" t="s">
+      <c r="A69" s="24" t="s">
         <v>131</v>
       </c>
-      <c r="B69" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="C69" s="19" t="s">
-        <v>136</v>
-      </c>
-      <c r="D69" s="12" t="s">
-        <v>222</v>
-      </c>
-      <c r="E69" s="12" t="s">
-        <v>123</v>
-      </c>
-      <c r="F69" s="12"/>
+      <c r="B69" t="s">
+        <v>119</v>
+      </c>
+      <c r="C69" s="25" t="s">
+        <v>137</v>
+      </c>
+      <c r="D69" s="13">
+        <v>1</v>
+      </c>
+      <c r="E69" s="13">
+        <v>1</v>
+      </c>
+      <c r="F69" s="13"/>
       <c r="G69" s="13"/>
       <c r="H69" s="13"/>
       <c r="I69" s="13"/>
       <c r="J69" s="13"/>
     </row>
     <row r="70" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="15" t="s">
+      <c r="A70" s="24" t="s">
         <v>131</v>
       </c>
-      <c r="B70" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="C70" s="19" t="s">
+      <c r="B70" t="s">
+        <v>119</v>
+      </c>
+      <c r="C70" s="25" t="s">
+        <v>136</v>
+      </c>
+      <c r="D70" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="E70" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="F70" s="12"/>
+      <c r="G70" s="12"/>
+      <c r="H70" s="12"/>
+      <c r="I70" s="12"/>
+      <c r="J70" s="12"/>
+    </row>
+    <row r="71" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A71" s="24" t="s">
+        <v>131</v>
+      </c>
+      <c r="B71" t="s">
+        <v>119</v>
+      </c>
+      <c r="C71" s="25" t="s">
         <v>110</v>
       </c>
-      <c r="D70" s="34" t="str">
-        <f>_xlfn.XLOOKUP(D69,table_listings!$B$2:$B$201,table_listings!$D$2:$D$201,,0)</f>
-        <v>Pol Year/Pol Term/Prem Term</v>
-      </c>
-      <c r="E70" s="34" t="str">
-        <f>_xlfn.XLOOKUP(E69,table_listings!$B$2:$B$201,table_listings!$D$2:$D$201,,0)</f>
-        <v>Pol Year/Pol Term</v>
-      </c>
-      <c r="F70" s="13"/>
-      <c r="G70" s="13"/>
-      <c r="H70" s="13"/>
-      <c r="I70" s="13"/>
-      <c r="J70" s="13"/>
-    </row>
-    <row r="71" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="15" t="s">
-        <v>131</v>
-      </c>
-      <c r="B71" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="C71" s="19" t="s">
-        <v>134</v>
-      </c>
-      <c r="D71" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="E71" s="13">
-        <v>0.5</v>
+      <c r="D71" s="33" t="str">
+        <f>_xlfn.XLOOKUP(D70,table_listings!$B$2:$B$201,table_listings!$D$2:$D$201,,0)</f>
+        <v>Policy Year</v>
+      </c>
+      <c r="E71" s="33" t="str">
+        <f>_xlfn.XLOOKUP(E70,table_listings!$B$2:$B$201,table_listings!$D$2:$D$201,,0)</f>
+        <v>Policy Year</v>
       </c>
       <c r="F71" s="13"/>
       <c r="G71" s="13"/>
@@ -4216,87 +4269,87 @@
         <v>119</v>
       </c>
       <c r="C72" s="25" t="s">
+        <v>134</v>
+      </c>
+      <c r="D72" s="12">
+        <v>0.2</v>
+      </c>
+      <c r="E72" s="12">
+        <v>0.2</v>
+      </c>
+      <c r="F72" s="12"/>
+      <c r="G72" s="12"/>
+      <c r="H72" s="12"/>
+      <c r="I72" s="12"/>
+      <c r="J72" s="12"/>
+    </row>
+    <row r="73" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="B73" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="C73" s="19" t="s">
         <v>137</v>
       </c>
-      <c r="D72" s="13">
+      <c r="D73" s="13">
         <v>1</v>
       </c>
-      <c r="E72" s="13">
+      <c r="E73" s="13">
         <v>1</v>
       </c>
-      <c r="F72" s="13"/>
-      <c r="G72" s="13"/>
-      <c r="H72" s="13"/>
-      <c r="I72" s="13"/>
-      <c r="J72" s="13"/>
-    </row>
-    <row r="73" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="24" t="s">
+      <c r="F73" s="13"/>
+      <c r="G73" s="13"/>
+      <c r="H73" s="13"/>
+      <c r="I73" s="13"/>
+      <c r="J73" s="13"/>
+    </row>
+    <row r="74" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A74" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="B73" t="s">
-        <v>119</v>
-      </c>
-      <c r="C73" s="25" t="s">
+      <c r="B74" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="C74" s="19" t="s">
         <v>136</v>
       </c>
-      <c r="D73" s="12" t="s">
-        <v>125</v>
-      </c>
-      <c r="E73" s="12" t="s">
-        <v>125</v>
-      </c>
-      <c r="F73" s="12"/>
-      <c r="G73" s="12"/>
-      <c r="H73" s="12"/>
-      <c r="I73" s="12"/>
-      <c r="J73" s="12"/>
-    </row>
-    <row r="74" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="24" t="s">
-        <v>131</v>
-      </c>
-      <c r="B74" t="s">
-        <v>119</v>
-      </c>
-      <c r="C74" s="25" t="s">
-        <v>110</v>
-      </c>
-      <c r="D74" s="34" t="str">
-        <f>_xlfn.XLOOKUP(D73,table_listings!$B$2:$B$201,table_listings!$D$2:$D$201,,0)</f>
-        <v>Policy Year</v>
-      </c>
-      <c r="E74" s="34" t="str">
-        <f>_xlfn.XLOOKUP(E73,table_listings!$B$2:$B$201,table_listings!$D$2:$D$201,,0)</f>
-        <v>Policy Year</v>
-      </c>
-      <c r="F74" s="13"/>
+      <c r="D74" s="12" t="s">
+        <v>231</v>
+      </c>
+      <c r="E74" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="F74" s="12"/>
       <c r="G74" s="13"/>
       <c r="H74" s="13"/>
       <c r="I74" s="13"/>
       <c r="J74" s="13"/>
     </row>
     <row r="75" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="24" t="s">
+      <c r="A75" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="B75" t="s">
-        <v>119</v>
-      </c>
-      <c r="C75" s="25" t="s">
-        <v>134</v>
-      </c>
-      <c r="D75" s="12">
-        <v>0.2</v>
-      </c>
-      <c r="E75" s="12">
-        <v>0.2</v>
-      </c>
-      <c r="F75" s="12"/>
-      <c r="G75" s="12"/>
-      <c r="H75" s="12"/>
-      <c r="I75" s="12"/>
-      <c r="J75" s="12"/>
+      <c r="B75" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="C75" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="D75" s="33" t="str">
+        <f>_xlfn.XLOOKUP(D74,table_listings!$B$2:$B$201,table_listings!$D$2:$D$201,,0)</f>
+        <v>Mix of Prj Year and Cal Year</v>
+      </c>
+      <c r="E75" s="33" t="str">
+        <f>_xlfn.XLOOKUP(E74,table_listings!$B$2:$B$201,table_listings!$D$2:$D$201,,0)</f>
+        <v>Prj Year</v>
+      </c>
+      <c r="F75" s="13"/>
+      <c r="G75" s="13"/>
+      <c r="H75" s="13"/>
+      <c r="I75" s="13"/>
+      <c r="J75" s="13"/>
     </row>
     <row r="76" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A76" s="15" t="s">
@@ -4306,13 +4359,13 @@
         <v>112</v>
       </c>
       <c r="C76" s="19" t="s">
-        <v>137</v>
-      </c>
-      <c r="D76" s="13">
-        <v>1</v>
-      </c>
-      <c r="E76" s="13">
-        <v>1</v>
+        <v>135</v>
+      </c>
+      <c r="D76" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="E76" s="13" t="s">
+        <v>113</v>
       </c>
       <c r="F76" s="13"/>
       <c r="G76" s="13"/>
@@ -4320,7 +4373,7 @@
       <c r="I76" s="13"/>
       <c r="J76" s="13"/>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A77" s="15" t="s">
         <v>131</v>
       </c>
@@ -4328,37 +4381,35 @@
         <v>112</v>
       </c>
       <c r="C77" s="19" t="s">
-        <v>136</v>
-      </c>
-      <c r="D77" s="12" t="s">
-        <v>231</v>
-      </c>
-      <c r="E77" s="12" t="s">
-        <v>126</v>
-      </c>
-      <c r="F77" s="12"/>
+        <v>134</v>
+      </c>
+      <c r="D77" s="13">
+        <v>0</v>
+      </c>
+      <c r="E77" s="13">
+        <v>0</v>
+      </c>
+      <c r="F77" s="13"/>
       <c r="G77" s="13"/>
       <c r="H77" s="13"/>
       <c r="I77" s="13"/>
       <c r="J77" s="13"/>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A78" s="15" t="s">
+      <c r="A78" s="24" t="s">
         <v>131</v>
       </c>
-      <c r="B78" s="16" t="s">
-        <v>112</v>
-      </c>
-      <c r="C78" s="19" t="s">
-        <v>110</v>
-      </c>
-      <c r="D78" s="34" t="str">
-        <f>_xlfn.XLOOKUP(D77,table_listings!$B$2:$B$201,table_listings!$D$2:$D$201,,0)</f>
-        <v>Mix of Prj Year and Cal Year</v>
-      </c>
-      <c r="E78" s="34" t="str">
-        <f>_xlfn.XLOOKUP(E77,table_listings!$B$2:$B$201,table_listings!$D$2:$D$201,,0)</f>
-        <v>Prj Year</v>
+      <c r="B78" t="s">
+        <v>121</v>
+      </c>
+      <c r="C78" s="25" t="s">
+        <v>137</v>
+      </c>
+      <c r="D78" s="13">
+        <v>1</v>
+      </c>
+      <c r="E78" s="13">
+        <v>1</v>
       </c>
       <c r="F78" s="13"/>
       <c r="G78" s="13"/>
@@ -4367,42 +4418,44 @@
       <c r="J78" s="13"/>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A79" s="15" t="s">
+      <c r="A79" s="24" t="s">
         <v>131</v>
       </c>
-      <c r="B79" s="16" t="s">
-        <v>112</v>
-      </c>
-      <c r="C79" s="19" t="s">
-        <v>135</v>
-      </c>
-      <c r="D79" s="13" t="s">
-        <v>113</v>
-      </c>
-      <c r="E79" s="13" t="s">
-        <v>113</v>
-      </c>
-      <c r="F79" s="13"/>
+      <c r="B79" t="s">
+        <v>121</v>
+      </c>
+      <c r="C79" s="25" t="s">
+        <v>136</v>
+      </c>
+      <c r="D79" s="12" t="s">
+        <v>237</v>
+      </c>
+      <c r="E79" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="F79" s="12"/>
       <c r="G79" s="13"/>
       <c r="H79" s="13"/>
       <c r="I79" s="13"/>
       <c r="J79" s="13"/>
     </row>
-    <row r="80" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="15" t="s">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A80" s="29" t="s">
         <v>131</v>
       </c>
-      <c r="B80" s="16" t="s">
-        <v>112</v>
-      </c>
-      <c r="C80" s="19" t="s">
-        <v>134</v>
-      </c>
-      <c r="D80" s="13">
-        <v>0</v>
-      </c>
-      <c r="E80" s="13">
-        <v>0</v>
+      <c r="B80" s="30" t="s">
+        <v>121</v>
+      </c>
+      <c r="C80" s="31" t="s">
+        <v>110</v>
+      </c>
+      <c r="D80" s="33" t="str">
+        <f>_xlfn.XLOOKUP(D79,table_listings!$B$2:$B$201,table_listings!$D$2:$D$201,,0)</f>
+        <v>Policy Year</v>
+      </c>
+      <c r="E80" s="33" t="str">
+        <f>_xlfn.XLOOKUP(E79,table_listings!$B$2:$B$201,table_listings!$D$2:$D$201,,0)</f>
+        <v>Scalar</v>
       </c>
       <c r="F80" s="13"/>
       <c r="G80" s="13"/>
@@ -4410,109 +4463,12 @@
       <c r="I80" s="13"/>
       <c r="J80" s="13"/>
     </row>
-    <row r="81" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="24" t="s">
-        <v>131</v>
-      </c>
-      <c r="B81" t="s">
-        <v>121</v>
-      </c>
-      <c r="C81" s="25" t="s">
-        <v>137</v>
-      </c>
-      <c r="D81" s="13">
-        <v>1</v>
-      </c>
-      <c r="E81" s="13">
-        <v>1</v>
-      </c>
-      <c r="F81" s="13"/>
-      <c r="G81" s="13"/>
-      <c r="H81" s="13"/>
-      <c r="I81" s="13"/>
-      <c r="J81" s="13"/>
-    </row>
-    <row r="82" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A82" s="24" t="s">
-        <v>131</v>
-      </c>
-      <c r="B82" t="s">
-        <v>121</v>
-      </c>
-      <c r="C82" s="25" t="s">
-        <v>136</v>
-      </c>
-      <c r="D82" s="12" t="s">
-        <v>127</v>
-      </c>
-      <c r="E82" s="12" t="s">
-        <v>127</v>
-      </c>
-      <c r="F82" s="12"/>
-      <c r="G82" s="13"/>
-      <c r="H82" s="13"/>
-      <c r="I82" s="13"/>
-      <c r="J82" s="13"/>
-    </row>
-    <row r="83" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="24" t="s">
-        <v>131</v>
-      </c>
-      <c r="B83" t="s">
-        <v>121</v>
-      </c>
-      <c r="C83" s="25" t="s">
-        <v>110</v>
-      </c>
-      <c r="D83" s="34" t="str">
-        <f>_xlfn.XLOOKUP(D82,table_listings!$B$2:$B$201,table_listings!$D$2:$D$201,,0)</f>
-        <v>Policy Year</v>
-      </c>
-      <c r="E83" s="34" t="str">
-        <f>_xlfn.XLOOKUP(E82,table_listings!$B$2:$B$201,table_listings!$D$2:$D$201,,0)</f>
-        <v>Policy Year</v>
-      </c>
-      <c r="F83" s="13"/>
-      <c r="G83" s="13"/>
-      <c r="H83" s="13"/>
-      <c r="I83" s="13"/>
-      <c r="J83" s="13"/>
-    </row>
-    <row r="84" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A84" s="30" t="s">
-        <v>131</v>
-      </c>
-      <c r="B84" s="31" t="s">
-        <v>121</v>
-      </c>
-      <c r="C84" s="32" t="s">
-        <v>135</v>
-      </c>
-      <c r="D84" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="E84" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="F84" s="12"/>
-      <c r="G84" s="12"/>
-      <c r="H84" s="12"/>
-      <c r="I84" s="12"/>
-      <c r="J84" s="12"/>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:C84" xr:uid="{C1E729B3-29BA-40F1-80D4-2208DEC4BA85}">
+  <autoFilter ref="A1:C80" xr:uid="{C1E729B3-29BA-40F1-80D4-2208DEC4BA85}">
     <filterColumn colId="1">
       <filters>
-        <filter val="disc_rate"/>
-        <filter val="invt_return"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="2">
-      <filters>
-        <filter val="Table"/>
-        <filter val="Table Column"/>
-        <filter val="Table Type"/>
+        <filter val="prem_tax"/>
+        <filter val="tax"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -4535,37 +4491,37 @@
           <x14:formula1>
             <xm:f>table_listings!$B$82:$B$101</xm:f>
           </x14:formula1>
-          <xm:sqref>D19:E19 D44:E44 D65:E65</xm:sqref>
+          <xm:sqref>D19:E19 D42:E42 D62:E62</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{9B11AC40-BA78-465E-A8C2-ABDE8DC86665}">
           <x14:formula1>
             <xm:f>table_listings!$B$102:$B$121</xm:f>
           </x14:formula1>
-          <xm:sqref>D22:E22 D48:E48 D69:E69</xm:sqref>
+          <xm:sqref>D22:E22 D46:E46 D66:E66</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{AE6B13E0-3C67-444A-9E02-E0311D9C7B6B}">
           <x14:formula1>
             <xm:f>table_listings!$B$122:$B$141</xm:f>
           </x14:formula1>
-          <xm:sqref>D52:E52 D73:E73 D25:E25</xm:sqref>
+          <xm:sqref>D50:E50 D70:E70 D25:E25</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{3672E154-D911-4052-9461-331AE0607E99}">
           <x14:formula1>
             <xm:f>table_listings!$B$142:$B$161</xm:f>
           </x14:formula1>
-          <xm:sqref>D28:E28 D56:E56 D32:E32 D77:E77</xm:sqref>
+          <xm:sqref>D28:E28 D54:E54 D32:E32 D74:E74</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{9147491E-BAE9-4A7D-A399-337FB5EBD658}">
           <x14:formula1>
             <xm:f>table_listings!$B$162:$B$181</xm:f>
           </x14:formula1>
-          <xm:sqref>D61:E61 D82:E82 D36:E36</xm:sqref>
+          <xm:sqref>D36:E36 D59:E59 D79:E79</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{A8A71A06-9618-4D56-9684-D28AB541F566}">
           <x14:formula1>
             <xm:f>table_listings!$B$182:$B$201</xm:f>
           </x14:formula1>
-          <xm:sqref>D40:E40</xm:sqref>
+          <xm:sqref>D39:E39</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{8D4735E1-493A-4394-A167-60A1C878702C}">
           <x14:formula1>
@@ -4596,7 +4552,7 @@
   <dimension ref="A1:D201"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B122" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B164" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="D142" sqref="D142:D144"/>
@@ -4610,16 +4566,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="34" t="s">
         <v>172</v>
       </c>
-      <c r="B1" s="35" t="s">
+      <c r="B1" s="34" t="s">
         <v>108</v>
       </c>
-      <c r="C1" s="35" t="s">
+      <c r="C1" s="34" t="s">
         <v>146</v>
       </c>
-      <c r="D1" s="35" t="s">
+      <c r="D1" s="34" t="s">
         <v>110</v>
       </c>
     </row>
@@ -7357,24 +7313,24 @@
       </c>
       <c r="D162" s="9" t="str">
         <f>[1]prem_tax!C2</f>
-        <v>Policy Year</v>
+        <v>Scalar</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A163" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="B163" s="9">
+      <c r="B163" s="9" t="str">
         <f>[1]prem_tax!A3</f>
-        <v>0</v>
-      </c>
-      <c r="C163" s="9">
+        <v>PREMTAX02</v>
+      </c>
+      <c r="C163" s="9" t="str">
         <f>[1]prem_tax!B3</f>
-        <v>0</v>
-      </c>
-      <c r="D163" s="9">
+        <v>Premium Tax Rate Table</v>
+      </c>
+      <c r="D163" s="9" t="str">
         <f>[1]prem_tax!C3</f>
-        <v>0</v>
+        <v>Policy Year</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.3">
@@ -7697,24 +7653,24 @@
       </c>
       <c r="D182" s="9" t="str">
         <f>[1]tax!C2</f>
-        <v>Policy Year</v>
+        <v>Scalar</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A183" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="B183" s="9">
+      <c r="B183" s="9" t="str">
         <f>[1]tax!A3</f>
-        <v>0</v>
-      </c>
-      <c r="C183" s="9">
+        <v>TAX02</v>
+      </c>
+      <c r="C183" s="9" t="str">
         <f>[1]tax!B3</f>
-        <v>0</v>
-      </c>
-      <c r="D183" s="9">
+        <v>Tax Rate Table</v>
+      </c>
+      <c r="D183" s="9" t="str">
         <f>[1]tax!C3</f>
-        <v>0</v>
+        <v>Policy Year</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.3">
@@ -8089,7 +8045,7 @@
       <c r="B4" t="s">
         <v>49</v>
       </c>
-      <c r="C4" s="38" t="s">
+      <c r="C4" s="37" t="s">
         <v>10</v>
       </c>
     </row>
@@ -8815,10 +8771,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA1111D6-CFD5-472E-AAF0-AF6E36C438B2}">
-  <dimension ref="B1:F46"/>
+  <dimension ref="B1:F48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8831,19 +8787,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="35" t="s">
         <v>195</v>
       </c>
-      <c r="C1" s="36" t="s">
+      <c r="C1" s="35" t="s">
         <v>188</v>
       </c>
-      <c r="D1" s="36" t="s">
+      <c r="D1" s="35" t="s">
         <v>190</v>
       </c>
-      <c r="E1" s="36" t="s">
+      <c r="E1" s="35" t="s">
         <v>189</v>
       </c>
-      <c r="F1" s="36" t="s">
+      <c r="F1" s="35" t="s">
         <v>224</v>
       </c>
     </row>
@@ -8969,14 +8925,14 @@
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B12" s="36" t="s">
+      <c r="B12" s="35" t="s">
         <v>209</v>
       </c>
-      <c r="C12" s="36" t="s">
+      <c r="C12" s="35" t="s">
         <v>188</v>
       </c>
-      <c r="D12" s="36"/>
-      <c r="E12" s="36"/>
+      <c r="D12" s="35"/>
+      <c r="E12" s="35"/>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
@@ -9068,10 +9024,10 @@
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
-        <v>118</v>
-      </c>
-      <c r="C21" t="s">
-        <v>215</v>
+        <v>117</v>
+      </c>
+      <c r="C21" s="38" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.3">
@@ -9079,26 +9035,26 @@
         <v>118</v>
       </c>
       <c r="C22" t="s">
-        <v>216</v>
-      </c>
-      <c r="D22" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C23" t="s">
-        <v>236</v>
+        <v>216</v>
+      </c>
+      <c r="D23" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
-        <v>112</v>
+        <v>119</v>
       </c>
       <c r="C24" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.3">
@@ -9106,7 +9062,7 @@
         <v>112</v>
       </c>
       <c r="C25" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.3">
@@ -9114,15 +9070,15 @@
         <v>112</v>
       </c>
       <c r="C26" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="C27" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.3">
@@ -9130,7 +9086,7 @@
         <v>120</v>
       </c>
       <c r="C28" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.3">
@@ -9138,28 +9094,28 @@
         <v>120</v>
       </c>
       <c r="C29" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
-        <v>121</v>
-      </c>
-      <c r="C30" t="s">
-        <v>235</v>
+        <v>120</v>
+      </c>
+      <c r="C30" s="38" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
-        <v>121</v>
-      </c>
-      <c r="C31" t="s">
-        <v>232</v>
+        <v>120</v>
+      </c>
+      <c r="C31" s="38" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C32" t="s">
         <v>235</v>
@@ -9167,73 +9123,89 @@
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C33" t="s">
         <v>232</v>
       </c>
     </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B34" t="s">
+        <v>122</v>
+      </c>
+      <c r="C34" t="s">
+        <v>235</v>
+      </c>
+    </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B35" s="36" t="s">
+      <c r="B35" t="s">
+        <v>122</v>
+      </c>
+      <c r="C35" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B37" s="35" t="s">
         <v>179</v>
       </c>
-      <c r="C35" s="36" t="s">
+      <c r="C37" s="35" t="s">
         <v>211</v>
       </c>
-      <c r="D35" s="36"/>
-    </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B36" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B37" t="s">
-        <v>181</v>
-      </c>
+      <c r="D37" s="35"/>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
-        <v>210</v>
+        <v>183</v>
       </c>
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B42" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B43" t="s">
-        <v>202</v>
+        <v>210</v>
       </c>
     </row>
     <row r="44" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B44" t="s">
-        <v>175</v>
+        <v>185</v>
       </c>
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B45" t="s">
-        <v>174</v>
+        <v>202</v>
       </c>
     </row>
     <row r="46" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B46" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="47" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B47" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="48" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B48" t="s">
         <v>186</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add time 0 to fix cashflow errors
</commit_message>
<xml_diff>
--- a/Input/Settings.xlsx
+++ b/Input/Settings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Julia\TradLifeModel\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F407EDF-4683-4738-AB26-56557784BFA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{361892B8-BCBE-43CE-B288-1F40304E047D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="889" activeTab="5" xr2:uid="{ADF8BBD9-0F7A-45CB-8EA8-A3D46B124E82}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="889" activeTab="2" xr2:uid="{ADF8BBD9-0F7A-45CB-8EA8-A3D46B124E82}"/>
   </bookViews>
   <sheets>
     <sheet name="general_settings" sheetId="13" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="882" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="882" uniqueCount="241">
   <si>
     <t>acq_exp_per_pol</t>
   </si>
@@ -670,9 +670,6 @@
   </si>
   <si>
     <t>Rate per 1000 sum assured by Policy Year and Issue Age and Premium Term</t>
-  </si>
-  <si>
-    <t>SV03</t>
   </si>
   <si>
     <t>Assumptions in product_setup</t>
@@ -1137,9 +1134,9 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
       <sheetData sheetId="4">
         <row r="2">
           <cell r="A2" t="str">
@@ -1164,8 +1161,8 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
       <sheetData sheetId="7">
         <row r="2">
           <cell r="A2" t="str">
@@ -1201,9 +1198,9 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="8" refreshError="1"/>
-      <sheetData sheetId="9" refreshError="1"/>
-      <sheetData sheetId="10" refreshError="1"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
       <sheetData sheetId="11">
         <row r="2">
           <cell r="A2" t="str">
@@ -1239,9 +1236,9 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="12" refreshError="1"/>
-      <sheetData sheetId="13" refreshError="1"/>
-      <sheetData sheetId="14" refreshError="1"/>
+      <sheetData sheetId="12"/>
+      <sheetData sheetId="13"/>
+      <sheetData sheetId="14"/>
       <sheetData sheetId="15">
         <row r="2">
           <cell r="A2" t="str">
@@ -1332,14 +1329,14 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="16" refreshError="1"/>
-      <sheetData sheetId="17" refreshError="1"/>
-      <sheetData sheetId="18" refreshError="1"/>
-      <sheetData sheetId="19" refreshError="1"/>
-      <sheetData sheetId="20" refreshError="1"/>
-      <sheetData sheetId="21" refreshError="1"/>
-      <sheetData sheetId="22" refreshError="1"/>
-      <sheetData sheetId="23" refreshError="1"/>
+      <sheetData sheetId="16"/>
+      <sheetData sheetId="17"/>
+      <sheetData sheetId="18"/>
+      <sheetData sheetId="19"/>
+      <sheetData sheetId="20"/>
+      <sheetData sheetId="21"/>
+      <sheetData sheetId="22"/>
+      <sheetData sheetId="23"/>
       <sheetData sheetId="24">
         <row r="2">
           <cell r="A2" t="str">
@@ -1364,8 +1361,8 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="25" refreshError="1"/>
-      <sheetData sheetId="26" refreshError="1"/>
+      <sheetData sheetId="25"/>
+      <sheetData sheetId="26"/>
       <sheetData sheetId="27">
         <row r="2">
           <cell r="A2" t="str">
@@ -1379,7 +1376,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="28" refreshError="1"/>
+      <sheetData sheetId="28"/>
       <sheetData sheetId="29">
         <row r="2">
           <cell r="A2" t="str">
@@ -1415,9 +1412,9 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="30" refreshError="1"/>
-      <sheetData sheetId="31" refreshError="1"/>
-      <sheetData sheetId="32" refreshError="1"/>
+      <sheetData sheetId="30"/>
+      <sheetData sheetId="31"/>
+      <sheetData sheetId="32"/>
       <sheetData sheetId="33">
         <row r="2">
           <cell r="A2" t="str">
@@ -1442,8 +1439,8 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="34" refreshError="1"/>
-      <sheetData sheetId="35" refreshError="1"/>
+      <sheetData sheetId="34"/>
+      <sheetData sheetId="35"/>
       <sheetData sheetId="36">
         <row r="2">
           <cell r="A2" t="str">
@@ -1468,8 +1465,8 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="37" refreshError="1"/>
-      <sheetData sheetId="38" refreshError="1"/>
+      <sheetData sheetId="37"/>
+      <sheetData sheetId="38"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -2066,7 +2063,7 @@
         <v>81</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>80</v>
@@ -2659,14 +2656,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1E729B3-29BA-40F1-80D4-2208DEC4BA85}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:J80"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D39" sqref="D39"/>
+      <selection pane="bottomRight" activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2697,7 +2693,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="2" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>141</v>
       </c>
@@ -2719,7 +2715,7 @@
       <c r="I2" s="13"/>
       <c r="J2" s="13"/>
     </row>
-    <row r="3" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>141</v>
       </c>
@@ -2741,7 +2737,7 @@
       <c r="I3" s="13"/>
       <c r="J3" s="13"/>
     </row>
-    <row r="4" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>141</v>
       </c>
@@ -2765,7 +2761,7 @@
       <c r="I4" s="13"/>
       <c r="J4" s="13"/>
     </row>
-    <row r="5" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>141</v>
       </c>
@@ -2783,7 +2779,7 @@
       <c r="I5" s="12"/>
       <c r="J5" s="12"/>
     </row>
-    <row r="6" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="15" t="s">
         <v>141</v>
       </c>
@@ -2805,7 +2801,7 @@
       <c r="I6" s="13"/>
       <c r="J6" s="13"/>
     </row>
-    <row r="7" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="15" t="s">
         <v>141</v>
       </c>
@@ -2827,7 +2823,7 @@
       <c r="I7" s="13"/>
       <c r="J7" s="13"/>
     </row>
-    <row r="8" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="15" t="s">
         <v>141</v>
       </c>
@@ -2851,7 +2847,7 @@
       <c r="I8" s="13"/>
       <c r="J8" s="13"/>
     </row>
-    <row r="9" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="15" t="s">
         <v>141</v>
       </c>
@@ -2871,7 +2867,7 @@
       <c r="I9" s="12"/>
       <c r="J9" s="12"/>
     </row>
-    <row r="10" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="24" t="s">
         <v>141</v>
       </c>
@@ -2893,7 +2889,7 @@
       <c r="I10" s="13"/>
       <c r="J10" s="13"/>
     </row>
-    <row r="11" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="24" t="s">
         <v>141</v>
       </c>
@@ -2904,7 +2900,7 @@
         <v>136</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>208</v>
+        <v>130</v>
       </c>
       <c r="E11" s="12" t="s">
         <v>130</v>
@@ -2915,7 +2911,7 @@
       <c r="I11" s="12"/>
       <c r="J11" s="12"/>
     </row>
-    <row r="12" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="24" t="s">
         <v>141</v>
       </c>
@@ -2927,7 +2923,7 @@
       </c>
       <c r="D12" s="33" t="str">
         <f>_xlfn.XLOOKUP(D11,table_listings!$B$2:$B$201,table_listings!$D$2:$D$201,,0)</f>
-        <v>Rate per 1000 SA by Pol Year/Issue Age/Prem Term</v>
+        <v>Rate per 1000 SA by Year/Age</v>
       </c>
       <c r="E12" s="33" t="str">
         <f>_xlfn.XLOOKUP(E11,table_listings!$B$2:$B$201,table_listings!$D$2:$D$201,,0)</f>
@@ -2939,7 +2935,7 @@
       <c r="I12" s="13"/>
       <c r="J12" s="13"/>
     </row>
-    <row r="13" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="24" t="s">
         <v>141</v>
       </c>
@@ -2957,7 +2953,7 @@
       <c r="I13" s="12"/>
       <c r="J13" s="12"/>
     </row>
-    <row r="14" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="15" t="s">
         <v>141</v>
       </c>
@@ -2979,7 +2975,7 @@
       <c r="I14" s="13"/>
       <c r="J14" s="13"/>
     </row>
-    <row r="15" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="15" t="s">
         <v>141</v>
       </c>
@@ -3001,7 +2997,7 @@
       <c r="I15" s="13"/>
       <c r="J15" s="13"/>
     </row>
-    <row r="16" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="15" t="s">
         <v>141</v>
       </c>
@@ -3025,7 +3021,7 @@
       <c r="I16" s="13"/>
       <c r="J16" s="13"/>
     </row>
-    <row r="17" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="15" t="s">
         <v>141</v>
       </c>
@@ -3043,7 +3039,7 @@
       <c r="I17" s="12"/>
       <c r="J17" s="12"/>
     </row>
-    <row r="18" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="21" t="s">
         <v>133</v>
       </c>
@@ -3065,7 +3061,7 @@
       <c r="I18" s="13"/>
       <c r="J18" s="13"/>
     </row>
-    <row r="19" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="24" t="s">
         <v>133</v>
       </c>
@@ -3076,7 +3072,7 @@
         <v>136</v>
       </c>
       <c r="D19" s="12" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E19" s="12" t="s">
         <v>109</v>
@@ -3087,7 +3083,7 @@
       <c r="I19" s="12"/>
       <c r="J19" s="12"/>
     </row>
-    <row r="20" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="24" t="s">
         <v>133</v>
       </c>
@@ -3111,7 +3107,7 @@
       <c r="I20" s="13"/>
       <c r="J20" s="13"/>
     </row>
-    <row r="21" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="15" t="s">
         <v>133</v>
       </c>
@@ -3133,7 +3129,7 @@
       <c r="I21" s="13"/>
       <c r="J21" s="13"/>
     </row>
-    <row r="22" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="15" t="s">
         <v>133</v>
       </c>
@@ -3144,7 +3140,7 @@
         <v>136</v>
       </c>
       <c r="D22" s="12" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E22" s="12" t="s">
         <v>123</v>
@@ -3155,7 +3151,7 @@
       <c r="I22" s="12"/>
       <c r="J22" s="12"/>
     </row>
-    <row r="23" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" s="15" t="s">
         <v>133</v>
       </c>
@@ -3179,7 +3175,7 @@
       <c r="I23" s="13"/>
       <c r="J23" s="13"/>
     </row>
-    <row r="24" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" s="24" t="s">
         <v>133</v>
       </c>
@@ -3201,7 +3197,7 @@
       <c r="I24" s="13"/>
       <c r="J24" s="13"/>
     </row>
-    <row r="25" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" s="24" t="s">
         <v>133</v>
       </c>
@@ -3223,7 +3219,7 @@
       <c r="I25" s="12"/>
       <c r="J25" s="12"/>
     </row>
-    <row r="26" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" s="24" t="s">
         <v>133</v>
       </c>
@@ -3247,7 +3243,7 @@
       <c r="I26" s="13"/>
       <c r="J26" s="13"/>
     </row>
-    <row r="27" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" s="15" t="s">
         <v>133</v>
       </c>
@@ -3269,7 +3265,7 @@
       <c r="I27" s="13"/>
       <c r="J27" s="13"/>
     </row>
-    <row r="28" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" s="15" t="s">
         <v>133</v>
       </c>
@@ -3280,7 +3276,7 @@
         <v>136</v>
       </c>
       <c r="D28" s="12" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E28" s="12" t="s">
         <v>126</v>
@@ -3291,7 +3287,7 @@
       <c r="I28" s="12"/>
       <c r="J28" s="12"/>
     </row>
-    <row r="29" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" s="15" t="s">
         <v>133</v>
       </c>
@@ -3315,7 +3311,7 @@
       <c r="I29" s="13"/>
       <c r="J29" s="13"/>
     </row>
-    <row r="30" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" s="15" t="s">
         <v>133</v>
       </c>
@@ -3337,7 +3333,7 @@
       <c r="I30" s="12"/>
       <c r="J30" s="12"/>
     </row>
-    <row r="31" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" s="24" t="s">
         <v>133</v>
       </c>
@@ -3359,7 +3355,7 @@
       <c r="I31" s="13"/>
       <c r="J31" s="13"/>
     </row>
-    <row r="32" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" s="24" t="s">
         <v>133</v>
       </c>
@@ -3370,7 +3366,7 @@
         <v>136</v>
       </c>
       <c r="D32" s="12" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E32" s="12" t="s">
         <v>126</v>
@@ -3381,7 +3377,7 @@
       <c r="I32" s="12"/>
       <c r="J32" s="12"/>
     </row>
-    <row r="33" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" s="24" t="s">
         <v>133</v>
       </c>
@@ -3405,7 +3401,7 @@
       <c r="I33" s="13"/>
       <c r="J33" s="13"/>
     </row>
-    <row r="34" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34" s="24" t="s">
         <v>133</v>
       </c>
@@ -3460,7 +3456,7 @@
         <v>136</v>
       </c>
       <c r="D36" s="12" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E36" s="12" t="s">
         <v>127</v>
@@ -3528,7 +3524,7 @@
         <v>136</v>
       </c>
       <c r="D39" s="12" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E39" s="12" t="s">
         <v>128</v>
@@ -3563,7 +3559,7 @@
       <c r="I40" s="13"/>
       <c r="J40" s="13"/>
     </row>
-    <row r="41" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41" s="17" t="s">
         <v>132</v>
       </c>
@@ -3585,7 +3581,7 @@
       <c r="I41" s="13"/>
       <c r="J41" s="13"/>
     </row>
-    <row r="42" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42" s="15" t="s">
         <v>132</v>
       </c>
@@ -3596,7 +3592,7 @@
         <v>136</v>
       </c>
       <c r="D42" s="12" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E42" s="12" t="s">
         <v>109</v>
@@ -3607,7 +3603,7 @@
       <c r="I42" s="12"/>
       <c r="J42" s="12"/>
     </row>
-    <row r="43" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43" s="15" t="s">
         <v>132</v>
       </c>
@@ -3631,7 +3627,7 @@
       <c r="I43" s="13"/>
       <c r="J43" s="13"/>
     </row>
-    <row r="44" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44" s="15" t="s">
         <v>132</v>
       </c>
@@ -3653,7 +3649,7 @@
       <c r="I44" s="12"/>
       <c r="J44" s="12"/>
     </row>
-    <row r="45" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45" s="24" t="s">
         <v>132</v>
       </c>
@@ -3675,7 +3671,7 @@
       <c r="I45" s="13"/>
       <c r="J45" s="13"/>
     </row>
-    <row r="46" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A46" s="24" t="s">
         <v>132</v>
       </c>
@@ -3686,7 +3682,7 @@
         <v>136</v>
       </c>
       <c r="D46" s="12" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E46" s="12" t="s">
         <v>123</v>
@@ -3697,7 +3693,7 @@
       <c r="I46" s="12"/>
       <c r="J46" s="12"/>
     </row>
-    <row r="47" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47" s="24" t="s">
         <v>132</v>
       </c>
@@ -3721,7 +3717,7 @@
       <c r="I47" s="13"/>
       <c r="J47" s="13"/>
     </row>
-    <row r="48" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A48" s="24" t="s">
         <v>132</v>
       </c>
@@ -3743,7 +3739,7 @@
       <c r="I48" s="12"/>
       <c r="J48" s="12"/>
     </row>
-    <row r="49" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A49" s="15" t="s">
         <v>132</v>
       </c>
@@ -3765,7 +3761,7 @@
       <c r="I49" s="13"/>
       <c r="J49" s="13"/>
     </row>
-    <row r="50" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A50" s="15" t="s">
         <v>132</v>
       </c>
@@ -3787,7 +3783,7 @@
       <c r="I50" s="12"/>
       <c r="J50" s="12"/>
     </row>
-    <row r="51" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A51" s="15" t="s">
         <v>132</v>
       </c>
@@ -3811,7 +3807,7 @@
       <c r="I51" s="13"/>
       <c r="J51" s="13"/>
     </row>
-    <row r="52" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A52" s="15" t="s">
         <v>132</v>
       </c>
@@ -3833,7 +3829,7 @@
       <c r="I52" s="12"/>
       <c r="J52" s="12"/>
     </row>
-    <row r="53" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A53" s="24" t="s">
         <v>132</v>
       </c>
@@ -3855,7 +3851,7 @@
       <c r="I53" s="13"/>
       <c r="J53" s="13"/>
     </row>
-    <row r="54" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A54" s="24" t="s">
         <v>132</v>
       </c>
@@ -3866,7 +3862,7 @@
         <v>136</v>
       </c>
       <c r="D54" s="12" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E54" s="12" t="s">
         <v>126</v>
@@ -3877,7 +3873,7 @@
       <c r="I54" s="12"/>
       <c r="J54" s="12"/>
     </row>
-    <row r="55" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A55" s="24" t="s">
         <v>132</v>
       </c>
@@ -3901,7 +3897,7 @@
       <c r="I55" s="13"/>
       <c r="J55" s="13"/>
     </row>
-    <row r="56" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A56" s="24" t="s">
         <v>132</v>
       </c>
@@ -3923,7 +3919,7 @@
       <c r="I56" s="13"/>
       <c r="J56" s="13"/>
     </row>
-    <row r="57" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A57" s="24" t="s">
         <v>132</v>
       </c>
@@ -3978,7 +3974,7 @@
         <v>136</v>
       </c>
       <c r="D59" s="12" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E59" s="12" t="s">
         <v>127</v>
@@ -4013,7 +4009,7 @@
       <c r="I60" s="13"/>
       <c r="J60" s="13"/>
     </row>
-    <row r="61" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A61" s="24" t="s">
         <v>131</v>
       </c>
@@ -4035,7 +4031,7 @@
       <c r="I61" s="13"/>
       <c r="J61" s="13"/>
     </row>
-    <row r="62" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A62" s="24" t="s">
         <v>131</v>
       </c>
@@ -4046,7 +4042,7 @@
         <v>136</v>
       </c>
       <c r="D62" s="12" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E62" s="12" t="s">
         <v>109</v>
@@ -4057,7 +4053,7 @@
       <c r="I62" s="12"/>
       <c r="J62" s="12"/>
     </row>
-    <row r="63" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A63" s="24" t="s">
         <v>131</v>
       </c>
@@ -4081,7 +4077,7 @@
       <c r="I63" s="13"/>
       <c r="J63" s="13"/>
     </row>
-    <row r="64" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A64" s="24" t="s">
         <v>131</v>
       </c>
@@ -4103,7 +4099,7 @@
       <c r="I64" s="12"/>
       <c r="J64" s="12"/>
     </row>
-    <row r="65" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A65" s="15" t="s">
         <v>131</v>
       </c>
@@ -4125,7 +4121,7 @@
       <c r="I65" s="13"/>
       <c r="J65" s="13"/>
     </row>
-    <row r="66" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A66" s="15" t="s">
         <v>131</v>
       </c>
@@ -4136,7 +4132,7 @@
         <v>136</v>
       </c>
       <c r="D66" s="12" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E66" s="12" t="s">
         <v>123</v>
@@ -4147,7 +4143,7 @@
       <c r="I66" s="13"/>
       <c r="J66" s="13"/>
     </row>
-    <row r="67" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A67" s="15" t="s">
         <v>131</v>
       </c>
@@ -4171,7 +4167,7 @@
       <c r="I67" s="13"/>
       <c r="J67" s="13"/>
     </row>
-    <row r="68" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A68" s="15" t="s">
         <v>131</v>
       </c>
@@ -4193,7 +4189,7 @@
       <c r="I68" s="13"/>
       <c r="J68" s="13"/>
     </row>
-    <row r="69" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A69" s="24" t="s">
         <v>131</v>
       </c>
@@ -4215,7 +4211,7 @@
       <c r="I69" s="13"/>
       <c r="J69" s="13"/>
     </row>
-    <row r="70" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A70" s="24" t="s">
         <v>131</v>
       </c>
@@ -4237,7 +4233,7 @@
       <c r="I70" s="12"/>
       <c r="J70" s="12"/>
     </row>
-    <row r="71" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A71" s="24" t="s">
         <v>131</v>
       </c>
@@ -4261,7 +4257,7 @@
       <c r="I71" s="13"/>
       <c r="J71" s="13"/>
     </row>
-    <row r="72" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A72" s="24" t="s">
         <v>131</v>
       </c>
@@ -4283,7 +4279,7 @@
       <c r="I72" s="12"/>
       <c r="J72" s="12"/>
     </row>
-    <row r="73" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A73" s="15" t="s">
         <v>131</v>
       </c>
@@ -4305,7 +4301,7 @@
       <c r="I73" s="13"/>
       <c r="J73" s="13"/>
     </row>
-    <row r="74" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A74" s="15" t="s">
         <v>131</v>
       </c>
@@ -4316,7 +4312,7 @@
         <v>136</v>
       </c>
       <c r="D74" s="12" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E74" s="12" t="s">
         <v>126</v>
@@ -4327,7 +4323,7 @@
       <c r="I74" s="13"/>
       <c r="J74" s="13"/>
     </row>
-    <row r="75" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A75" s="15" t="s">
         <v>131</v>
       </c>
@@ -4351,7 +4347,7 @@
       <c r="I75" s="13"/>
       <c r="J75" s="13"/>
     </row>
-    <row r="76" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A76" s="15" t="s">
         <v>131</v>
       </c>
@@ -4373,7 +4369,7 @@
       <c r="I76" s="13"/>
       <c r="J76" s="13"/>
     </row>
-    <row r="77" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A77" s="15" t="s">
         <v>131</v>
       </c>
@@ -4428,7 +4424,7 @@
         <v>136</v>
       </c>
       <c r="D79" s="12" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E79" s="12" t="s">
         <v>127</v>
@@ -4464,14 +4460,7 @@
       <c r="J80" s="13"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C80" xr:uid="{C1E729B3-29BA-40F1-80D4-2208DEC4BA85}">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="prem_tax"/>
-        <filter val="tax"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:C80" xr:uid="{C1E729B3-29BA-40F1-80D4-2208DEC4BA85}"/>
   <conditionalFormatting sqref="D5:E5 D9:E9 D13:E13 D17:E17">
     <cfRule type="expression" dxfId="0" priority="4">
       <formula>D4&lt;&gt;"User Defined Table"</formula>
@@ -8040,7 +8029,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B4" t="s">
         <v>49</v>
@@ -8773,7 +8762,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA1111D6-CFD5-472E-AAF0-AF6E36C438B2}">
   <dimension ref="B1:F48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
@@ -8800,7 +8789,7 @@
         <v>189</v>
       </c>
       <c r="F1" s="35" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="2" spans="2:6" x14ac:dyDescent="0.3">
@@ -8831,7 +8820,7 @@
         <v>174</v>
       </c>
       <c r="F3" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.3">
@@ -8890,7 +8879,7 @@
         <v>178</v>
       </c>
       <c r="F7" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.3">
@@ -8921,12 +8910,12 @@
         <v>200</v>
       </c>
       <c r="F9" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B12" s="35" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C12" s="35" t="s">
         <v>188</v>
@@ -8939,10 +8928,10 @@
         <v>117</v>
       </c>
       <c r="C13" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D13" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.3">
@@ -8950,10 +8939,10 @@
         <v>117</v>
       </c>
       <c r="C14" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D14" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.3">
@@ -8961,10 +8950,10 @@
         <v>117</v>
       </c>
       <c r="C15" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D15" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.3">
@@ -8972,10 +8961,10 @@
         <v>117</v>
       </c>
       <c r="C16" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D16" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.3">
@@ -8983,10 +8972,10 @@
         <v>117</v>
       </c>
       <c r="C17" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D17" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.3">
@@ -8994,10 +8983,10 @@
         <v>117</v>
       </c>
       <c r="C18" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D18" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.3">
@@ -9005,10 +8994,10 @@
         <v>117</v>
       </c>
       <c r="C19" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D19" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.3">
@@ -9016,10 +9005,10 @@
         <v>117</v>
       </c>
       <c r="C20" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D20" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.3">
@@ -9027,7 +9016,7 @@
         <v>117</v>
       </c>
       <c r="C21" s="38" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.3">
@@ -9035,7 +9024,7 @@
         <v>118</v>
       </c>
       <c r="C22" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.3">
@@ -9043,10 +9032,10 @@
         <v>118</v>
       </c>
       <c r="C23" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D23" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.3">
@@ -9054,7 +9043,7 @@
         <v>119</v>
       </c>
       <c r="C24" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.3">
@@ -9062,7 +9051,7 @@
         <v>112</v>
       </c>
       <c r="C25" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.3">
@@ -9070,7 +9059,7 @@
         <v>112</v>
       </c>
       <c r="C26" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.3">
@@ -9078,7 +9067,7 @@
         <v>112</v>
       </c>
       <c r="C27" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.3">
@@ -9086,7 +9075,7 @@
         <v>120</v>
       </c>
       <c r="C28" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.3">
@@ -9094,7 +9083,7 @@
         <v>120</v>
       </c>
       <c r="C29" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.3">
@@ -9102,7 +9091,7 @@
         <v>120</v>
       </c>
       <c r="C30" s="38" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.3">
@@ -9110,7 +9099,7 @@
         <v>120</v>
       </c>
       <c r="C31" s="38" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.3">
@@ -9118,7 +9107,7 @@
         <v>121</v>
       </c>
       <c r="C32" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.3">
@@ -9126,7 +9115,7 @@
         <v>121</v>
       </c>
       <c r="C33" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.3">
@@ -9134,7 +9123,7 @@
         <v>122</v>
       </c>
       <c r="C34" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.3">
@@ -9142,7 +9131,7 @@
         <v>122</v>
       </c>
       <c r="C35" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.3">
@@ -9150,7 +9139,7 @@
         <v>179</v>
       </c>
       <c r="C37" s="35" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D37" s="35"/>
     </row>
@@ -9181,7 +9170,7 @@
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B43" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="44" spans="2:4" x14ac:dyDescent="0.3">

</xml_diff>